<commit_message>
Dev Team Template Update
</commit_message>
<xml_diff>
--- a/UDM.Insurance.Interface/Templates/ReportTemplateBatchExport.xlsx
+++ b/UDM.Insurance.Interface/Templates/ReportTemplateBatchExport.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Source\udminsure\UDM.Insurance.Interface\Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DaneB\source\repos\Insure\UDM.Insurance.Interface\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BC9CF4F-6105-4835-B0CE-00DAC138EF01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="28830" windowHeight="6405" activeTab="2"/>
+    <workbookView xWindow="-24120" yWindow="1185" windowWidth="24240" windowHeight="13140" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Batch Cover Sheet" sheetId="2" r:id="rId1"/>
@@ -19,7 +20,18 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Policy Data'!$A$3:$HK$32</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -656,9 +668,6 @@
     <t>LA2Units 68</t>
   </si>
   <si>
-    <t>Halo of Hope</t>
-  </si>
-  <si>
     <t>LA2Relationship</t>
   </si>
   <si>
@@ -816,12 +825,15 @@
   </si>
   <si>
     <t>BN4Percentage21</t>
+  </si>
+  <si>
+    <t>Mandate Response</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="00000"/>
     <numFmt numFmtId="165" formatCode="&quot;R&quot;\ #,##0.00"/>
@@ -2260,6 +2272,24 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="22" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -2284,15 +2314,6 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
-    </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -2311,103 +2332,118 @@
     <xf numFmtId="0" fontId="3" fillId="22" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="26" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="26" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="26" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="8" fillId="19" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="8" fillId="19" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="8" fillId="19" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="15" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="15" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="15" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="12" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="12" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="12" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="16" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="16" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="16" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="11" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="11" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="23" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="23" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="23" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="24" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="24" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="9" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="7" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="7" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="7" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="8" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="8" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="8" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="10" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="10" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="10" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="6" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="6" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="13" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="13" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="13" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="14" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="14" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="14" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="6" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="6" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="6" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="21" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="21" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="21" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="5" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="5" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="11" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2440,15 +2476,6 @@
     <xf numFmtId="49" fontId="8" fillId="5" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="8" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -2458,15 +2485,6 @@
     <xf numFmtId="49" fontId="8" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="6" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="6" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="6" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="8" fillId="9" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -2476,101 +2494,95 @@
     <xf numFmtId="49" fontId="8" fillId="9" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="8" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="8" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="8" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="10" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="26" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="10" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="26" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="10" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="26" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="8" fillId="19" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="8" fillId="19" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="8" fillId="19" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="7" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="7" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="7" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="15" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="6" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="15" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="6" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="15" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="12" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="13" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="12" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="13" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="12" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="13" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="16" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="14" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="16" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="14" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="16" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="14" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="11" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="21" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="11" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="21" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="23" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="21" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="23" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="5" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="23" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="5" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="24" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="24" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal_Policy Data" xfId="1"/>
-    <cellStyle name="Normal_Policy Data 2" xfId="2"/>
+    <cellStyle name="Normal_Policy Data" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal_Policy Data 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -3068,7 +3080,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor indexed="12"/>
   </sheetPr>
@@ -4536,7 +4548,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor indexed="57"/>
   </sheetPr>
@@ -4629,28 +4641,28 @@
       <c r="Y9" s="2"/>
     </row>
     <row r="10" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D10" s="237" t="s">
+      <c r="D10" s="231" t="s">
         <v>0</v>
       </c>
-      <c r="E10" s="238"/>
-      <c r="F10" s="238"/>
-      <c r="G10" s="238"/>
-      <c r="H10" s="238"/>
-      <c r="I10" s="238"/>
-      <c r="J10" s="238"/>
-      <c r="K10" s="238"/>
-      <c r="L10" s="239"/>
-      <c r="M10" s="246" t="s">
+      <c r="E10" s="232"/>
+      <c r="F10" s="232"/>
+      <c r="G10" s="232"/>
+      <c r="H10" s="232"/>
+      <c r="I10" s="232"/>
+      <c r="J10" s="232"/>
+      <c r="K10" s="232"/>
+      <c r="L10" s="233"/>
+      <c r="M10" s="234" t="s">
         <v>9</v>
       </c>
-      <c r="N10" s="247"/>
-      <c r="O10" s="247"/>
-      <c r="P10" s="247"/>
-      <c r="Q10" s="247"/>
-      <c r="R10" s="247"/>
-      <c r="S10" s="247"/>
-      <c r="T10" s="247"/>
-      <c r="U10" s="248"/>
+      <c r="N10" s="235"/>
+      <c r="O10" s="235"/>
+      <c r="P10" s="235"/>
+      <c r="Q10" s="235"/>
+      <c r="R10" s="235"/>
+      <c r="S10" s="235"/>
+      <c r="T10" s="235"/>
+      <c r="U10" s="236"/>
       <c r="W10" s="3"/>
       <c r="X10" s="3"/>
       <c r="Y10" s="2"/>
@@ -4669,26 +4681,26 @@
       <c r="X11" s="3"/>
     </row>
     <row r="12" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D12" s="237" t="s">
+      <c r="D12" s="231" t="s">
         <v>1</v>
       </c>
-      <c r="E12" s="238"/>
-      <c r="F12" s="238"/>
-      <c r="G12" s="238"/>
-      <c r="H12" s="238"/>
-      <c r="I12" s="238"/>
-      <c r="J12" s="238"/>
-      <c r="K12" s="238"/>
-      <c r="L12" s="239"/>
-      <c r="M12" s="246"/>
-      <c r="N12" s="247"/>
-      <c r="O12" s="247"/>
-      <c r="P12" s="247"/>
-      <c r="Q12" s="247"/>
-      <c r="R12" s="247"/>
-      <c r="S12" s="247"/>
-      <c r="T12" s="247"/>
-      <c r="U12" s="248"/>
+      <c r="E12" s="232"/>
+      <c r="F12" s="232"/>
+      <c r="G12" s="232"/>
+      <c r="H12" s="232"/>
+      <c r="I12" s="232"/>
+      <c r="J12" s="232"/>
+      <c r="K12" s="232"/>
+      <c r="L12" s="233"/>
+      <c r="M12" s="234"/>
+      <c r="N12" s="235"/>
+      <c r="O12" s="235"/>
+      <c r="P12" s="235"/>
+      <c r="Q12" s="235"/>
+      <c r="R12" s="235"/>
+      <c r="S12" s="235"/>
+      <c r="T12" s="235"/>
+      <c r="U12" s="236"/>
       <c r="W12" s="3"/>
       <c r="X12" s="3"/>
       <c r="Y12" s="2"/>
@@ -4707,26 +4719,26 @@
       <c r="X13" s="3"/>
     </row>
     <row r="14" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D14" s="237" t="s">
+      <c r="D14" s="231" t="s">
         <v>2</v>
       </c>
-      <c r="E14" s="238"/>
-      <c r="F14" s="238"/>
-      <c r="G14" s="238"/>
-      <c r="H14" s="238"/>
-      <c r="I14" s="238"/>
-      <c r="J14" s="238"/>
-      <c r="K14" s="238"/>
-      <c r="L14" s="239"/>
-      <c r="M14" s="246"/>
-      <c r="N14" s="247"/>
-      <c r="O14" s="247"/>
-      <c r="P14" s="247"/>
-      <c r="Q14" s="247"/>
-      <c r="R14" s="247"/>
-      <c r="S14" s="247"/>
-      <c r="T14" s="247"/>
-      <c r="U14" s="248"/>
+      <c r="E14" s="232"/>
+      <c r="F14" s="232"/>
+      <c r="G14" s="232"/>
+      <c r="H14" s="232"/>
+      <c r="I14" s="232"/>
+      <c r="J14" s="232"/>
+      <c r="K14" s="232"/>
+      <c r="L14" s="233"/>
+      <c r="M14" s="234"/>
+      <c r="N14" s="235"/>
+      <c r="O14" s="235"/>
+      <c r="P14" s="235"/>
+      <c r="Q14" s="235"/>
+      <c r="R14" s="235"/>
+      <c r="S14" s="235"/>
+      <c r="T14" s="235"/>
+      <c r="U14" s="236"/>
       <c r="W14" s="3"/>
       <c r="X14" s="3"/>
       <c r="Y14" s="2"/>
@@ -4747,26 +4759,26 @@
     <row r="16" spans="1:25" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="81"/>
       <c r="B16" s="81"/>
-      <c r="D16" s="237" t="s">
+      <c r="D16" s="231" t="s">
         <v>3</v>
       </c>
-      <c r="E16" s="238"/>
-      <c r="F16" s="238"/>
-      <c r="G16" s="238"/>
-      <c r="H16" s="238"/>
-      <c r="I16" s="238"/>
-      <c r="J16" s="238"/>
-      <c r="K16" s="238"/>
-      <c r="L16" s="239"/>
-      <c r="M16" s="246"/>
-      <c r="N16" s="247"/>
-      <c r="O16" s="247"/>
-      <c r="P16" s="247"/>
-      <c r="Q16" s="247"/>
-      <c r="R16" s="247"/>
-      <c r="S16" s="247"/>
-      <c r="T16" s="247"/>
-      <c r="U16" s="248"/>
+      <c r="E16" s="232"/>
+      <c r="F16" s="232"/>
+      <c r="G16" s="232"/>
+      <c r="H16" s="232"/>
+      <c r="I16" s="232"/>
+      <c r="J16" s="232"/>
+      <c r="K16" s="232"/>
+      <c r="L16" s="233"/>
+      <c r="M16" s="234"/>
+      <c r="N16" s="235"/>
+      <c r="O16" s="235"/>
+      <c r="P16" s="235"/>
+      <c r="Q16" s="235"/>
+      <c r="R16" s="235"/>
+      <c r="S16" s="235"/>
+      <c r="T16" s="235"/>
+      <c r="U16" s="236"/>
     </row>
     <row r="17" spans="1:24" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D17" s="80"/>
@@ -4784,26 +4796,26 @@
     <row r="18" spans="1:24" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="82"/>
       <c r="B18" s="82"/>
-      <c r="D18" s="237" t="s">
+      <c r="D18" s="231" t="s">
         <v>4</v>
       </c>
-      <c r="E18" s="238"/>
-      <c r="F18" s="238"/>
-      <c r="G18" s="238"/>
-      <c r="H18" s="238"/>
-      <c r="I18" s="238"/>
-      <c r="J18" s="238"/>
-      <c r="K18" s="238"/>
-      <c r="L18" s="239"/>
-      <c r="M18" s="240"/>
-      <c r="N18" s="241"/>
-      <c r="O18" s="241"/>
-      <c r="P18" s="241"/>
-      <c r="Q18" s="241"/>
-      <c r="R18" s="241"/>
-      <c r="S18" s="241"/>
-      <c r="T18" s="241"/>
-      <c r="U18" s="242"/>
+      <c r="E18" s="232"/>
+      <c r="F18" s="232"/>
+      <c r="G18" s="232"/>
+      <c r="H18" s="232"/>
+      <c r="I18" s="232"/>
+      <c r="J18" s="232"/>
+      <c r="K18" s="232"/>
+      <c r="L18" s="233"/>
+      <c r="M18" s="243"/>
+      <c r="N18" s="244"/>
+      <c r="O18" s="244"/>
+      <c r="P18" s="244"/>
+      <c r="Q18" s="244"/>
+      <c r="R18" s="244"/>
+      <c r="S18" s="244"/>
+      <c r="T18" s="244"/>
+      <c r="U18" s="245"/>
     </row>
     <row r="19" spans="1:24" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G19" s="83"/>
@@ -4811,60 +4823,60 @@
       <c r="I19" s="83"/>
     </row>
     <row r="20" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C20" s="243" t="s">
+      <c r="C20" s="246" t="s">
         <v>5</v>
       </c>
-      <c r="D20" s="243"/>
-      <c r="E20" s="244" t="s">
-        <v>225</v>
-      </c>
-      <c r="F20" s="244"/>
-      <c r="G20" s="244"/>
-      <c r="H20" s="244"/>
-      <c r="I20" s="244"/>
-      <c r="J20" s="244"/>
-      <c r="K20" s="243" t="s">
+      <c r="D20" s="246"/>
+      <c r="E20" s="247" t="s">
+        <v>224</v>
+      </c>
+      <c r="F20" s="247"/>
+      <c r="G20" s="247"/>
+      <c r="H20" s="247"/>
+      <c r="I20" s="247"/>
+      <c r="J20" s="247"/>
+      <c r="K20" s="246" t="s">
         <v>6</v>
       </c>
-      <c r="L20" s="243"/>
-      <c r="M20" s="243"/>
-      <c r="N20" s="243"/>
-      <c r="O20" s="243"/>
-      <c r="P20" s="243"/>
-      <c r="Q20" s="245" t="s">
+      <c r="L20" s="246"/>
+      <c r="M20" s="246"/>
+      <c r="N20" s="246"/>
+      <c r="O20" s="246"/>
+      <c r="P20" s="246"/>
+      <c r="Q20" s="248" t="s">
         <v>7</v>
       </c>
-      <c r="R20" s="245"/>
-      <c r="S20" s="245"/>
-      <c r="T20" s="245"/>
-      <c r="U20" s="245"/>
-      <c r="V20" s="245"/>
+      <c r="R20" s="248"/>
+      <c r="S20" s="248"/>
+      <c r="T20" s="248"/>
+      <c r="U20" s="248"/>
+      <c r="V20" s="248"/>
       <c r="W20" s="3"/>
       <c r="X20" s="3"/>
     </row>
     <row r="21" spans="1:24" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C21" s="231">
+      <c r="C21" s="237">
         <v>1</v>
       </c>
-      <c r="D21" s="231"/>
-      <c r="E21" s="232"/>
-      <c r="F21" s="233"/>
-      <c r="G21" s="233"/>
-      <c r="H21" s="233"/>
-      <c r="I21" s="233"/>
-      <c r="J21" s="234"/>
-      <c r="K21" s="235"/>
-      <c r="L21" s="236"/>
-      <c r="M21" s="236"/>
-      <c r="N21" s="236"/>
-      <c r="O21" s="236"/>
-      <c r="P21" s="236"/>
-      <c r="Q21" s="235"/>
-      <c r="R21" s="236"/>
-      <c r="S21" s="236"/>
-      <c r="T21" s="236"/>
-      <c r="U21" s="236"/>
-      <c r="V21" s="236"/>
+      <c r="D21" s="237"/>
+      <c r="E21" s="238"/>
+      <c r="F21" s="239"/>
+      <c r="G21" s="239"/>
+      <c r="H21" s="239"/>
+      <c r="I21" s="239"/>
+      <c r="J21" s="240"/>
+      <c r="K21" s="241"/>
+      <c r="L21" s="242"/>
+      <c r="M21" s="242"/>
+      <c r="N21" s="242"/>
+      <c r="O21" s="242"/>
+      <c r="P21" s="242"/>
+      <c r="Q21" s="241"/>
+      <c r="R21" s="242"/>
+      <c r="S21" s="242"/>
+      <c r="T21" s="242"/>
+      <c r="U21" s="242"/>
+      <c r="V21" s="242"/>
     </row>
     <row r="22" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="W22" s="3"/>
@@ -5156,14 +5168,6 @@
     <protectedRange password="CB1D" sqref="C9:D9 D10:E18" name="BatchData" securityDescriptor="O:WDG:WDD:(D;;CC;;;S-1-5-21-343818398-1326574676-839522115-1142)(D;;CC;;;S-1-5-21-343818398-1326574676-839522115-1141)(A;;CC;;;S-1-5-21-343818398-1326574676-839522115-1136)(A;;CC;;;S-1-5-21-343818398-1326574676-839522115-1137)"/>
   </protectedRanges>
   <mergeCells count="18">
-    <mergeCell ref="D16:L16"/>
-    <mergeCell ref="M16:U16"/>
-    <mergeCell ref="D10:L10"/>
-    <mergeCell ref="M10:U10"/>
-    <mergeCell ref="D12:L12"/>
-    <mergeCell ref="M12:U12"/>
-    <mergeCell ref="D14:L14"/>
-    <mergeCell ref="M14:U14"/>
     <mergeCell ref="C21:D21"/>
     <mergeCell ref="E21:J21"/>
     <mergeCell ref="K21:P21"/>
@@ -5174,6 +5178,14 @@
     <mergeCell ref="E20:J20"/>
     <mergeCell ref="K20:P20"/>
     <mergeCell ref="Q20:V20"/>
+    <mergeCell ref="D16:L16"/>
+    <mergeCell ref="M16:U16"/>
+    <mergeCell ref="D10:L10"/>
+    <mergeCell ref="M10:U10"/>
+    <mergeCell ref="D12:L12"/>
+    <mergeCell ref="M12:U12"/>
+    <mergeCell ref="D14:L14"/>
+    <mergeCell ref="M14:U14"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -5184,15 +5196,15 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor indexed="10"/>
   </sheetPr>
   <dimension ref="A1:HN494"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="GG1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="HG1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="GL2" sqref="GL2:GU2"/>
+      <selection pane="bottomLeft" activeCell="HK3" sqref="HK3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5407,236 +5419,236 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:222" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="313" t="s">
+      <c r="A1" s="264" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="314"/>
-      <c r="C1" s="314"/>
-      <c r="D1" s="314"/>
-      <c r="E1" s="314"/>
-      <c r="F1" s="314"/>
-      <c r="G1" s="314"/>
-      <c r="H1" s="314"/>
-      <c r="I1" s="314"/>
-      <c r="J1" s="314"/>
-      <c r="K1" s="314"/>
-      <c r="L1" s="315"/>
-      <c r="M1" s="277"/>
-      <c r="N1" s="278"/>
-      <c r="O1" s="278"/>
-      <c r="P1" s="278"/>
-      <c r="Q1" s="278"/>
-      <c r="R1" s="278"/>
-      <c r="S1" s="278"/>
-      <c r="T1" s="278"/>
-      <c r="U1" s="278"/>
-      <c r="V1" s="278"/>
-      <c r="W1" s="278"/>
-      <c r="X1" s="278"/>
-      <c r="Y1" s="278"/>
-      <c r="Z1" s="278"/>
-      <c r="AA1" s="278"/>
-      <c r="AB1" s="278"/>
-      <c r="AC1" s="278"/>
-      <c r="AD1" s="278"/>
-      <c r="AE1" s="278"/>
-      <c r="AF1" s="278"/>
-      <c r="AG1" s="278"/>
-      <c r="AH1" s="278"/>
-      <c r="AI1" s="278"/>
-      <c r="AJ1" s="278"/>
-      <c r="AK1" s="278"/>
-      <c r="AL1" s="278"/>
-      <c r="AM1" s="278"/>
-      <c r="AN1" s="278"/>
-      <c r="AO1" s="278"/>
-      <c r="AP1" s="278"/>
-      <c r="AQ1" s="278"/>
-      <c r="AR1" s="278"/>
-      <c r="AS1" s="278"/>
-      <c r="AT1" s="278"/>
-      <c r="AU1" s="278"/>
-      <c r="AV1" s="278"/>
-      <c r="AW1" s="278"/>
-      <c r="AX1" s="278"/>
-      <c r="AY1" s="278"/>
-      <c r="AZ1" s="278"/>
-      <c r="BA1" s="278"/>
-      <c r="BB1" s="306"/>
-      <c r="BC1" s="313" t="s">
+      <c r="B1" s="265"/>
+      <c r="C1" s="265"/>
+      <c r="D1" s="265"/>
+      <c r="E1" s="265"/>
+      <c r="F1" s="265"/>
+      <c r="G1" s="265"/>
+      <c r="H1" s="265"/>
+      <c r="I1" s="265"/>
+      <c r="J1" s="265"/>
+      <c r="K1" s="265"/>
+      <c r="L1" s="266"/>
+      <c r="M1" s="254"/>
+      <c r="N1" s="249"/>
+      <c r="O1" s="249"/>
+      <c r="P1" s="249"/>
+      <c r="Q1" s="249"/>
+      <c r="R1" s="249"/>
+      <c r="S1" s="249"/>
+      <c r="T1" s="249"/>
+      <c r="U1" s="249"/>
+      <c r="V1" s="249"/>
+      <c r="W1" s="249"/>
+      <c r="X1" s="249"/>
+      <c r="Y1" s="249"/>
+      <c r="Z1" s="249"/>
+      <c r="AA1" s="249"/>
+      <c r="AB1" s="249"/>
+      <c r="AC1" s="249"/>
+      <c r="AD1" s="249"/>
+      <c r="AE1" s="249"/>
+      <c r="AF1" s="249"/>
+      <c r="AG1" s="249"/>
+      <c r="AH1" s="249"/>
+      <c r="AI1" s="249"/>
+      <c r="AJ1" s="249"/>
+      <c r="AK1" s="249"/>
+      <c r="AL1" s="249"/>
+      <c r="AM1" s="249"/>
+      <c r="AN1" s="249"/>
+      <c r="AO1" s="249"/>
+      <c r="AP1" s="249"/>
+      <c r="AQ1" s="249"/>
+      <c r="AR1" s="249"/>
+      <c r="AS1" s="249"/>
+      <c r="AT1" s="249"/>
+      <c r="AU1" s="249"/>
+      <c r="AV1" s="249"/>
+      <c r="AW1" s="249"/>
+      <c r="AX1" s="249"/>
+      <c r="AY1" s="249"/>
+      <c r="AZ1" s="249"/>
+      <c r="BA1" s="249"/>
+      <c r="BB1" s="250"/>
+      <c r="BC1" s="264" t="s">
         <v>16</v>
       </c>
-      <c r="BD1" s="314"/>
-      <c r="BE1" s="314"/>
-      <c r="BF1" s="314"/>
-      <c r="BG1" s="314"/>
-      <c r="BH1" s="314"/>
-      <c r="BI1" s="315"/>
-      <c r="BJ1" s="316" t="s">
+      <c r="BD1" s="265"/>
+      <c r="BE1" s="265"/>
+      <c r="BF1" s="265"/>
+      <c r="BG1" s="265"/>
+      <c r="BH1" s="265"/>
+      <c r="BI1" s="266"/>
+      <c r="BJ1" s="267" t="s">
         <v>17</v>
       </c>
-      <c r="BK1" s="317"/>
-      <c r="BL1" s="317"/>
-      <c r="BM1" s="317"/>
-      <c r="BN1" s="318"/>
-      <c r="BO1" s="319" t="s">
+      <c r="BK1" s="268"/>
+      <c r="BL1" s="268"/>
+      <c r="BM1" s="268"/>
+      <c r="BN1" s="269"/>
+      <c r="BO1" s="270" t="s">
         <v>18</v>
       </c>
-      <c r="BP1" s="320"/>
-      <c r="BQ1" s="320"/>
-      <c r="BR1" s="320"/>
-      <c r="BS1" s="320"/>
-      <c r="BT1" s="320"/>
-      <c r="BU1" s="320"/>
-      <c r="BV1" s="320"/>
-      <c r="BW1" s="320"/>
-      <c r="BX1" s="320"/>
-      <c r="BY1" s="320"/>
-      <c r="BZ1" s="320"/>
-      <c r="CA1" s="320"/>
-      <c r="CB1" s="320"/>
-      <c r="CC1" s="320"/>
-      <c r="CD1" s="320"/>
-      <c r="CE1" s="320"/>
-      <c r="CF1" s="320"/>
-      <c r="CG1" s="320"/>
-      <c r="CH1" s="320"/>
-      <c r="CI1" s="320"/>
-      <c r="CJ1" s="320"/>
-      <c r="CK1" s="320"/>
-      <c r="CL1" s="320"/>
-      <c r="CM1" s="320"/>
-      <c r="CN1" s="320"/>
-      <c r="CO1" s="320"/>
-      <c r="CP1" s="320"/>
-      <c r="CQ1" s="320"/>
-      <c r="CR1" s="320"/>
-      <c r="CS1" s="320"/>
-      <c r="CT1" s="320"/>
-      <c r="CU1" s="320"/>
-      <c r="CV1" s="320"/>
-      <c r="CW1" s="320"/>
-      <c r="CX1" s="320"/>
-      <c r="CY1" s="320"/>
-      <c r="CZ1" s="320"/>
-      <c r="DA1" s="320"/>
-      <c r="DB1" s="320"/>
-      <c r="DC1" s="321"/>
-      <c r="DD1" s="291" t="s">
+      <c r="BP1" s="271"/>
+      <c r="BQ1" s="271"/>
+      <c r="BR1" s="271"/>
+      <c r="BS1" s="271"/>
+      <c r="BT1" s="271"/>
+      <c r="BU1" s="271"/>
+      <c r="BV1" s="271"/>
+      <c r="BW1" s="271"/>
+      <c r="BX1" s="271"/>
+      <c r="BY1" s="271"/>
+      <c r="BZ1" s="271"/>
+      <c r="CA1" s="271"/>
+      <c r="CB1" s="271"/>
+      <c r="CC1" s="271"/>
+      <c r="CD1" s="271"/>
+      <c r="CE1" s="271"/>
+      <c r="CF1" s="271"/>
+      <c r="CG1" s="271"/>
+      <c r="CH1" s="271"/>
+      <c r="CI1" s="271"/>
+      <c r="CJ1" s="271"/>
+      <c r="CK1" s="271"/>
+      <c r="CL1" s="271"/>
+      <c r="CM1" s="271"/>
+      <c r="CN1" s="271"/>
+      <c r="CO1" s="271"/>
+      <c r="CP1" s="271"/>
+      <c r="CQ1" s="271"/>
+      <c r="CR1" s="271"/>
+      <c r="CS1" s="271"/>
+      <c r="CT1" s="271"/>
+      <c r="CU1" s="271"/>
+      <c r="CV1" s="271"/>
+      <c r="CW1" s="271"/>
+      <c r="CX1" s="271"/>
+      <c r="CY1" s="271"/>
+      <c r="CZ1" s="271"/>
+      <c r="DA1" s="271"/>
+      <c r="DB1" s="271"/>
+      <c r="DC1" s="272"/>
+      <c r="DD1" s="296" t="s">
         <v>19</v>
       </c>
-      <c r="DE1" s="292"/>
-      <c r="DF1" s="292"/>
-      <c r="DG1" s="292"/>
-      <c r="DH1" s="292"/>
-      <c r="DI1" s="292"/>
-      <c r="DJ1" s="292"/>
-      <c r="DK1" s="292"/>
-      <c r="DL1" s="292"/>
-      <c r="DM1" s="292"/>
-      <c r="DN1" s="292"/>
-      <c r="DO1" s="292"/>
-      <c r="DP1" s="292"/>
-      <c r="DQ1" s="292"/>
-      <c r="DR1" s="292"/>
-      <c r="DS1" s="292"/>
-      <c r="DT1" s="292"/>
-      <c r="DU1" s="292"/>
-      <c r="DV1" s="292"/>
-      <c r="DW1" s="292"/>
-      <c r="DX1" s="292"/>
-      <c r="DY1" s="292"/>
-      <c r="DZ1" s="292"/>
-      <c r="EA1" s="292"/>
-      <c r="EB1" s="292"/>
-      <c r="EC1" s="292"/>
-      <c r="ED1" s="292"/>
-      <c r="EE1" s="292"/>
-      <c r="EF1" s="292"/>
-      <c r="EG1" s="292"/>
-      <c r="EH1" s="292"/>
-      <c r="EI1" s="292"/>
-      <c r="EJ1" s="292"/>
-      <c r="EK1" s="292"/>
-      <c r="EL1" s="292"/>
-      <c r="EM1" s="293"/>
-      <c r="EN1" s="277"/>
-      <c r="EO1" s="278"/>
-      <c r="EP1" s="278"/>
-      <c r="EQ1" s="278"/>
-      <c r="ER1" s="278"/>
-      <c r="ES1" s="278"/>
-      <c r="ET1" s="278"/>
-      <c r="EU1" s="278"/>
-      <c r="EV1" s="278"/>
-      <c r="EW1" s="278"/>
-      <c r="EX1" s="278"/>
-      <c r="EY1" s="278"/>
-      <c r="EZ1" s="278"/>
-      <c r="FA1" s="278"/>
-      <c r="FB1" s="278"/>
-      <c r="FC1" s="278"/>
-      <c r="FD1" s="278"/>
-      <c r="FE1" s="278"/>
-      <c r="FF1" s="278"/>
-      <c r="FG1" s="278"/>
-      <c r="FH1" s="278"/>
-      <c r="FI1" s="278"/>
-      <c r="FJ1" s="278"/>
-      <c r="FK1" s="278"/>
-      <c r="FL1" s="278"/>
-      <c r="FM1" s="278"/>
-      <c r="FN1" s="278"/>
-      <c r="FO1" s="278"/>
-      <c r="FP1" s="278"/>
-      <c r="FQ1" s="278"/>
-      <c r="FR1" s="278"/>
-      <c r="FS1" s="278"/>
-      <c r="FT1" s="278"/>
-      <c r="FU1" s="278"/>
-      <c r="FV1" s="278"/>
-      <c r="FW1" s="278"/>
-      <c r="FX1" s="278"/>
-      <c r="FY1" s="278"/>
-      <c r="FZ1" s="278"/>
-      <c r="GA1" s="278"/>
-      <c r="GB1" s="278"/>
-      <c r="GC1" s="278"/>
-      <c r="GD1" s="278"/>
-      <c r="GE1" s="278"/>
-      <c r="GF1" s="278"/>
-      <c r="GG1" s="278"/>
-      <c r="GH1" s="278"/>
-      <c r="GI1" s="278"/>
-      <c r="GJ1" s="278"/>
-      <c r="GK1" s="278"/>
-      <c r="GL1" s="278"/>
-      <c r="GM1" s="278"/>
-      <c r="GN1" s="278"/>
-      <c r="GO1" s="278"/>
-      <c r="GP1" s="278"/>
-      <c r="GQ1" s="278"/>
-      <c r="GR1" s="278"/>
-      <c r="GS1" s="278"/>
-      <c r="GT1" s="278"/>
-      <c r="GU1" s="278"/>
-      <c r="GV1" s="258" t="s">
-        <v>231</v>
-      </c>
-      <c r="GW1" s="259"/>
-      <c r="GX1" s="259"/>
-      <c r="GY1" s="260"/>
+      <c r="DE1" s="297"/>
+      <c r="DF1" s="297"/>
+      <c r="DG1" s="297"/>
+      <c r="DH1" s="297"/>
+      <c r="DI1" s="297"/>
+      <c r="DJ1" s="297"/>
+      <c r="DK1" s="297"/>
+      <c r="DL1" s="297"/>
+      <c r="DM1" s="297"/>
+      <c r="DN1" s="297"/>
+      <c r="DO1" s="297"/>
+      <c r="DP1" s="297"/>
+      <c r="DQ1" s="297"/>
+      <c r="DR1" s="297"/>
+      <c r="DS1" s="297"/>
+      <c r="DT1" s="297"/>
+      <c r="DU1" s="297"/>
+      <c r="DV1" s="297"/>
+      <c r="DW1" s="297"/>
+      <c r="DX1" s="297"/>
+      <c r="DY1" s="297"/>
+      <c r="DZ1" s="297"/>
+      <c r="EA1" s="297"/>
+      <c r="EB1" s="297"/>
+      <c r="EC1" s="297"/>
+      <c r="ED1" s="297"/>
+      <c r="EE1" s="297"/>
+      <c r="EF1" s="297"/>
+      <c r="EG1" s="297"/>
+      <c r="EH1" s="297"/>
+      <c r="EI1" s="297"/>
+      <c r="EJ1" s="297"/>
+      <c r="EK1" s="297"/>
+      <c r="EL1" s="297"/>
+      <c r="EM1" s="298"/>
+      <c r="EN1" s="254"/>
+      <c r="EO1" s="249"/>
+      <c r="EP1" s="249"/>
+      <c r="EQ1" s="249"/>
+      <c r="ER1" s="249"/>
+      <c r="ES1" s="249"/>
+      <c r="ET1" s="249"/>
+      <c r="EU1" s="249"/>
+      <c r="EV1" s="249"/>
+      <c r="EW1" s="249"/>
+      <c r="EX1" s="249"/>
+      <c r="EY1" s="249"/>
+      <c r="EZ1" s="249"/>
+      <c r="FA1" s="249"/>
+      <c r="FB1" s="249"/>
+      <c r="FC1" s="249"/>
+      <c r="FD1" s="249"/>
+      <c r="FE1" s="249"/>
+      <c r="FF1" s="249"/>
+      <c r="FG1" s="249"/>
+      <c r="FH1" s="249"/>
+      <c r="FI1" s="249"/>
+      <c r="FJ1" s="249"/>
+      <c r="FK1" s="249"/>
+      <c r="FL1" s="249"/>
+      <c r="FM1" s="249"/>
+      <c r="FN1" s="249"/>
+      <c r="FO1" s="249"/>
+      <c r="FP1" s="249"/>
+      <c r="FQ1" s="249"/>
+      <c r="FR1" s="249"/>
+      <c r="FS1" s="249"/>
+      <c r="FT1" s="249"/>
+      <c r="FU1" s="249"/>
+      <c r="FV1" s="249"/>
+      <c r="FW1" s="249"/>
+      <c r="FX1" s="249"/>
+      <c r="FY1" s="249"/>
+      <c r="FZ1" s="249"/>
+      <c r="GA1" s="249"/>
+      <c r="GB1" s="249"/>
+      <c r="GC1" s="249"/>
+      <c r="GD1" s="249"/>
+      <c r="GE1" s="249"/>
+      <c r="GF1" s="249"/>
+      <c r="GG1" s="249"/>
+      <c r="GH1" s="249"/>
+      <c r="GI1" s="249"/>
+      <c r="GJ1" s="249"/>
+      <c r="GK1" s="249"/>
+      <c r="GL1" s="249"/>
+      <c r="GM1" s="249"/>
+      <c r="GN1" s="249"/>
+      <c r="GO1" s="249"/>
+      <c r="GP1" s="249"/>
+      <c r="GQ1" s="249"/>
+      <c r="GR1" s="249"/>
+      <c r="GS1" s="249"/>
+      <c r="GT1" s="249"/>
+      <c r="GU1" s="249"/>
+      <c r="GV1" s="311" t="s">
+        <v>230</v>
+      </c>
+      <c r="GW1" s="312"/>
+      <c r="GX1" s="312"/>
+      <c r="GY1" s="313"/>
       <c r="HA1" s="194"/>
       <c r="HB1" s="194"/>
       <c r="HC1" s="194"/>
-      <c r="HD1" s="249" t="s">
-        <v>218</v>
-      </c>
-      <c r="HE1" s="250"/>
-      <c r="HF1" s="250"/>
-      <c r="HG1" s="250"/>
-      <c r="HH1" s="250"/>
-      <c r="HI1" s="251"/>
+      <c r="HD1" s="302" t="s">
+        <v>217</v>
+      </c>
+      <c r="HE1" s="303"/>
+      <c r="HF1" s="303"/>
+      <c r="HG1" s="303"/>
+      <c r="HH1" s="303"/>
+      <c r="HI1" s="304"/>
       <c r="HJ1" s="92"/>
       <c r="HK1" s="91"/>
       <c r="HL1" s="97"/>
@@ -5644,267 +5656,267 @@
       <c r="HN1" s="110"/>
     </row>
     <row r="2" spans="1:222" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="278"/>
-      <c r="B2" s="278"/>
-      <c r="C2" s="278"/>
-      <c r="D2" s="278"/>
-      <c r="E2" s="278"/>
-      <c r="F2" s="278"/>
-      <c r="G2" s="278"/>
-      <c r="H2" s="278"/>
-      <c r="I2" s="306"/>
-      <c r="J2" s="325" t="s">
+      <c r="A2" s="249"/>
+      <c r="B2" s="249"/>
+      <c r="C2" s="249"/>
+      <c r="D2" s="249"/>
+      <c r="E2" s="249"/>
+      <c r="F2" s="249"/>
+      <c r="G2" s="249"/>
+      <c r="H2" s="249"/>
+      <c r="I2" s="250"/>
+      <c r="J2" s="282" t="s">
         <v>20</v>
       </c>
-      <c r="K2" s="326"/>
+      <c r="K2" s="283"/>
       <c r="L2" s="48"/>
-      <c r="M2" s="307"/>
-      <c r="N2" s="308"/>
-      <c r="O2" s="308"/>
-      <c r="P2" s="308"/>
-      <c r="Q2" s="308"/>
-      <c r="R2" s="308"/>
-      <c r="S2" s="308"/>
-      <c r="T2" s="309"/>
-      <c r="U2" s="327" t="s">
+      <c r="M2" s="251"/>
+      <c r="N2" s="252"/>
+      <c r="O2" s="252"/>
+      <c r="P2" s="252"/>
+      <c r="Q2" s="252"/>
+      <c r="R2" s="252"/>
+      <c r="S2" s="252"/>
+      <c r="T2" s="253"/>
+      <c r="U2" s="284" t="s">
         <v>21</v>
       </c>
-      <c r="V2" s="328"/>
-      <c r="W2" s="328"/>
-      <c r="X2" s="328"/>
-      <c r="Y2" s="328"/>
-      <c r="Z2" s="328"/>
-      <c r="AA2" s="328"/>
-      <c r="AB2" s="328"/>
-      <c r="AC2" s="328"/>
-      <c r="AD2" s="328"/>
-      <c r="AE2" s="328"/>
-      <c r="AF2" s="328"/>
-      <c r="AG2" s="328"/>
-      <c r="AH2" s="328"/>
-      <c r="AI2" s="328"/>
-      <c r="AJ2" s="328"/>
-      <c r="AK2" s="329"/>
-      <c r="AL2" s="279" t="s">
+      <c r="V2" s="285"/>
+      <c r="W2" s="285"/>
+      <c r="X2" s="285"/>
+      <c r="Y2" s="285"/>
+      <c r="Z2" s="285"/>
+      <c r="AA2" s="285"/>
+      <c r="AB2" s="285"/>
+      <c r="AC2" s="285"/>
+      <c r="AD2" s="285"/>
+      <c r="AE2" s="285"/>
+      <c r="AF2" s="285"/>
+      <c r="AG2" s="285"/>
+      <c r="AH2" s="285"/>
+      <c r="AI2" s="285"/>
+      <c r="AJ2" s="285"/>
+      <c r="AK2" s="286"/>
+      <c r="AL2" s="287" t="s">
         <v>22</v>
       </c>
-      <c r="AM2" s="280"/>
-      <c r="AN2" s="280"/>
-      <c r="AO2" s="280"/>
-      <c r="AP2" s="280"/>
-      <c r="AQ2" s="280"/>
-      <c r="AR2" s="280"/>
-      <c r="AS2" s="280"/>
-      <c r="AT2" s="280"/>
-      <c r="AU2" s="281"/>
-      <c r="AV2" s="282" t="s">
+      <c r="AM2" s="288"/>
+      <c r="AN2" s="288"/>
+      <c r="AO2" s="288"/>
+      <c r="AP2" s="288"/>
+      <c r="AQ2" s="288"/>
+      <c r="AR2" s="288"/>
+      <c r="AS2" s="288"/>
+      <c r="AT2" s="288"/>
+      <c r="AU2" s="289"/>
+      <c r="AV2" s="290" t="s">
         <v>23</v>
       </c>
-      <c r="AW2" s="283"/>
-      <c r="AX2" s="283"/>
-      <c r="AY2" s="283"/>
-      <c r="AZ2" s="283"/>
-      <c r="BA2" s="283"/>
-      <c r="BB2" s="284"/>
-      <c r="BC2" s="288"/>
-      <c r="BD2" s="289"/>
-      <c r="BE2" s="289"/>
-      <c r="BF2" s="289"/>
-      <c r="BG2" s="289"/>
-      <c r="BH2" s="289"/>
-      <c r="BI2" s="290"/>
-      <c r="BJ2" s="288"/>
-      <c r="BK2" s="289"/>
-      <c r="BL2" s="289"/>
-      <c r="BM2" s="289"/>
-      <c r="BN2" s="290"/>
-      <c r="BO2" s="285" t="s">
+      <c r="AW2" s="291"/>
+      <c r="AX2" s="291"/>
+      <c r="AY2" s="291"/>
+      <c r="AZ2" s="291"/>
+      <c r="BA2" s="291"/>
+      <c r="BB2" s="292"/>
+      <c r="BC2" s="279"/>
+      <c r="BD2" s="280"/>
+      <c r="BE2" s="280"/>
+      <c r="BF2" s="280"/>
+      <c r="BG2" s="280"/>
+      <c r="BH2" s="280"/>
+      <c r="BI2" s="281"/>
+      <c r="BJ2" s="279"/>
+      <c r="BK2" s="280"/>
+      <c r="BL2" s="280"/>
+      <c r="BM2" s="280"/>
+      <c r="BN2" s="281"/>
+      <c r="BO2" s="293" t="s">
         <v>24</v>
       </c>
-      <c r="BP2" s="286"/>
-      <c r="BQ2" s="286"/>
-      <c r="BR2" s="286"/>
-      <c r="BS2" s="286"/>
-      <c r="BT2" s="286"/>
-      <c r="BU2" s="286"/>
-      <c r="BV2" s="286"/>
-      <c r="BW2" s="286"/>
-      <c r="BX2" s="286"/>
-      <c r="BY2" s="287"/>
-      <c r="BZ2" s="294" t="s">
+      <c r="BP2" s="294"/>
+      <c r="BQ2" s="294"/>
+      <c r="BR2" s="294"/>
+      <c r="BS2" s="294"/>
+      <c r="BT2" s="294"/>
+      <c r="BU2" s="294"/>
+      <c r="BV2" s="294"/>
+      <c r="BW2" s="294"/>
+      <c r="BX2" s="294"/>
+      <c r="BY2" s="295"/>
+      <c r="BZ2" s="273" t="s">
         <v>25</v>
       </c>
-      <c r="CA2" s="295"/>
-      <c r="CB2" s="295"/>
-      <c r="CC2" s="295"/>
-      <c r="CD2" s="296"/>
-      <c r="CE2" s="310" t="s">
+      <c r="CA2" s="274"/>
+      <c r="CB2" s="274"/>
+      <c r="CC2" s="274"/>
+      <c r="CD2" s="275"/>
+      <c r="CE2" s="255" t="s">
         <v>26</v>
       </c>
-      <c r="CF2" s="311"/>
-      <c r="CG2" s="311"/>
-      <c r="CH2" s="311"/>
-      <c r="CI2" s="312"/>
-      <c r="CJ2" s="300" t="s">
+      <c r="CF2" s="256"/>
+      <c r="CG2" s="256"/>
+      <c r="CH2" s="256"/>
+      <c r="CI2" s="257"/>
+      <c r="CJ2" s="258" t="s">
         <v>27</v>
       </c>
-      <c r="CK2" s="301"/>
-      <c r="CL2" s="301"/>
-      <c r="CM2" s="301"/>
-      <c r="CN2" s="302"/>
-      <c r="CO2" s="297" t="s">
+      <c r="CK2" s="259"/>
+      <c r="CL2" s="259"/>
+      <c r="CM2" s="259"/>
+      <c r="CN2" s="260"/>
+      <c r="CO2" s="299" t="s">
         <v>28</v>
       </c>
-      <c r="CP2" s="298"/>
-      <c r="CQ2" s="298"/>
-      <c r="CR2" s="298"/>
-      <c r="CS2" s="299"/>
-      <c r="CT2" s="303" t="s">
-        <v>228</v>
-      </c>
-      <c r="CU2" s="304"/>
-      <c r="CV2" s="304"/>
-      <c r="CW2" s="304"/>
-      <c r="CX2" s="305"/>
-      <c r="CY2" s="322" t="s">
-        <v>217</v>
-      </c>
-      <c r="CZ2" s="323"/>
-      <c r="DA2" s="323"/>
-      <c r="DB2" s="323"/>
-      <c r="DC2" s="324"/>
-      <c r="DD2" s="285" t="s">
+      <c r="CP2" s="300"/>
+      <c r="CQ2" s="300"/>
+      <c r="CR2" s="300"/>
+      <c r="CS2" s="301"/>
+      <c r="CT2" s="261" t="s">
+        <v>227</v>
+      </c>
+      <c r="CU2" s="262"/>
+      <c r="CV2" s="262"/>
+      <c r="CW2" s="262"/>
+      <c r="CX2" s="263"/>
+      <c r="CY2" s="276" t="s">
+        <v>216</v>
+      </c>
+      <c r="CZ2" s="277"/>
+      <c r="DA2" s="277"/>
+      <c r="DB2" s="277"/>
+      <c r="DC2" s="278"/>
+      <c r="DD2" s="293" t="s">
         <v>24</v>
       </c>
-      <c r="DE2" s="286"/>
-      <c r="DF2" s="286"/>
-      <c r="DG2" s="286"/>
-      <c r="DH2" s="286"/>
-      <c r="DI2" s="286"/>
-      <c r="DJ2" s="286"/>
-      <c r="DK2" s="286"/>
-      <c r="DL2" s="286"/>
-      <c r="DM2" s="286"/>
-      <c r="DN2" s="287"/>
-      <c r="DO2" s="294" t="s">
+      <c r="DE2" s="294"/>
+      <c r="DF2" s="294"/>
+      <c r="DG2" s="294"/>
+      <c r="DH2" s="294"/>
+      <c r="DI2" s="294"/>
+      <c r="DJ2" s="294"/>
+      <c r="DK2" s="294"/>
+      <c r="DL2" s="294"/>
+      <c r="DM2" s="294"/>
+      <c r="DN2" s="295"/>
+      <c r="DO2" s="273" t="s">
         <v>29</v>
       </c>
-      <c r="DP2" s="295"/>
-      <c r="DQ2" s="295"/>
-      <c r="DR2" s="295"/>
-      <c r="DS2" s="296"/>
-      <c r="DT2" s="310" t="s">
+      <c r="DP2" s="274"/>
+      <c r="DQ2" s="274"/>
+      <c r="DR2" s="274"/>
+      <c r="DS2" s="275"/>
+      <c r="DT2" s="255" t="s">
         <v>30</v>
       </c>
-      <c r="DU2" s="311"/>
-      <c r="DV2" s="311"/>
-      <c r="DW2" s="311"/>
-      <c r="DX2" s="312"/>
-      <c r="DY2" s="300" t="s">
+      <c r="DU2" s="256"/>
+      <c r="DV2" s="256"/>
+      <c r="DW2" s="256"/>
+      <c r="DX2" s="257"/>
+      <c r="DY2" s="258" t="s">
         <v>31</v>
       </c>
-      <c r="DZ2" s="301"/>
-      <c r="EA2" s="301"/>
-      <c r="EB2" s="301"/>
-      <c r="EC2" s="302"/>
-      <c r="ED2" s="297" t="s">
+      <c r="DZ2" s="259"/>
+      <c r="EA2" s="259"/>
+      <c r="EB2" s="259"/>
+      <c r="EC2" s="260"/>
+      <c r="ED2" s="299" t="s">
         <v>32</v>
       </c>
-      <c r="EE2" s="298"/>
-      <c r="EF2" s="298"/>
-      <c r="EG2" s="298"/>
-      <c r="EH2" s="299"/>
-      <c r="EI2" s="303" t="s">
+      <c r="EE2" s="300"/>
+      <c r="EF2" s="300"/>
+      <c r="EG2" s="300"/>
+      <c r="EH2" s="301"/>
+      <c r="EI2" s="261" t="s">
         <v>33</v>
       </c>
-      <c r="EJ2" s="304"/>
-      <c r="EK2" s="304"/>
-      <c r="EL2" s="304"/>
-      <c r="EM2" s="305"/>
-      <c r="EN2" s="261" t="s">
+      <c r="EJ2" s="262"/>
+      <c r="EK2" s="262"/>
+      <c r="EL2" s="262"/>
+      <c r="EM2" s="263"/>
+      <c r="EN2" s="314" t="s">
         <v>34</v>
       </c>
-      <c r="EO2" s="262"/>
-      <c r="EP2" s="262"/>
-      <c r="EQ2" s="262"/>
-      <c r="ER2" s="262"/>
-      <c r="ES2" s="262"/>
-      <c r="ET2" s="262"/>
-      <c r="EU2" s="262"/>
-      <c r="EV2" s="262"/>
-      <c r="EW2" s="263"/>
-      <c r="EX2" s="264" t="s">
+      <c r="EO2" s="315"/>
+      <c r="EP2" s="315"/>
+      <c r="EQ2" s="315"/>
+      <c r="ER2" s="315"/>
+      <c r="ES2" s="315"/>
+      <c r="ET2" s="315"/>
+      <c r="EU2" s="315"/>
+      <c r="EV2" s="315"/>
+      <c r="EW2" s="316"/>
+      <c r="EX2" s="317" t="s">
         <v>35</v>
       </c>
-      <c r="EY2" s="265"/>
-      <c r="EZ2" s="265"/>
-      <c r="FA2" s="265"/>
-      <c r="FB2" s="265"/>
-      <c r="FC2" s="265"/>
-      <c r="FD2" s="265"/>
-      <c r="FE2" s="265"/>
-      <c r="FF2" s="265"/>
-      <c r="FG2" s="266"/>
-      <c r="FH2" s="267" t="s">
+      <c r="EY2" s="318"/>
+      <c r="EZ2" s="318"/>
+      <c r="FA2" s="318"/>
+      <c r="FB2" s="318"/>
+      <c r="FC2" s="318"/>
+      <c r="FD2" s="318"/>
+      <c r="FE2" s="318"/>
+      <c r="FF2" s="318"/>
+      <c r="FG2" s="319"/>
+      <c r="FH2" s="320" t="s">
         <v>36</v>
       </c>
-      <c r="FI2" s="268"/>
-      <c r="FJ2" s="268"/>
-      <c r="FK2" s="268"/>
-      <c r="FL2" s="268"/>
-      <c r="FM2" s="268"/>
-      <c r="FN2" s="268"/>
-      <c r="FO2" s="268"/>
-      <c r="FP2" s="268"/>
-      <c r="FQ2" s="269"/>
-      <c r="FR2" s="270" t="s">
+      <c r="FI2" s="321"/>
+      <c r="FJ2" s="321"/>
+      <c r="FK2" s="321"/>
+      <c r="FL2" s="321"/>
+      <c r="FM2" s="321"/>
+      <c r="FN2" s="321"/>
+      <c r="FO2" s="321"/>
+      <c r="FP2" s="321"/>
+      <c r="FQ2" s="322"/>
+      <c r="FR2" s="323" t="s">
         <v>37</v>
       </c>
-      <c r="FS2" s="271"/>
-      <c r="FT2" s="271"/>
-      <c r="FU2" s="271"/>
-      <c r="FV2" s="271"/>
-      <c r="FW2" s="271"/>
-      <c r="FX2" s="271"/>
-      <c r="FY2" s="271"/>
-      <c r="FZ2" s="271"/>
-      <c r="GA2" s="271"/>
-      <c r="GB2" s="272" t="s">
+      <c r="FS2" s="324"/>
+      <c r="FT2" s="324"/>
+      <c r="FU2" s="324"/>
+      <c r="FV2" s="324"/>
+      <c r="FW2" s="324"/>
+      <c r="FX2" s="324"/>
+      <c r="FY2" s="324"/>
+      <c r="FZ2" s="324"/>
+      <c r="GA2" s="324"/>
+      <c r="GB2" s="325" t="s">
+        <v>225</v>
+      </c>
+      <c r="GC2" s="326"/>
+      <c r="GD2" s="326"/>
+      <c r="GE2" s="326"/>
+      <c r="GF2" s="326"/>
+      <c r="GG2" s="326"/>
+      <c r="GH2" s="326"/>
+      <c r="GI2" s="326"/>
+      <c r="GJ2" s="326"/>
+      <c r="GK2" s="327"/>
+      <c r="GL2" s="328" t="s">
         <v>226</v>
       </c>
-      <c r="GC2" s="273"/>
-      <c r="GD2" s="273"/>
-      <c r="GE2" s="273"/>
-      <c r="GF2" s="273"/>
-      <c r="GG2" s="273"/>
-      <c r="GH2" s="273"/>
-      <c r="GI2" s="273"/>
-      <c r="GJ2" s="273"/>
-      <c r="GK2" s="274"/>
-      <c r="GL2" s="275" t="s">
-        <v>227</v>
-      </c>
-      <c r="GM2" s="276"/>
-      <c r="GN2" s="276"/>
-      <c r="GO2" s="276"/>
-      <c r="GP2" s="276"/>
-      <c r="GQ2" s="276"/>
-      <c r="GR2" s="276"/>
-      <c r="GS2" s="276"/>
-      <c r="GT2" s="276"/>
-      <c r="GU2" s="276"/>
-      <c r="GV2" s="255" t="s">
-        <v>232</v>
-      </c>
-      <c r="GW2" s="256"/>
-      <c r="GX2" s="256"/>
-      <c r="GY2" s="257"/>
-      <c r="GZ2" s="252" t="s">
-        <v>243</v>
-      </c>
-      <c r="HA2" s="253"/>
-      <c r="HB2" s="253"/>
-      <c r="HC2" s="254"/>
+      <c r="GM2" s="329"/>
+      <c r="GN2" s="329"/>
+      <c r="GO2" s="329"/>
+      <c r="GP2" s="329"/>
+      <c r="GQ2" s="329"/>
+      <c r="GR2" s="329"/>
+      <c r="GS2" s="329"/>
+      <c r="GT2" s="329"/>
+      <c r="GU2" s="329"/>
+      <c r="GV2" s="308" t="s">
+        <v>231</v>
+      </c>
+      <c r="GW2" s="309"/>
+      <c r="GX2" s="309"/>
+      <c r="GY2" s="310"/>
+      <c r="GZ2" s="305" t="s">
+        <v>242</v>
+      </c>
+      <c r="HA2" s="306"/>
+      <c r="HB2" s="306"/>
+      <c r="HC2" s="307"/>
       <c r="HD2" s="90"/>
       <c r="HE2" s="90"/>
       <c r="HF2" s="90"/>
@@ -5912,14 +5924,14 @@
       <c r="HH2" s="90"/>
       <c r="HI2" s="94"/>
       <c r="HJ2" s="95" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="HK2" s="96"/>
       <c r="HL2" s="98"/>
       <c r="HM2" s="109"/>
       <c r="HN2" s="111"/>
     </row>
-    <row r="3" spans="1:222" ht="12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:222" ht="24" x14ac:dyDescent="0.2">
       <c r="A3" s="115" t="s">
         <v>2</v>
       </c>
@@ -6227,19 +6239,19 @@
         <v>204</v>
       </c>
       <c r="CY3" s="170" t="s">
+        <v>211</v>
+      </c>
+      <c r="CZ3" s="171" t="s">
         <v>212</v>
       </c>
-      <c r="CZ3" s="171" t="s">
+      <c r="DA3" s="171" t="s">
         <v>213</v>
       </c>
-      <c r="DA3" s="171" t="s">
+      <c r="DB3" s="172" t="s">
         <v>214</v>
       </c>
-      <c r="DB3" s="172" t="s">
+      <c r="DC3" s="173" t="s">
         <v>215</v>
-      </c>
-      <c r="DC3" s="173" t="s">
-        <v>216</v>
       </c>
       <c r="DD3" s="174" t="s">
         <v>127</v>
@@ -6374,7 +6386,7 @@
         <v>165</v>
       </c>
       <c r="EV3" s="151" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="EW3" s="77" t="s">
         <v>166</v>
@@ -6404,7 +6416,7 @@
         <v>174</v>
       </c>
       <c r="FF3" s="128" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="FG3" s="131" t="s">
         <v>175</v>
@@ -6434,7 +6446,7 @@
         <v>183</v>
       </c>
       <c r="FP3" s="128" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="FQ3" s="131" t="s">
         <v>184</v>
@@ -6464,127 +6476,127 @@
         <v>192</v>
       </c>
       <c r="FZ3" s="128" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="GA3" s="77" t="s">
         <v>193</v>
       </c>
       <c r="GB3" s="176" t="s">
+        <v>243</v>
+      </c>
+      <c r="GC3" s="128" t="s">
         <v>244</v>
       </c>
-      <c r="GC3" s="128" t="s">
+      <c r="GD3" s="128" t="s">
         <v>245</v>
       </c>
-      <c r="GD3" s="128" t="s">
+      <c r="GE3" s="128" t="s">
         <v>246</v>
       </c>
-      <c r="GE3" s="128" t="s">
+      <c r="GF3" s="128" t="s">
         <v>247</v>
       </c>
-      <c r="GF3" s="128" t="s">
+      <c r="GG3" s="129" t="s">
         <v>248</v>
       </c>
-      <c r="GG3" s="129" t="s">
+      <c r="GH3" s="128" t="s">
         <v>249</v>
       </c>
-      <c r="GH3" s="128" t="s">
+      <c r="GI3" s="128" t="s">
         <v>250</v>
       </c>
-      <c r="GI3" s="128" t="s">
+      <c r="GJ3" s="128" t="s">
         <v>251</v>
       </c>
-      <c r="GJ3" s="128" t="s">
+      <c r="GK3" s="77" t="s">
         <v>252</v>
       </c>
-      <c r="GK3" s="77" t="s">
+      <c r="GL3" s="176" t="s">
         <v>253</v>
       </c>
-      <c r="GL3" s="176" t="s">
+      <c r="GM3" s="128" t="s">
         <v>254</v>
       </c>
-      <c r="GM3" s="128" t="s">
+      <c r="GN3" s="128" t="s">
         <v>255</v>
       </c>
-      <c r="GN3" s="128" t="s">
+      <c r="GO3" s="128" t="s">
         <v>256</v>
       </c>
-      <c r="GO3" s="128" t="s">
+      <c r="GP3" s="128" t="s">
         <v>257</v>
       </c>
-      <c r="GP3" s="128" t="s">
+      <c r="GQ3" s="129" t="s">
         <v>258</v>
       </c>
-      <c r="GQ3" s="129" t="s">
+      <c r="GR3" s="128" t="s">
         <v>259</v>
       </c>
-      <c r="GR3" s="128" t="s">
+      <c r="GS3" s="128" t="s">
         <v>260</v>
       </c>
-      <c r="GS3" s="128" t="s">
+      <c r="GT3" s="128" t="s">
         <v>261</v>
       </c>
-      <c r="GT3" s="128" t="s">
+      <c r="GU3" s="77" t="s">
         <v>262</v>
       </c>
-      <c r="GU3" s="77" t="s">
+      <c r="GV3" s="93" t="s">
+        <v>232</v>
+      </c>
+      <c r="GW3" s="93" t="s">
+        <v>233</v>
+      </c>
+      <c r="GX3" s="93" t="s">
+        <v>234</v>
+      </c>
+      <c r="GY3" s="93" t="s">
+        <v>235</v>
+      </c>
+      <c r="GZ3" s="77" t="s">
+        <v>238</v>
+      </c>
+      <c r="HA3" s="77" t="s">
+        <v>239</v>
+      </c>
+      <c r="HB3" s="77" t="s">
+        <v>240</v>
+      </c>
+      <c r="HC3" s="77" t="s">
+        <v>241</v>
+      </c>
+      <c r="HD3" s="77" t="s">
+        <v>218</v>
+      </c>
+      <c r="HE3" s="77" t="s">
+        <v>219</v>
+      </c>
+      <c r="HF3" s="77" t="s">
+        <v>220</v>
+      </c>
+      <c r="HG3" s="77" t="s">
+        <v>221</v>
+      </c>
+      <c r="HH3" s="77" t="s">
+        <v>222</v>
+      </c>
+      <c r="HI3" s="77" t="s">
+        <v>223</v>
+      </c>
+      <c r="HJ3" s="63" t="s">
+        <v>210</v>
+      </c>
+      <c r="HK3" s="177" t="s">
         <v>263</v>
       </c>
-      <c r="GV3" s="93" t="s">
-        <v>233</v>
-      </c>
-      <c r="GW3" s="93" t="s">
-        <v>234</v>
-      </c>
-      <c r="GX3" s="93" t="s">
-        <v>235</v>
-      </c>
-      <c r="GY3" s="93" t="s">
-        <v>236</v>
-      </c>
-      <c r="GZ3" s="77" t="s">
-        <v>239</v>
-      </c>
-      <c r="HA3" s="77" t="s">
-        <v>240</v>
-      </c>
-      <c r="HB3" s="77" t="s">
-        <v>241</v>
-      </c>
-      <c r="HC3" s="77" t="s">
-        <v>242</v>
-      </c>
-      <c r="HD3" s="77" t="s">
-        <v>219</v>
-      </c>
-      <c r="HE3" s="77" t="s">
-        <v>220</v>
-      </c>
-      <c r="HF3" s="77" t="s">
-        <v>221</v>
-      </c>
-      <c r="HG3" s="77" t="s">
-        <v>222</v>
-      </c>
-      <c r="HH3" s="77" t="s">
-        <v>223</v>
-      </c>
-      <c r="HI3" s="77" t="s">
-        <v>224</v>
-      </c>
-      <c r="HJ3" s="63" t="s">
-        <v>211</v>
-      </c>
-      <c r="HK3" s="177" t="s">
-        <v>210</v>
-      </c>
       <c r="HL3" s="178" t="s">
+        <v>228</v>
+      </c>
+      <c r="HM3" s="179" t="s">
         <v>229</v>
       </c>
-      <c r="HM3" s="179" t="s">
-        <v>230</v>
-      </c>
       <c r="HN3" s="180" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="4" spans="1:222" s="60" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11526,8 +11538,30 @@
     <protectedRange password="CB1D" sqref="A22:BA22" name="InsertData_1" securityDescriptor="O:WDG:WDD:(A;;CC;;;S-1-5-21-343818398-1326574676-839522115-1136)(A;;CC;;;S-1-5-21-343818398-1326574676-839522115-1142)(A;;CC;;;S-1-5-21-343818398-1326574676-839522115-1141)(A;;CC;;;S-1-5-21-343818398-1326574676-839522115-1137)"/>
     <protectedRange password="CB1D" sqref="DD22:DI22" name="InsertData_2_1" securityDescriptor="O:WDG:WDD:(A;;CC;;;S-1-5-21-343818398-1326574676-839522115-1136)(A;;CC;;;S-1-5-21-343818398-1326574676-839522115-1142)(A;;CC;;;S-1-5-21-343818398-1326574676-839522115-1141)(A;;CC;;;S-1-5-21-343818398-1326574676-839522115-1137)"/>
   </protectedRanges>
-  <autoFilter ref="A3:HK32"/>
+  <autoFilter ref="A3:HK32" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
   <mergeCells count="38">
+    <mergeCell ref="HD1:HI1"/>
+    <mergeCell ref="GZ2:HC2"/>
+    <mergeCell ref="GV2:GY2"/>
+    <mergeCell ref="GV1:GY1"/>
+    <mergeCell ref="EN2:EW2"/>
+    <mergeCell ref="EX2:FG2"/>
+    <mergeCell ref="FH2:FQ2"/>
+    <mergeCell ref="FR2:GA2"/>
+    <mergeCell ref="GB2:GK2"/>
+    <mergeCell ref="GL2:GU2"/>
+    <mergeCell ref="EN1:GU1"/>
+    <mergeCell ref="AL2:AU2"/>
+    <mergeCell ref="AV2:BB2"/>
+    <mergeCell ref="BO2:BY2"/>
+    <mergeCell ref="BJ2:BN2"/>
+    <mergeCell ref="DD1:EM1"/>
+    <mergeCell ref="DO2:DS2"/>
+    <mergeCell ref="DD2:DN2"/>
+    <mergeCell ref="CO2:CS2"/>
+    <mergeCell ref="DY2:EC2"/>
+    <mergeCell ref="ED2:EH2"/>
+    <mergeCell ref="EI2:EM2"/>
     <mergeCell ref="A2:I2"/>
     <mergeCell ref="M2:T2"/>
     <mergeCell ref="M1:BB1"/>
@@ -11544,28 +11578,6 @@
     <mergeCell ref="BC2:BI2"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="U2:AK2"/>
-    <mergeCell ref="AL2:AU2"/>
-    <mergeCell ref="AV2:BB2"/>
-    <mergeCell ref="BO2:BY2"/>
-    <mergeCell ref="BJ2:BN2"/>
-    <mergeCell ref="DD1:EM1"/>
-    <mergeCell ref="DO2:DS2"/>
-    <mergeCell ref="DD2:DN2"/>
-    <mergeCell ref="CO2:CS2"/>
-    <mergeCell ref="DY2:EC2"/>
-    <mergeCell ref="ED2:EH2"/>
-    <mergeCell ref="EI2:EM2"/>
-    <mergeCell ref="HD1:HI1"/>
-    <mergeCell ref="GZ2:HC2"/>
-    <mergeCell ref="GV2:GY2"/>
-    <mergeCell ref="GV1:GY1"/>
-    <mergeCell ref="EN2:EW2"/>
-    <mergeCell ref="EX2:FG2"/>
-    <mergeCell ref="FH2:FQ2"/>
-    <mergeCell ref="FR2:GA2"/>
-    <mergeCell ref="GB2:GK2"/>
-    <mergeCell ref="GL2:GU2"/>
-    <mergeCell ref="EN1:GU1"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Passport Batch export update
</commit_message>
<xml_diff>
--- a/UDM.Insurance.Interface/Templates/ReportTemplateBatchExport.xlsx
+++ b/UDM.Insurance.Interface/Templates/ReportTemplateBatchExport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DaneB\source\repos\Insure\UDM.Insurance.Interface\Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TyronR\Desktop\Source\udminsure\UDM.Insurance.Interface\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BC9CF4F-6105-4835-B0CE-00DAC138EF01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBED9518-C9E4-4FF5-ABBA-98A622AE81D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24120" yWindow="1185" windowWidth="24240" windowHeight="13140" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24120" yWindow="3345" windowWidth="24240" windowHeight="13020" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Batch Cover Sheet" sheetId="2" r:id="rId1"/>
@@ -695,15 +695,6 @@
     <t>Future Field5</t>
   </si>
   <si>
-    <t>Future Field6</t>
-  </si>
-  <si>
-    <t>Future Field7</t>
-  </si>
-  <si>
-    <t>Future Field8</t>
-  </si>
-  <si>
     <t>Future Field9</t>
   </si>
   <si>
@@ -828,6 +819,15 @@
   </si>
   <si>
     <t>Mandate Response</t>
+  </si>
+  <si>
+    <t>LA1 Passport</t>
+  </si>
+  <si>
+    <t>LA2 Passport</t>
+  </si>
+  <si>
+    <t>Premium Payer Passport Number</t>
   </si>
 </sst>
 </file>
@@ -2158,22 +2158,40 @@
     <xf numFmtId="49" fontId="8" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="2" fillId="12" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="12" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="12" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="5" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="5" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="5" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="5" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="5" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="12" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -2185,15 +2203,6 @@
     <xf numFmtId="164" fontId="3" fillId="12" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="12" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="12" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="12" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
-    </xf>
     <xf numFmtId="4" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -2201,51 +2210,6 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="4" fontId="2" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="12" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="12" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="12" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="12" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="12" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -2272,23 +2236,41 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="167" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="5" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="5" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="5" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="5" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="5" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="12" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="12" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="12" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="12" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="12" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="22" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -2314,6 +2296,15 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
+    </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -2332,118 +2323,103 @@
     <xf numFmtId="0" fontId="3" fillId="22" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="26" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="26" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="26" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="8" fillId="19" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="8" fillId="19" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="8" fillId="19" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="15" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="15" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="15" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="12" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="12" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="12" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="16" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="16" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="16" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="11" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="11" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="23" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="23" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="23" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="24" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="24" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="9" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="7" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="7" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="7" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="8" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="8" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="8" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="10" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="10" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="10" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="6" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="6" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="13" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="13" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="13" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="14" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="14" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="14" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="6" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="6" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="6" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="21" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="21" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="21" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="5" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="5" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="11" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2476,6 +2452,15 @@
     <xf numFmtId="49" fontId="8" fillId="5" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="8" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -2485,6 +2470,15 @@
     <xf numFmtId="49" fontId="8" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="8" fillId="6" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="6" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="6" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="8" fillId="9" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -2494,88 +2488,94 @@
     <xf numFmtId="49" fontId="8" fillId="9" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="8" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="8" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="8" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="26" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="10" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="26" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="10" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="26" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="10" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="19" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="19" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="19" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="7" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="7" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="15" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="7" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="15" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="6" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="15" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="6" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="12" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="12" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="13" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="12" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="13" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="16" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="13" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="16" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="14" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="16" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="14" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="11" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="14" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="11" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="21" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="23" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="21" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="23" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="21" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="23" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="5" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="24" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="5" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="24" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3090,14 +3090,14 @@
       <selection activeCell="B31" sqref="B31:W32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="24" width="3.7109375" style="42" customWidth="1"/>
-    <col min="25" max="25" width="3.7109375" style="42" hidden="1" customWidth="1"/>
+    <col min="1" max="24" width="3.7265625" style="42" customWidth="1"/>
+    <col min="25" max="25" width="3.7265625" style="42" hidden="1" customWidth="1"/>
     <col min="26" max="16384" width="0" style="8" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7"/>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -3124,7 +3124,7 @@
       <c r="X1" s="7"/>
       <c r="Y1" s="7"/>
     </row>
-    <row r="2" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
@@ -3151,7 +3151,7 @@
       <c r="X2" s="7"/>
       <c r="Y2" s="7"/>
     </row>
-    <row r="3" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
@@ -3178,7 +3178,7 @@
       <c r="X3" s="7"/>
       <c r="Y3" s="7"/>
     </row>
-    <row r="4" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7"/>
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
@@ -3205,7 +3205,7 @@
       <c r="X4" s="7"/>
       <c r="Y4" s="7"/>
     </row>
-    <row r="5" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
@@ -3232,7 +3232,7 @@
       <c r="X5" s="7"/>
       <c r="Y5" s="7"/>
     </row>
-    <row r="6" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
@@ -3259,7 +3259,7 @@
       <c r="X6" s="7"/>
       <c r="Y6" s="7"/>
     </row>
-    <row r="7" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
@@ -3286,7 +3286,7 @@
       <c r="X7" s="7"/>
       <c r="Y7" s="7"/>
     </row>
-    <row r="8" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
@@ -3313,7 +3313,7 @@
       <c r="X8" s="7"/>
       <c r="Y8" s="7"/>
     </row>
-    <row r="9" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
@@ -3340,7 +3340,7 @@
       <c r="X9" s="7"/>
       <c r="Y9" s="7"/>
     </row>
-    <row r="10" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10"/>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -3367,63 +3367,63 @@
       <c r="X10" s="12"/>
       <c r="Y10" s="12"/>
     </row>
-    <row r="11" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="13"/>
-      <c r="B11" s="210" t="s">
+      <c r="B11" s="225" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="211"/>
-      <c r="D11" s="211"/>
-      <c r="E11" s="211"/>
-      <c r="F11" s="211"/>
-      <c r="G11" s="211"/>
-      <c r="H11" s="211"/>
-      <c r="I11" s="211"/>
-      <c r="J11" s="211"/>
-      <c r="K11" s="211"/>
-      <c r="L11" s="211"/>
-      <c r="M11" s="211"/>
-      <c r="N11" s="211"/>
-      <c r="O11" s="211"/>
-      <c r="P11" s="211"/>
-      <c r="Q11" s="211"/>
-      <c r="R11" s="211"/>
-      <c r="S11" s="211"/>
-      <c r="T11" s="211"/>
-      <c r="U11" s="211"/>
-      <c r="V11" s="211"/>
-      <c r="W11" s="212"/>
+      <c r="C11" s="226"/>
+      <c r="D11" s="226"/>
+      <c r="E11" s="226"/>
+      <c r="F11" s="226"/>
+      <c r="G11" s="226"/>
+      <c r="H11" s="226"/>
+      <c r="I11" s="226"/>
+      <c r="J11" s="226"/>
+      <c r="K11" s="226"/>
+      <c r="L11" s="226"/>
+      <c r="M11" s="226"/>
+      <c r="N11" s="226"/>
+      <c r="O11" s="226"/>
+      <c r="P11" s="226"/>
+      <c r="Q11" s="226"/>
+      <c r="R11" s="226"/>
+      <c r="S11" s="226"/>
+      <c r="T11" s="226"/>
+      <c r="U11" s="226"/>
+      <c r="V11" s="226"/>
+      <c r="W11" s="227"/>
       <c r="X11" s="14"/>
       <c r="Y11" s="15"/>
     </row>
-    <row r="12" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="16"/>
-      <c r="B12" s="213"/>
-      <c r="C12" s="214"/>
-      <c r="D12" s="214"/>
-      <c r="E12" s="214"/>
-      <c r="F12" s="214"/>
-      <c r="G12" s="214"/>
-      <c r="H12" s="214"/>
-      <c r="I12" s="214"/>
-      <c r="J12" s="214"/>
-      <c r="K12" s="214"/>
-      <c r="L12" s="214"/>
-      <c r="M12" s="214"/>
-      <c r="N12" s="214"/>
-      <c r="O12" s="214"/>
-      <c r="P12" s="214"/>
-      <c r="Q12" s="214"/>
-      <c r="R12" s="214"/>
-      <c r="S12" s="214"/>
-      <c r="T12" s="214"/>
-      <c r="U12" s="214"/>
-      <c r="V12" s="214"/>
-      <c r="W12" s="215"/>
+      <c r="B12" s="228"/>
+      <c r="C12" s="229"/>
+      <c r="D12" s="229"/>
+      <c r="E12" s="229"/>
+      <c r="F12" s="229"/>
+      <c r="G12" s="229"/>
+      <c r="H12" s="229"/>
+      <c r="I12" s="229"/>
+      <c r="J12" s="229"/>
+      <c r="K12" s="229"/>
+      <c r="L12" s="229"/>
+      <c r="M12" s="229"/>
+      <c r="N12" s="229"/>
+      <c r="O12" s="229"/>
+      <c r="P12" s="229"/>
+      <c r="Q12" s="229"/>
+      <c r="R12" s="229"/>
+      <c r="S12" s="229"/>
+      <c r="T12" s="229"/>
+      <c r="U12" s="229"/>
+      <c r="V12" s="229"/>
+      <c r="W12" s="230"/>
       <c r="X12" s="14"/>
       <c r="Y12" s="15"/>
     </row>
-    <row r="13" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="16"/>
       <c r="B13" s="17"/>
       <c r="C13" s="17"/>
@@ -3450,92 +3450,92 @@
       <c r="X13" s="18"/>
       <c r="Y13" s="15"/>
     </row>
-    <row r="14" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="13"/>
-      <c r="B14" s="201" t="s">
+      <c r="B14" s="207" t="s">
         <v>0</v>
       </c>
-      <c r="C14" s="202"/>
-      <c r="D14" s="202"/>
-      <c r="E14" s="202"/>
-      <c r="F14" s="202"/>
-      <c r="G14" s="202"/>
-      <c r="H14" s="202"/>
-      <c r="I14" s="202"/>
-      <c r="J14" s="202"/>
-      <c r="K14" s="202"/>
-      <c r="L14" s="202"/>
-      <c r="M14" s="202"/>
-      <c r="N14" s="202"/>
-      <c r="O14" s="202"/>
-      <c r="P14" s="202"/>
-      <c r="Q14" s="202"/>
-      <c r="R14" s="202"/>
-      <c r="S14" s="202"/>
-      <c r="T14" s="202"/>
-      <c r="U14" s="202"/>
-      <c r="V14" s="202"/>
-      <c r="W14" s="203"/>
+      <c r="C14" s="208"/>
+      <c r="D14" s="208"/>
+      <c r="E14" s="208"/>
+      <c r="F14" s="208"/>
+      <c r="G14" s="208"/>
+      <c r="H14" s="208"/>
+      <c r="I14" s="208"/>
+      <c r="J14" s="208"/>
+      <c r="K14" s="208"/>
+      <c r="L14" s="208"/>
+      <c r="M14" s="208"/>
+      <c r="N14" s="208"/>
+      <c r="O14" s="208"/>
+      <c r="P14" s="208"/>
+      <c r="Q14" s="208"/>
+      <c r="R14" s="208"/>
+      <c r="S14" s="208"/>
+      <c r="T14" s="208"/>
+      <c r="U14" s="208"/>
+      <c r="V14" s="208"/>
+      <c r="W14" s="209"/>
       <c r="X14" s="19"/>
       <c r="Y14" s="15"/>
     </row>
-    <row r="15" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="16"/>
-      <c r="B15" s="216" t="s">
+      <c r="B15" s="201" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="217"/>
-      <c r="D15" s="217"/>
-      <c r="E15" s="217"/>
-      <c r="F15" s="217"/>
-      <c r="G15" s="217"/>
-      <c r="H15" s="217"/>
-      <c r="I15" s="217"/>
-      <c r="J15" s="217"/>
-      <c r="K15" s="217"/>
-      <c r="L15" s="217"/>
-      <c r="M15" s="217"/>
-      <c r="N15" s="217"/>
-      <c r="O15" s="217"/>
-      <c r="P15" s="217"/>
-      <c r="Q15" s="217"/>
-      <c r="R15" s="217"/>
-      <c r="S15" s="217"/>
-      <c r="T15" s="217"/>
-      <c r="U15" s="217"/>
-      <c r="V15" s="217"/>
-      <c r="W15" s="218"/>
+      <c r="C15" s="202"/>
+      <c r="D15" s="202"/>
+      <c r="E15" s="202"/>
+      <c r="F15" s="202"/>
+      <c r="G15" s="202"/>
+      <c r="H15" s="202"/>
+      <c r="I15" s="202"/>
+      <c r="J15" s="202"/>
+      <c r="K15" s="202"/>
+      <c r="L15" s="202"/>
+      <c r="M15" s="202"/>
+      <c r="N15" s="202"/>
+      <c r="O15" s="202"/>
+      <c r="P15" s="202"/>
+      <c r="Q15" s="202"/>
+      <c r="R15" s="202"/>
+      <c r="S15" s="202"/>
+      <c r="T15" s="202"/>
+      <c r="U15" s="202"/>
+      <c r="V15" s="202"/>
+      <c r="W15" s="203"/>
       <c r="X15" s="20"/>
       <c r="Y15" s="15"/>
     </row>
-    <row r="16" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="16"/>
-      <c r="B16" s="219"/>
-      <c r="C16" s="220"/>
-      <c r="D16" s="220"/>
-      <c r="E16" s="220"/>
-      <c r="F16" s="220"/>
-      <c r="G16" s="220"/>
-      <c r="H16" s="220"/>
-      <c r="I16" s="220"/>
-      <c r="J16" s="220"/>
-      <c r="K16" s="220"/>
-      <c r="L16" s="220"/>
-      <c r="M16" s="220"/>
-      <c r="N16" s="220"/>
-      <c r="O16" s="220"/>
-      <c r="P16" s="220"/>
-      <c r="Q16" s="220"/>
-      <c r="R16" s="220"/>
-      <c r="S16" s="220"/>
-      <c r="T16" s="220"/>
-      <c r="U16" s="220"/>
-      <c r="V16" s="220"/>
-      <c r="W16" s="221"/>
+      <c r="B16" s="204"/>
+      <c r="C16" s="205"/>
+      <c r="D16" s="205"/>
+      <c r="E16" s="205"/>
+      <c r="F16" s="205"/>
+      <c r="G16" s="205"/>
+      <c r="H16" s="205"/>
+      <c r="I16" s="205"/>
+      <c r="J16" s="205"/>
+      <c r="K16" s="205"/>
+      <c r="L16" s="205"/>
+      <c r="M16" s="205"/>
+      <c r="N16" s="205"/>
+      <c r="O16" s="205"/>
+      <c r="P16" s="205"/>
+      <c r="Q16" s="205"/>
+      <c r="R16" s="205"/>
+      <c r="S16" s="205"/>
+      <c r="T16" s="205"/>
+      <c r="U16" s="205"/>
+      <c r="V16" s="205"/>
+      <c r="W16" s="206"/>
       <c r="X16" s="20"/>
       <c r="Y16" s="15"/>
     </row>
-    <row r="17" spans="1:25" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:25" ht="5.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="16"/>
       <c r="B17" s="21"/>
       <c r="C17" s="21"/>
@@ -3562,90 +3562,90 @@
       <c r="X17" s="22"/>
       <c r="Y17" s="15"/>
     </row>
-    <row r="18" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="16"/>
-      <c r="B18" s="201" t="s">
+      <c r="B18" s="207" t="s">
         <v>1</v>
       </c>
-      <c r="C18" s="202"/>
-      <c r="D18" s="202"/>
-      <c r="E18" s="202"/>
-      <c r="F18" s="202"/>
-      <c r="G18" s="202"/>
-      <c r="H18" s="202"/>
-      <c r="I18" s="202"/>
-      <c r="J18" s="202"/>
-      <c r="K18" s="202"/>
-      <c r="L18" s="202"/>
-      <c r="M18" s="202"/>
-      <c r="N18" s="202"/>
-      <c r="O18" s="202"/>
-      <c r="P18" s="202"/>
-      <c r="Q18" s="202"/>
-      <c r="R18" s="202"/>
-      <c r="S18" s="202"/>
-      <c r="T18" s="202"/>
-      <c r="U18" s="202"/>
-      <c r="V18" s="202"/>
-      <c r="W18" s="203"/>
+      <c r="C18" s="208"/>
+      <c r="D18" s="208"/>
+      <c r="E18" s="208"/>
+      <c r="F18" s="208"/>
+      <c r="G18" s="208"/>
+      <c r="H18" s="208"/>
+      <c r="I18" s="208"/>
+      <c r="J18" s="208"/>
+      <c r="K18" s="208"/>
+      <c r="L18" s="208"/>
+      <c r="M18" s="208"/>
+      <c r="N18" s="208"/>
+      <c r="O18" s="208"/>
+      <c r="P18" s="208"/>
+      <c r="Q18" s="208"/>
+      <c r="R18" s="208"/>
+      <c r="S18" s="208"/>
+      <c r="T18" s="208"/>
+      <c r="U18" s="208"/>
+      <c r="V18" s="208"/>
+      <c r="W18" s="209"/>
       <c r="X18" s="19"/>
       <c r="Y18" s="15"/>
     </row>
-    <row r="19" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="16"/>
-      <c r="B19" s="216"/>
-      <c r="C19" s="217"/>
-      <c r="D19" s="217"/>
-      <c r="E19" s="217"/>
-      <c r="F19" s="217"/>
-      <c r="G19" s="217"/>
-      <c r="H19" s="217"/>
-      <c r="I19" s="217"/>
-      <c r="J19" s="217"/>
-      <c r="K19" s="217"/>
-      <c r="L19" s="217"/>
-      <c r="M19" s="217"/>
-      <c r="N19" s="217"/>
-      <c r="O19" s="217"/>
-      <c r="P19" s="217"/>
-      <c r="Q19" s="217"/>
-      <c r="R19" s="217"/>
-      <c r="S19" s="217"/>
-      <c r="T19" s="217"/>
-      <c r="U19" s="217"/>
-      <c r="V19" s="217"/>
-      <c r="W19" s="218"/>
+      <c r="B19" s="201"/>
+      <c r="C19" s="202"/>
+      <c r="D19" s="202"/>
+      <c r="E19" s="202"/>
+      <c r="F19" s="202"/>
+      <c r="G19" s="202"/>
+      <c r="H19" s="202"/>
+      <c r="I19" s="202"/>
+      <c r="J19" s="202"/>
+      <c r="K19" s="202"/>
+      <c r="L19" s="202"/>
+      <c r="M19" s="202"/>
+      <c r="N19" s="202"/>
+      <c r="O19" s="202"/>
+      <c r="P19" s="202"/>
+      <c r="Q19" s="202"/>
+      <c r="R19" s="202"/>
+      <c r="S19" s="202"/>
+      <c r="T19" s="202"/>
+      <c r="U19" s="202"/>
+      <c r="V19" s="202"/>
+      <c r="W19" s="203"/>
       <c r="X19" s="20"/>
       <c r="Y19" s="15"/>
     </row>
-    <row r="20" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="16"/>
-      <c r="B20" s="219"/>
-      <c r="C20" s="220"/>
-      <c r="D20" s="220"/>
-      <c r="E20" s="220"/>
-      <c r="F20" s="220"/>
-      <c r="G20" s="220"/>
-      <c r="H20" s="220"/>
-      <c r="I20" s="220"/>
-      <c r="J20" s="220"/>
-      <c r="K20" s="220"/>
-      <c r="L20" s="220"/>
-      <c r="M20" s="220"/>
-      <c r="N20" s="220"/>
-      <c r="O20" s="220"/>
-      <c r="P20" s="220"/>
-      <c r="Q20" s="220"/>
-      <c r="R20" s="220"/>
-      <c r="S20" s="220"/>
-      <c r="T20" s="220"/>
-      <c r="U20" s="220"/>
-      <c r="V20" s="220"/>
-      <c r="W20" s="221"/>
+      <c r="B20" s="204"/>
+      <c r="C20" s="205"/>
+      <c r="D20" s="205"/>
+      <c r="E20" s="205"/>
+      <c r="F20" s="205"/>
+      <c r="G20" s="205"/>
+      <c r="H20" s="205"/>
+      <c r="I20" s="205"/>
+      <c r="J20" s="205"/>
+      <c r="K20" s="205"/>
+      <c r="L20" s="205"/>
+      <c r="M20" s="205"/>
+      <c r="N20" s="205"/>
+      <c r="O20" s="205"/>
+      <c r="P20" s="205"/>
+      <c r="Q20" s="205"/>
+      <c r="R20" s="205"/>
+      <c r="S20" s="205"/>
+      <c r="T20" s="205"/>
+      <c r="U20" s="205"/>
+      <c r="V20" s="205"/>
+      <c r="W20" s="206"/>
       <c r="X20" s="20"/>
       <c r="Y20" s="15"/>
     </row>
-    <row r="21" spans="1:25" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:25" ht="5.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="16"/>
       <c r="B21" s="21"/>
       <c r="C21" s="21"/>
@@ -3672,90 +3672,90 @@
       <c r="X21" s="22"/>
       <c r="Y21" s="15"/>
     </row>
-    <row r="22" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="16"/>
-      <c r="B22" s="201" t="s">
+      <c r="B22" s="207" t="s">
         <v>2</v>
       </c>
-      <c r="C22" s="202"/>
-      <c r="D22" s="202"/>
-      <c r="E22" s="202"/>
-      <c r="F22" s="202"/>
-      <c r="G22" s="202"/>
-      <c r="H22" s="202"/>
-      <c r="I22" s="202"/>
-      <c r="J22" s="202"/>
-      <c r="K22" s="202"/>
-      <c r="L22" s="202"/>
-      <c r="M22" s="202"/>
-      <c r="N22" s="202"/>
-      <c r="O22" s="202"/>
-      <c r="P22" s="202"/>
-      <c r="Q22" s="202"/>
-      <c r="R22" s="202"/>
-      <c r="S22" s="202"/>
-      <c r="T22" s="202"/>
-      <c r="U22" s="202"/>
-      <c r="V22" s="202"/>
-      <c r="W22" s="203"/>
+      <c r="C22" s="208"/>
+      <c r="D22" s="208"/>
+      <c r="E22" s="208"/>
+      <c r="F22" s="208"/>
+      <c r="G22" s="208"/>
+      <c r="H22" s="208"/>
+      <c r="I22" s="208"/>
+      <c r="J22" s="208"/>
+      <c r="K22" s="208"/>
+      <c r="L22" s="208"/>
+      <c r="M22" s="208"/>
+      <c r="N22" s="208"/>
+      <c r="O22" s="208"/>
+      <c r="P22" s="208"/>
+      <c r="Q22" s="208"/>
+      <c r="R22" s="208"/>
+      <c r="S22" s="208"/>
+      <c r="T22" s="208"/>
+      <c r="U22" s="208"/>
+      <c r="V22" s="208"/>
+      <c r="W22" s="209"/>
       <c r="X22" s="19"/>
       <c r="Y22" s="15"/>
     </row>
-    <row r="23" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="16"/>
-      <c r="B23" s="216"/>
-      <c r="C23" s="217"/>
-      <c r="D23" s="217"/>
-      <c r="E23" s="217"/>
-      <c r="F23" s="217"/>
-      <c r="G23" s="217"/>
-      <c r="H23" s="217"/>
-      <c r="I23" s="217"/>
-      <c r="J23" s="217"/>
-      <c r="K23" s="217"/>
-      <c r="L23" s="217"/>
-      <c r="M23" s="217"/>
-      <c r="N23" s="217"/>
-      <c r="O23" s="217"/>
-      <c r="P23" s="217"/>
-      <c r="Q23" s="217"/>
-      <c r="R23" s="217"/>
-      <c r="S23" s="217"/>
-      <c r="T23" s="217"/>
-      <c r="U23" s="217"/>
-      <c r="V23" s="217"/>
-      <c r="W23" s="218"/>
+      <c r="B23" s="201"/>
+      <c r="C23" s="202"/>
+      <c r="D23" s="202"/>
+      <c r="E23" s="202"/>
+      <c r="F23" s="202"/>
+      <c r="G23" s="202"/>
+      <c r="H23" s="202"/>
+      <c r="I23" s="202"/>
+      <c r="J23" s="202"/>
+      <c r="K23" s="202"/>
+      <c r="L23" s="202"/>
+      <c r="M23" s="202"/>
+      <c r="N23" s="202"/>
+      <c r="O23" s="202"/>
+      <c r="P23" s="202"/>
+      <c r="Q23" s="202"/>
+      <c r="R23" s="202"/>
+      <c r="S23" s="202"/>
+      <c r="T23" s="202"/>
+      <c r="U23" s="202"/>
+      <c r="V23" s="202"/>
+      <c r="W23" s="203"/>
       <c r="X23" s="20"/>
       <c r="Y23" s="15"/>
     </row>
-    <row r="24" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="16"/>
-      <c r="B24" s="219"/>
-      <c r="C24" s="220"/>
-      <c r="D24" s="220"/>
-      <c r="E24" s="220"/>
-      <c r="F24" s="220"/>
-      <c r="G24" s="220"/>
-      <c r="H24" s="220"/>
-      <c r="I24" s="220"/>
-      <c r="J24" s="220"/>
-      <c r="K24" s="220"/>
-      <c r="L24" s="220"/>
-      <c r="M24" s="220"/>
-      <c r="N24" s="220"/>
-      <c r="O24" s="220"/>
-      <c r="P24" s="220"/>
-      <c r="Q24" s="220"/>
-      <c r="R24" s="220"/>
-      <c r="S24" s="220"/>
-      <c r="T24" s="220"/>
-      <c r="U24" s="220"/>
-      <c r="V24" s="220"/>
-      <c r="W24" s="221"/>
+      <c r="B24" s="204"/>
+      <c r="C24" s="205"/>
+      <c r="D24" s="205"/>
+      <c r="E24" s="205"/>
+      <c r="F24" s="205"/>
+      <c r="G24" s="205"/>
+      <c r="H24" s="205"/>
+      <c r="I24" s="205"/>
+      <c r="J24" s="205"/>
+      <c r="K24" s="205"/>
+      <c r="L24" s="205"/>
+      <c r="M24" s="205"/>
+      <c r="N24" s="205"/>
+      <c r="O24" s="205"/>
+      <c r="P24" s="205"/>
+      <c r="Q24" s="205"/>
+      <c r="R24" s="205"/>
+      <c r="S24" s="205"/>
+      <c r="T24" s="205"/>
+      <c r="U24" s="205"/>
+      <c r="V24" s="205"/>
+      <c r="W24" s="206"/>
       <c r="X24" s="20"/>
       <c r="Y24" s="15"/>
     </row>
-    <row r="25" spans="1:25" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:25" ht="5.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="16"/>
       <c r="B25" s="21"/>
       <c r="C25" s="21"/>
@@ -3782,90 +3782,90 @@
       <c r="X25" s="22"/>
       <c r="Y25" s="15"/>
     </row>
-    <row r="26" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="16"/>
-      <c r="B26" s="201" t="s">
+      <c r="B26" s="207" t="s">
         <v>3</v>
       </c>
-      <c r="C26" s="202"/>
-      <c r="D26" s="202"/>
-      <c r="E26" s="202"/>
-      <c r="F26" s="202"/>
-      <c r="G26" s="202"/>
-      <c r="H26" s="202"/>
-      <c r="I26" s="202"/>
-      <c r="J26" s="202"/>
-      <c r="K26" s="202"/>
-      <c r="L26" s="202"/>
-      <c r="M26" s="202"/>
-      <c r="N26" s="202"/>
-      <c r="O26" s="202"/>
-      <c r="P26" s="202"/>
-      <c r="Q26" s="202"/>
-      <c r="R26" s="202"/>
-      <c r="S26" s="202"/>
-      <c r="T26" s="202"/>
-      <c r="U26" s="202"/>
-      <c r="V26" s="202"/>
-      <c r="W26" s="203"/>
+      <c r="C26" s="208"/>
+      <c r="D26" s="208"/>
+      <c r="E26" s="208"/>
+      <c r="F26" s="208"/>
+      <c r="G26" s="208"/>
+      <c r="H26" s="208"/>
+      <c r="I26" s="208"/>
+      <c r="J26" s="208"/>
+      <c r="K26" s="208"/>
+      <c r="L26" s="208"/>
+      <c r="M26" s="208"/>
+      <c r="N26" s="208"/>
+      <c r="O26" s="208"/>
+      <c r="P26" s="208"/>
+      <c r="Q26" s="208"/>
+      <c r="R26" s="208"/>
+      <c r="S26" s="208"/>
+      <c r="T26" s="208"/>
+      <c r="U26" s="208"/>
+      <c r="V26" s="208"/>
+      <c r="W26" s="209"/>
       <c r="X26" s="19"/>
       <c r="Y26" s="15"/>
     </row>
-    <row r="27" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="16"/>
-      <c r="B27" s="225"/>
-      <c r="C27" s="226"/>
-      <c r="D27" s="226"/>
-      <c r="E27" s="226"/>
-      <c r="F27" s="226"/>
-      <c r="G27" s="226"/>
-      <c r="H27" s="226"/>
-      <c r="I27" s="226"/>
-      <c r="J27" s="226"/>
-      <c r="K27" s="226"/>
-      <c r="L27" s="226"/>
-      <c r="M27" s="226"/>
-      <c r="N27" s="226"/>
-      <c r="O27" s="226"/>
-      <c r="P27" s="226"/>
-      <c r="Q27" s="226"/>
-      <c r="R27" s="226"/>
-      <c r="S27" s="226"/>
-      <c r="T27" s="226"/>
-      <c r="U27" s="226"/>
-      <c r="V27" s="226"/>
-      <c r="W27" s="227"/>
+      <c r="B27" s="213"/>
+      <c r="C27" s="214"/>
+      <c r="D27" s="214"/>
+      <c r="E27" s="214"/>
+      <c r="F27" s="214"/>
+      <c r="G27" s="214"/>
+      <c r="H27" s="214"/>
+      <c r="I27" s="214"/>
+      <c r="J27" s="214"/>
+      <c r="K27" s="214"/>
+      <c r="L27" s="214"/>
+      <c r="M27" s="214"/>
+      <c r="N27" s="214"/>
+      <c r="O27" s="214"/>
+      <c r="P27" s="214"/>
+      <c r="Q27" s="214"/>
+      <c r="R27" s="214"/>
+      <c r="S27" s="214"/>
+      <c r="T27" s="214"/>
+      <c r="U27" s="214"/>
+      <c r="V27" s="214"/>
+      <c r="W27" s="215"/>
       <c r="X27" s="23"/>
       <c r="Y27" s="15"/>
     </row>
-    <row r="28" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="16"/>
-      <c r="B28" s="228"/>
-      <c r="C28" s="229"/>
-      <c r="D28" s="229"/>
-      <c r="E28" s="229"/>
-      <c r="F28" s="229"/>
-      <c r="G28" s="229"/>
-      <c r="H28" s="229"/>
-      <c r="I28" s="229"/>
-      <c r="J28" s="229"/>
-      <c r="K28" s="229"/>
-      <c r="L28" s="229"/>
-      <c r="M28" s="229"/>
-      <c r="N28" s="229"/>
-      <c r="O28" s="229"/>
-      <c r="P28" s="229"/>
-      <c r="Q28" s="229"/>
-      <c r="R28" s="229"/>
-      <c r="S28" s="229"/>
-      <c r="T28" s="229"/>
-      <c r="U28" s="229"/>
-      <c r="V28" s="229"/>
-      <c r="W28" s="230"/>
+      <c r="B28" s="216"/>
+      <c r="C28" s="217"/>
+      <c r="D28" s="217"/>
+      <c r="E28" s="217"/>
+      <c r="F28" s="217"/>
+      <c r="G28" s="217"/>
+      <c r="H28" s="217"/>
+      <c r="I28" s="217"/>
+      <c r="J28" s="217"/>
+      <c r="K28" s="217"/>
+      <c r="L28" s="217"/>
+      <c r="M28" s="217"/>
+      <c r="N28" s="217"/>
+      <c r="O28" s="217"/>
+      <c r="P28" s="217"/>
+      <c r="Q28" s="217"/>
+      <c r="R28" s="217"/>
+      <c r="S28" s="217"/>
+      <c r="T28" s="217"/>
+      <c r="U28" s="217"/>
+      <c r="V28" s="217"/>
+      <c r="W28" s="218"/>
       <c r="X28" s="23"/>
       <c r="Y28" s="15"/>
     </row>
-    <row r="29" spans="1:25" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:25" ht="5.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="16"/>
       <c r="B29" s="21"/>
       <c r="C29" s="21"/>
@@ -3892,90 +3892,90 @@
       <c r="X29" s="22"/>
       <c r="Y29" s="15"/>
     </row>
-    <row r="30" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="16"/>
-      <c r="B30" s="201" t="s">
+      <c r="B30" s="207" t="s">
         <v>4</v>
       </c>
-      <c r="C30" s="202"/>
-      <c r="D30" s="202"/>
-      <c r="E30" s="202"/>
-      <c r="F30" s="202"/>
-      <c r="G30" s="202"/>
-      <c r="H30" s="202"/>
-      <c r="I30" s="202"/>
-      <c r="J30" s="202"/>
-      <c r="K30" s="202"/>
-      <c r="L30" s="202"/>
-      <c r="M30" s="202"/>
-      <c r="N30" s="202"/>
-      <c r="O30" s="202"/>
-      <c r="P30" s="202"/>
-      <c r="Q30" s="202"/>
-      <c r="R30" s="202"/>
-      <c r="S30" s="202"/>
-      <c r="T30" s="202"/>
-      <c r="U30" s="202"/>
-      <c r="V30" s="202"/>
-      <c r="W30" s="203"/>
+      <c r="C30" s="208"/>
+      <c r="D30" s="208"/>
+      <c r="E30" s="208"/>
+      <c r="F30" s="208"/>
+      <c r="G30" s="208"/>
+      <c r="H30" s="208"/>
+      <c r="I30" s="208"/>
+      <c r="J30" s="208"/>
+      <c r="K30" s="208"/>
+      <c r="L30" s="208"/>
+      <c r="M30" s="208"/>
+      <c r="N30" s="208"/>
+      <c r="O30" s="208"/>
+      <c r="P30" s="208"/>
+      <c r="Q30" s="208"/>
+      <c r="R30" s="208"/>
+      <c r="S30" s="208"/>
+      <c r="T30" s="208"/>
+      <c r="U30" s="208"/>
+      <c r="V30" s="208"/>
+      <c r="W30" s="209"/>
       <c r="X30" s="19"/>
       <c r="Y30" s="15"/>
     </row>
-    <row r="31" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="16"/>
-      <c r="B31" s="195"/>
-      <c r="C31" s="196"/>
-      <c r="D31" s="196"/>
-      <c r="E31" s="196"/>
-      <c r="F31" s="196"/>
-      <c r="G31" s="196"/>
-      <c r="H31" s="196"/>
-      <c r="I31" s="196"/>
-      <c r="J31" s="196"/>
-      <c r="K31" s="196"/>
-      <c r="L31" s="196"/>
-      <c r="M31" s="196"/>
-      <c r="N31" s="196"/>
-      <c r="O31" s="196"/>
-      <c r="P31" s="196"/>
-      <c r="Q31" s="196"/>
-      <c r="R31" s="196"/>
-      <c r="S31" s="196"/>
-      <c r="T31" s="196"/>
-      <c r="U31" s="196"/>
-      <c r="V31" s="196"/>
-      <c r="W31" s="197"/>
+      <c r="B31" s="219"/>
+      <c r="C31" s="220"/>
+      <c r="D31" s="220"/>
+      <c r="E31" s="220"/>
+      <c r="F31" s="220"/>
+      <c r="G31" s="220"/>
+      <c r="H31" s="220"/>
+      <c r="I31" s="220"/>
+      <c r="J31" s="220"/>
+      <c r="K31" s="220"/>
+      <c r="L31" s="220"/>
+      <c r="M31" s="220"/>
+      <c r="N31" s="220"/>
+      <c r="O31" s="220"/>
+      <c r="P31" s="220"/>
+      <c r="Q31" s="220"/>
+      <c r="R31" s="220"/>
+      <c r="S31" s="220"/>
+      <c r="T31" s="220"/>
+      <c r="U31" s="220"/>
+      <c r="V31" s="220"/>
+      <c r="W31" s="221"/>
       <c r="X31" s="24"/>
       <c r="Y31" s="15"/>
     </row>
-    <row r="32" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="16"/>
-      <c r="B32" s="198"/>
-      <c r="C32" s="199"/>
-      <c r="D32" s="199"/>
-      <c r="E32" s="199"/>
-      <c r="F32" s="199"/>
-      <c r="G32" s="199"/>
-      <c r="H32" s="199"/>
-      <c r="I32" s="199"/>
-      <c r="J32" s="199"/>
-      <c r="K32" s="199"/>
-      <c r="L32" s="199"/>
-      <c r="M32" s="199"/>
-      <c r="N32" s="199"/>
-      <c r="O32" s="199"/>
-      <c r="P32" s="199"/>
-      <c r="Q32" s="199"/>
-      <c r="R32" s="199"/>
-      <c r="S32" s="199"/>
-      <c r="T32" s="199"/>
-      <c r="U32" s="199"/>
-      <c r="V32" s="199"/>
-      <c r="W32" s="200"/>
+      <c r="B32" s="222"/>
+      <c r="C32" s="223"/>
+      <c r="D32" s="223"/>
+      <c r="E32" s="223"/>
+      <c r="F32" s="223"/>
+      <c r="G32" s="223"/>
+      <c r="H32" s="223"/>
+      <c r="I32" s="223"/>
+      <c r="J32" s="223"/>
+      <c r="K32" s="223"/>
+      <c r="L32" s="223"/>
+      <c r="M32" s="223"/>
+      <c r="N32" s="223"/>
+      <c r="O32" s="223"/>
+      <c r="P32" s="223"/>
+      <c r="Q32" s="223"/>
+      <c r="R32" s="223"/>
+      <c r="S32" s="223"/>
+      <c r="T32" s="223"/>
+      <c r="U32" s="223"/>
+      <c r="V32" s="223"/>
+      <c r="W32" s="224"/>
       <c r="X32" s="24"/>
       <c r="Y32" s="15"/>
     </row>
-    <row r="33" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="16"/>
       <c r="B33" s="17"/>
       <c r="C33" s="17"/>
@@ -4002,7 +4002,7 @@
       <c r="X33" s="18"/>
       <c r="Y33" s="15"/>
     </row>
-    <row r="34" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="16"/>
       <c r="B34" s="17"/>
       <c r="C34" s="17"/>
@@ -4029,7 +4029,7 @@
       <c r="X34" s="18"/>
       <c r="Y34" s="15"/>
     </row>
-    <row r="35" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="16"/>
       <c r="B35" s="17"/>
       <c r="C35" s="17"/>
@@ -4056,36 +4056,36 @@
       <c r="X35" s="18"/>
       <c r="Y35" s="15"/>
     </row>
-    <row r="36" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="16"/>
-      <c r="B36" s="201" t="s">
+      <c r="B36" s="207" t="s">
         <v>10</v>
       </c>
-      <c r="C36" s="202"/>
-      <c r="D36" s="202"/>
-      <c r="E36" s="202"/>
-      <c r="F36" s="202"/>
-      <c r="G36" s="202"/>
-      <c r="H36" s="202"/>
-      <c r="I36" s="202"/>
-      <c r="J36" s="202"/>
-      <c r="K36" s="202"/>
-      <c r="L36" s="202"/>
-      <c r="M36" s="202"/>
-      <c r="N36" s="202"/>
-      <c r="O36" s="202"/>
-      <c r="P36" s="202"/>
-      <c r="Q36" s="202"/>
-      <c r="R36" s="202"/>
-      <c r="S36" s="202"/>
-      <c r="T36" s="202"/>
-      <c r="U36" s="202"/>
-      <c r="V36" s="202"/>
-      <c r="W36" s="203"/>
+      <c r="C36" s="208"/>
+      <c r="D36" s="208"/>
+      <c r="E36" s="208"/>
+      <c r="F36" s="208"/>
+      <c r="G36" s="208"/>
+      <c r="H36" s="208"/>
+      <c r="I36" s="208"/>
+      <c r="J36" s="208"/>
+      <c r="K36" s="208"/>
+      <c r="L36" s="208"/>
+      <c r="M36" s="208"/>
+      <c r="N36" s="208"/>
+      <c r="O36" s="208"/>
+      <c r="P36" s="208"/>
+      <c r="Q36" s="208"/>
+      <c r="R36" s="208"/>
+      <c r="S36" s="208"/>
+      <c r="T36" s="208"/>
+      <c r="U36" s="208"/>
+      <c r="V36" s="208"/>
+      <c r="W36" s="209"/>
       <c r="X36" s="19"/>
       <c r="Y36" s="15"/>
     </row>
-    <row r="37" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="16"/>
       <c r="B37" s="25"/>
       <c r="C37" s="26"/>
@@ -4112,36 +4112,36 @@
       <c r="X37" s="28"/>
       <c r="Y37" s="29"/>
     </row>
-    <row r="38" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="16"/>
       <c r="B38" s="30"/>
       <c r="C38" s="31"/>
-      <c r="D38" s="204" t="s">
+      <c r="D38" s="195" t="s">
         <v>11</v>
       </c>
-      <c r="E38" s="205"/>
-      <c r="F38" s="205"/>
-      <c r="G38" s="205"/>
-      <c r="H38" s="205"/>
-      <c r="I38" s="205"/>
-      <c r="J38" s="205"/>
-      <c r="K38" s="205"/>
-      <c r="L38" s="206"/>
-      <c r="M38" s="207"/>
-      <c r="N38" s="208"/>
-      <c r="O38" s="208"/>
-      <c r="P38" s="208"/>
-      <c r="Q38" s="208"/>
-      <c r="R38" s="208"/>
-      <c r="S38" s="208"/>
-      <c r="T38" s="208"/>
-      <c r="U38" s="209"/>
+      <c r="E38" s="196"/>
+      <c r="F38" s="196"/>
+      <c r="G38" s="196"/>
+      <c r="H38" s="196"/>
+      <c r="I38" s="196"/>
+      <c r="J38" s="196"/>
+      <c r="K38" s="196"/>
+      <c r="L38" s="197"/>
+      <c r="M38" s="210"/>
+      <c r="N38" s="211"/>
+      <c r="O38" s="211"/>
+      <c r="P38" s="211"/>
+      <c r="Q38" s="211"/>
+      <c r="R38" s="211"/>
+      <c r="S38" s="211"/>
+      <c r="T38" s="211"/>
+      <c r="U38" s="212"/>
       <c r="V38" s="31"/>
       <c r="W38" s="32"/>
       <c r="X38" s="18"/>
       <c r="Y38" s="29"/>
     </row>
-    <row r="39" spans="1:25" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:25" ht="5.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="16"/>
       <c r="B39" s="30"/>
       <c r="C39" s="31"/>
@@ -4168,36 +4168,36 @@
       <c r="X39" s="18"/>
       <c r="Y39" s="29"/>
     </row>
-    <row r="40" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="16"/>
       <c r="B40" s="30"/>
       <c r="C40" s="31"/>
-      <c r="D40" s="204" t="s">
+      <c r="D40" s="195" t="s">
         <v>12</v>
       </c>
-      <c r="E40" s="205"/>
-      <c r="F40" s="205"/>
-      <c r="G40" s="205"/>
-      <c r="H40" s="205"/>
-      <c r="I40" s="205"/>
-      <c r="J40" s="205"/>
-      <c r="K40" s="205"/>
-      <c r="L40" s="206"/>
-      <c r="M40" s="207"/>
-      <c r="N40" s="208"/>
-      <c r="O40" s="208"/>
-      <c r="P40" s="208"/>
-      <c r="Q40" s="208"/>
-      <c r="R40" s="208"/>
-      <c r="S40" s="208"/>
-      <c r="T40" s="208"/>
-      <c r="U40" s="209"/>
+      <c r="E40" s="196"/>
+      <c r="F40" s="196"/>
+      <c r="G40" s="196"/>
+      <c r="H40" s="196"/>
+      <c r="I40" s="196"/>
+      <c r="J40" s="196"/>
+      <c r="K40" s="196"/>
+      <c r="L40" s="197"/>
+      <c r="M40" s="210"/>
+      <c r="N40" s="211"/>
+      <c r="O40" s="211"/>
+      <c r="P40" s="211"/>
+      <c r="Q40" s="211"/>
+      <c r="R40" s="211"/>
+      <c r="S40" s="211"/>
+      <c r="T40" s="211"/>
+      <c r="U40" s="212"/>
       <c r="V40" s="31"/>
       <c r="W40" s="32"/>
       <c r="X40" s="18"/>
       <c r="Y40" s="29"/>
     </row>
-    <row r="41" spans="1:25" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:25" ht="5.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="16"/>
       <c r="B41" s="30"/>
       <c r="C41" s="31"/>
@@ -4224,36 +4224,36 @@
       <c r="X41" s="18"/>
       <c r="Y41" s="29"/>
     </row>
-    <row r="42" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="16"/>
       <c r="B42" s="30"/>
       <c r="C42" s="31"/>
-      <c r="D42" s="204" t="s">
+      <c r="D42" s="195" t="s">
         <v>13</v>
       </c>
-      <c r="E42" s="205"/>
-      <c r="F42" s="205"/>
-      <c r="G42" s="205"/>
-      <c r="H42" s="205"/>
-      <c r="I42" s="205"/>
-      <c r="J42" s="205"/>
-      <c r="K42" s="205"/>
-      <c r="L42" s="206"/>
-      <c r="M42" s="222"/>
-      <c r="N42" s="223"/>
-      <c r="O42" s="223"/>
-      <c r="P42" s="223"/>
-      <c r="Q42" s="223"/>
-      <c r="R42" s="223"/>
-      <c r="S42" s="223"/>
-      <c r="T42" s="223"/>
-      <c r="U42" s="224"/>
+      <c r="E42" s="196"/>
+      <c r="F42" s="196"/>
+      <c r="G42" s="196"/>
+      <c r="H42" s="196"/>
+      <c r="I42" s="196"/>
+      <c r="J42" s="196"/>
+      <c r="K42" s="196"/>
+      <c r="L42" s="197"/>
+      <c r="M42" s="198"/>
+      <c r="N42" s="199"/>
+      <c r="O42" s="199"/>
+      <c r="P42" s="199"/>
+      <c r="Q42" s="199"/>
+      <c r="R42" s="199"/>
+      <c r="S42" s="199"/>
+      <c r="T42" s="199"/>
+      <c r="U42" s="200"/>
       <c r="V42" s="31"/>
       <c r="W42" s="32"/>
       <c r="X42" s="18"/>
       <c r="Y42" s="29"/>
     </row>
-    <row r="43" spans="1:25" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:25" ht="5.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="16"/>
       <c r="B43" s="30"/>
       <c r="C43" s="31"/>
@@ -4280,39 +4280,39 @@
       <c r="X43" s="18"/>
       <c r="Y43" s="29"/>
     </row>
-    <row r="44" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="16"/>
       <c r="B44" s="30"/>
       <c r="C44" s="31"/>
-      <c r="D44" s="204" t="s">
+      <c r="D44" s="195" t="s">
         <v>14</v>
       </c>
-      <c r="E44" s="205"/>
-      <c r="F44" s="205"/>
-      <c r="G44" s="205"/>
-      <c r="H44" s="205"/>
-      <c r="I44" s="205"/>
-      <c r="J44" s="205"/>
-      <c r="K44" s="205"/>
-      <c r="L44" s="206"/>
-      <c r="M44" s="222" t="e">
+      <c r="E44" s="196"/>
+      <c r="F44" s="196"/>
+      <c r="G44" s="196"/>
+      <c r="H44" s="196"/>
+      <c r="I44" s="196"/>
+      <c r="J44" s="196"/>
+      <c r="K44" s="196"/>
+      <c r="L44" s="197"/>
+      <c r="M44" s="198" t="e">
         <f>M42/M38</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N44" s="223"/>
-      <c r="O44" s="223"/>
-      <c r="P44" s="223"/>
-      <c r="Q44" s="223"/>
-      <c r="R44" s="223"/>
-      <c r="S44" s="223"/>
-      <c r="T44" s="223"/>
-      <c r="U44" s="224"/>
+      <c r="N44" s="199"/>
+      <c r="O44" s="199"/>
+      <c r="P44" s="199"/>
+      <c r="Q44" s="199"/>
+      <c r="R44" s="199"/>
+      <c r="S44" s="199"/>
+      <c r="T44" s="199"/>
+      <c r="U44" s="200"/>
       <c r="V44" s="31"/>
       <c r="W44" s="32"/>
       <c r="X44" s="18"/>
       <c r="Y44" s="29"/>
     </row>
-    <row r="45" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="16"/>
       <c r="B45" s="36"/>
       <c r="C45" s="37"/>
@@ -4339,7 +4339,7 @@
       <c r="X45" s="18"/>
       <c r="Y45" s="29"/>
     </row>
-    <row r="46" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="16"/>
       <c r="B46" s="17"/>
       <c r="C46" s="17"/>
@@ -4366,7 +4366,7 @@
       <c r="X46" s="18"/>
       <c r="Y46" s="15"/>
     </row>
-    <row r="47" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="16"/>
       <c r="B47" s="17"/>
       <c r="C47" s="17"/>
@@ -4393,7 +4393,7 @@
       <c r="X47" s="15"/>
       <c r="Y47" s="15"/>
     </row>
-    <row r="48" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="16"/>
       <c r="B48" s="17"/>
       <c r="C48" s="17"/>
@@ -4420,7 +4420,7 @@
       <c r="X48" s="15"/>
       <c r="Y48" s="15"/>
     </row>
-    <row r="49" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="16"/>
       <c r="B49" s="17"/>
       <c r="C49" s="17"/>
@@ -4447,7 +4447,7 @@
       <c r="X49" s="15"/>
       <c r="Y49" s="15"/>
     </row>
-    <row r="50" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="39"/>
       <c r="B50" s="40"/>
       <c r="C50" s="40"/>
@@ -4474,19 +4474,19 @@
       <c r="X50" s="41"/>
       <c r="Y50" s="41"/>
     </row>
-    <row r="51" spans="1:25" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:25" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="13"/>
       <c r="Y51" s="43"/>
     </row>
-    <row r="52" spans="1:25" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:25" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="13"/>
       <c r="Y52" s="43"/>
     </row>
-    <row r="53" spans="1:25" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:25" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="13"/>
       <c r="Y53" s="43"/>
     </row>
-    <row r="54" spans="1:25" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:25" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="44"/>
       <c r="B54" s="45"/>
       <c r="C54" s="45"/>
@@ -4518,6 +4518,10 @@
     <protectedRange password="CB1D" sqref="C17:D18" name="BatchData" securityDescriptor="O:WDG:WDD:(D;;CC;;;S-1-5-21-343818398-1326574676-839522115-1142)(D;;CC;;;S-1-5-21-343818398-1326574676-839522115-1141)(A;;CC;;;S-1-5-21-343818398-1326574676-839522115-1136)(A;;CC;;;S-1-5-21-343818398-1326574676-839522115-1137)"/>
   </protectedRanges>
   <mergeCells count="20">
+    <mergeCell ref="B11:W12"/>
+    <mergeCell ref="B14:W14"/>
+    <mergeCell ref="B15:W16"/>
+    <mergeCell ref="B18:W18"/>
     <mergeCell ref="D44:L44"/>
     <mergeCell ref="M44:U44"/>
     <mergeCell ref="B19:W20"/>
@@ -4534,10 +4538,6 @@
     <mergeCell ref="B36:W36"/>
     <mergeCell ref="D38:L38"/>
     <mergeCell ref="M38:U38"/>
-    <mergeCell ref="B11:W12"/>
-    <mergeCell ref="B14:W14"/>
-    <mergeCell ref="B15:W16"/>
-    <mergeCell ref="B18:W18"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4560,11 +4560,11 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="6" width="3.7109375" style="3" customWidth="1"/>
-    <col min="7" max="9" width="3.7109375" style="6" customWidth="1"/>
-    <col min="10" max="22" width="3.7109375" style="3" customWidth="1"/>
-    <col min="23" max="24" width="3.7109375" style="1" customWidth="1"/>
-    <col min="25" max="16384" width="3.7109375" style="3" hidden="1"/>
+    <col min="1" max="6" width="3.7265625" style="3" customWidth="1"/>
+    <col min="7" max="9" width="3.7265625" style="6" customWidth="1"/>
+    <col min="10" max="22" width="3.7265625" style="3" customWidth="1"/>
+    <col min="23" max="24" width="3.7265625" style="1" customWidth="1"/>
+    <col min="25" max="16384" width="3.7265625" style="3" hidden="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4641,33 +4641,33 @@
       <c r="Y9" s="2"/>
     </row>
     <row r="10" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D10" s="231" t="s">
+      <c r="D10" s="237" t="s">
         <v>0</v>
       </c>
-      <c r="E10" s="232"/>
-      <c r="F10" s="232"/>
-      <c r="G10" s="232"/>
-      <c r="H10" s="232"/>
-      <c r="I10" s="232"/>
-      <c r="J10" s="232"/>
-      <c r="K10" s="232"/>
-      <c r="L10" s="233"/>
-      <c r="M10" s="234" t="s">
+      <c r="E10" s="238"/>
+      <c r="F10" s="238"/>
+      <c r="G10" s="238"/>
+      <c r="H10" s="238"/>
+      <c r="I10" s="238"/>
+      <c r="J10" s="238"/>
+      <c r="K10" s="238"/>
+      <c r="L10" s="239"/>
+      <c r="M10" s="246" t="s">
         <v>9</v>
       </c>
-      <c r="N10" s="235"/>
-      <c r="O10" s="235"/>
-      <c r="P10" s="235"/>
-      <c r="Q10" s="235"/>
-      <c r="R10" s="235"/>
-      <c r="S10" s="235"/>
-      <c r="T10" s="235"/>
-      <c r="U10" s="236"/>
+      <c r="N10" s="247"/>
+      <c r="O10" s="247"/>
+      <c r="P10" s="247"/>
+      <c r="Q10" s="247"/>
+      <c r="R10" s="247"/>
+      <c r="S10" s="247"/>
+      <c r="T10" s="247"/>
+      <c r="U10" s="248"/>
       <c r="W10" s="3"/>
       <c r="X10" s="3"/>
       <c r="Y10" s="2"/>
     </row>
-    <row r="11" spans="1:25" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" ht="5.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D11" s="80"/>
       <c r="E11" s="80"/>
       <c r="F11" s="80"/>
@@ -4681,31 +4681,31 @@
       <c r="X11" s="3"/>
     </row>
     <row r="12" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D12" s="231" t="s">
+      <c r="D12" s="237" t="s">
         <v>1</v>
       </c>
-      <c r="E12" s="232"/>
-      <c r="F12" s="232"/>
-      <c r="G12" s="232"/>
-      <c r="H12" s="232"/>
-      <c r="I12" s="232"/>
-      <c r="J12" s="232"/>
-      <c r="K12" s="232"/>
-      <c r="L12" s="233"/>
-      <c r="M12" s="234"/>
-      <c r="N12" s="235"/>
-      <c r="O12" s="235"/>
-      <c r="P12" s="235"/>
-      <c r="Q12" s="235"/>
-      <c r="R12" s="235"/>
-      <c r="S12" s="235"/>
-      <c r="T12" s="235"/>
-      <c r="U12" s="236"/>
+      <c r="E12" s="238"/>
+      <c r="F12" s="238"/>
+      <c r="G12" s="238"/>
+      <c r="H12" s="238"/>
+      <c r="I12" s="238"/>
+      <c r="J12" s="238"/>
+      <c r="K12" s="238"/>
+      <c r="L12" s="239"/>
+      <c r="M12" s="246"/>
+      <c r="N12" s="247"/>
+      <c r="O12" s="247"/>
+      <c r="P12" s="247"/>
+      <c r="Q12" s="247"/>
+      <c r="R12" s="247"/>
+      <c r="S12" s="247"/>
+      <c r="T12" s="247"/>
+      <c r="U12" s="248"/>
       <c r="W12" s="3"/>
       <c r="X12" s="3"/>
       <c r="Y12" s="2"/>
     </row>
-    <row r="13" spans="1:25" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" ht="5.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D13" s="80"/>
       <c r="E13" s="80"/>
       <c r="F13" s="80"/>
@@ -4719,31 +4719,31 @@
       <c r="X13" s="3"/>
     </row>
     <row r="14" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D14" s="231" t="s">
+      <c r="D14" s="237" t="s">
         <v>2</v>
       </c>
-      <c r="E14" s="232"/>
-      <c r="F14" s="232"/>
-      <c r="G14" s="232"/>
-      <c r="H14" s="232"/>
-      <c r="I14" s="232"/>
-      <c r="J14" s="232"/>
-      <c r="K14" s="232"/>
-      <c r="L14" s="233"/>
-      <c r="M14" s="234"/>
-      <c r="N14" s="235"/>
-      <c r="O14" s="235"/>
-      <c r="P14" s="235"/>
-      <c r="Q14" s="235"/>
-      <c r="R14" s="235"/>
-      <c r="S14" s="235"/>
-      <c r="T14" s="235"/>
-      <c r="U14" s="236"/>
+      <c r="E14" s="238"/>
+      <c r="F14" s="238"/>
+      <c r="G14" s="238"/>
+      <c r="H14" s="238"/>
+      <c r="I14" s="238"/>
+      <c r="J14" s="238"/>
+      <c r="K14" s="238"/>
+      <c r="L14" s="239"/>
+      <c r="M14" s="246"/>
+      <c r="N14" s="247"/>
+      <c r="O14" s="247"/>
+      <c r="P14" s="247"/>
+      <c r="Q14" s="247"/>
+      <c r="R14" s="247"/>
+      <c r="S14" s="247"/>
+      <c r="T14" s="247"/>
+      <c r="U14" s="248"/>
       <c r="W14" s="3"/>
       <c r="X14" s="3"/>
       <c r="Y14" s="2"/>
     </row>
-    <row r="15" spans="1:25" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" ht="5.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D15" s="80"/>
       <c r="E15" s="80"/>
       <c r="F15" s="80"/>
@@ -4759,28 +4759,28 @@
     <row r="16" spans="1:25" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="81"/>
       <c r="B16" s="81"/>
-      <c r="D16" s="231" t="s">
+      <c r="D16" s="237" t="s">
         <v>3</v>
       </c>
-      <c r="E16" s="232"/>
-      <c r="F16" s="232"/>
-      <c r="G16" s="232"/>
-      <c r="H16" s="232"/>
-      <c r="I16" s="232"/>
-      <c r="J16" s="232"/>
-      <c r="K16" s="232"/>
-      <c r="L16" s="233"/>
-      <c r="M16" s="234"/>
-      <c r="N16" s="235"/>
-      <c r="O16" s="235"/>
-      <c r="P16" s="235"/>
-      <c r="Q16" s="235"/>
-      <c r="R16" s="235"/>
-      <c r="S16" s="235"/>
-      <c r="T16" s="235"/>
-      <c r="U16" s="236"/>
-    </row>
-    <row r="17" spans="1:24" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E16" s="238"/>
+      <c r="F16" s="238"/>
+      <c r="G16" s="238"/>
+      <c r="H16" s="238"/>
+      <c r="I16" s="238"/>
+      <c r="J16" s="238"/>
+      <c r="K16" s="238"/>
+      <c r="L16" s="239"/>
+      <c r="M16" s="246"/>
+      <c r="N16" s="247"/>
+      <c r="O16" s="247"/>
+      <c r="P16" s="247"/>
+      <c r="Q16" s="247"/>
+      <c r="R16" s="247"/>
+      <c r="S16" s="247"/>
+      <c r="T16" s="247"/>
+      <c r="U16" s="248"/>
+    </row>
+    <row r="17" spans="1:24" ht="5.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D17" s="80"/>
       <c r="E17" s="80"/>
       <c r="F17" s="80"/>
@@ -4796,26 +4796,26 @@
     <row r="18" spans="1:24" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="82"/>
       <c r="B18" s="82"/>
-      <c r="D18" s="231" t="s">
+      <c r="D18" s="237" t="s">
         <v>4</v>
       </c>
-      <c r="E18" s="232"/>
-      <c r="F18" s="232"/>
-      <c r="G18" s="232"/>
-      <c r="H18" s="232"/>
-      <c r="I18" s="232"/>
-      <c r="J18" s="232"/>
-      <c r="K18" s="232"/>
-      <c r="L18" s="233"/>
-      <c r="M18" s="243"/>
-      <c r="N18" s="244"/>
-      <c r="O18" s="244"/>
-      <c r="P18" s="244"/>
-      <c r="Q18" s="244"/>
-      <c r="R18" s="244"/>
-      <c r="S18" s="244"/>
-      <c r="T18" s="244"/>
-      <c r="U18" s="245"/>
+      <c r="E18" s="238"/>
+      <c r="F18" s="238"/>
+      <c r="G18" s="238"/>
+      <c r="H18" s="238"/>
+      <c r="I18" s="238"/>
+      <c r="J18" s="238"/>
+      <c r="K18" s="238"/>
+      <c r="L18" s="239"/>
+      <c r="M18" s="240"/>
+      <c r="N18" s="241"/>
+      <c r="O18" s="241"/>
+      <c r="P18" s="241"/>
+      <c r="Q18" s="241"/>
+      <c r="R18" s="241"/>
+      <c r="S18" s="241"/>
+      <c r="T18" s="241"/>
+      <c r="U18" s="242"/>
     </row>
     <row r="19" spans="1:24" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G19" s="83"/>
@@ -4823,60 +4823,60 @@
       <c r="I19" s="83"/>
     </row>
     <row r="20" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C20" s="246" t="s">
+      <c r="C20" s="243" t="s">
         <v>5</v>
       </c>
-      <c r="D20" s="246"/>
-      <c r="E20" s="247" t="s">
-        <v>224</v>
-      </c>
-      <c r="F20" s="247"/>
-      <c r="G20" s="247"/>
-      <c r="H20" s="247"/>
-      <c r="I20" s="247"/>
-      <c r="J20" s="247"/>
-      <c r="K20" s="246" t="s">
+      <c r="D20" s="243"/>
+      <c r="E20" s="244" t="s">
+        <v>221</v>
+      </c>
+      <c r="F20" s="244"/>
+      <c r="G20" s="244"/>
+      <c r="H20" s="244"/>
+      <c r="I20" s="244"/>
+      <c r="J20" s="244"/>
+      <c r="K20" s="243" t="s">
         <v>6</v>
       </c>
-      <c r="L20" s="246"/>
-      <c r="M20" s="246"/>
-      <c r="N20" s="246"/>
-      <c r="O20" s="246"/>
-      <c r="P20" s="246"/>
-      <c r="Q20" s="248" t="s">
+      <c r="L20" s="243"/>
+      <c r="M20" s="243"/>
+      <c r="N20" s="243"/>
+      <c r="O20" s="243"/>
+      <c r="P20" s="243"/>
+      <c r="Q20" s="245" t="s">
         <v>7</v>
       </c>
-      <c r="R20" s="248"/>
-      <c r="S20" s="248"/>
-      <c r="T20" s="248"/>
-      <c r="U20" s="248"/>
-      <c r="V20" s="248"/>
+      <c r="R20" s="245"/>
+      <c r="S20" s="245"/>
+      <c r="T20" s="245"/>
+      <c r="U20" s="245"/>
+      <c r="V20" s="245"/>
       <c r="W20" s="3"/>
       <c r="X20" s="3"/>
     </row>
     <row r="21" spans="1:24" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C21" s="237">
+      <c r="C21" s="231">
         <v>1</v>
       </c>
-      <c r="D21" s="237"/>
-      <c r="E21" s="238"/>
-      <c r="F21" s="239"/>
-      <c r="G21" s="239"/>
-      <c r="H21" s="239"/>
-      <c r="I21" s="239"/>
-      <c r="J21" s="240"/>
-      <c r="K21" s="241"/>
-      <c r="L21" s="242"/>
-      <c r="M21" s="242"/>
-      <c r="N21" s="242"/>
-      <c r="O21" s="242"/>
-      <c r="P21" s="242"/>
-      <c r="Q21" s="241"/>
-      <c r="R21" s="242"/>
-      <c r="S21" s="242"/>
-      <c r="T21" s="242"/>
-      <c r="U21" s="242"/>
-      <c r="V21" s="242"/>
+      <c r="D21" s="231"/>
+      <c r="E21" s="232"/>
+      <c r="F21" s="233"/>
+      <c r="G21" s="233"/>
+      <c r="H21" s="233"/>
+      <c r="I21" s="233"/>
+      <c r="J21" s="234"/>
+      <c r="K21" s="235"/>
+      <c r="L21" s="236"/>
+      <c r="M21" s="236"/>
+      <c r="N21" s="236"/>
+      <c r="O21" s="236"/>
+      <c r="P21" s="236"/>
+      <c r="Q21" s="235"/>
+      <c r="R21" s="236"/>
+      <c r="S21" s="236"/>
+      <c r="T21" s="236"/>
+      <c r="U21" s="236"/>
+      <c r="V21" s="236"/>
     </row>
     <row r="22" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="W22" s="3"/>
@@ -5168,6 +5168,14 @@
     <protectedRange password="CB1D" sqref="C9:D9 D10:E18" name="BatchData" securityDescriptor="O:WDG:WDD:(D;;CC;;;S-1-5-21-343818398-1326574676-839522115-1142)(D;;CC;;;S-1-5-21-343818398-1326574676-839522115-1141)(A;;CC;;;S-1-5-21-343818398-1326574676-839522115-1136)(A;;CC;;;S-1-5-21-343818398-1326574676-839522115-1137)"/>
   </protectedRanges>
   <mergeCells count="18">
+    <mergeCell ref="D16:L16"/>
+    <mergeCell ref="M16:U16"/>
+    <mergeCell ref="D10:L10"/>
+    <mergeCell ref="M10:U10"/>
+    <mergeCell ref="D12:L12"/>
+    <mergeCell ref="M12:U12"/>
+    <mergeCell ref="D14:L14"/>
+    <mergeCell ref="M14:U14"/>
     <mergeCell ref="C21:D21"/>
     <mergeCell ref="E21:J21"/>
     <mergeCell ref="K21:P21"/>
@@ -5178,14 +5186,6 @@
     <mergeCell ref="E20:J20"/>
     <mergeCell ref="K20:P20"/>
     <mergeCell ref="Q20:V20"/>
-    <mergeCell ref="D16:L16"/>
-    <mergeCell ref="M16:U16"/>
-    <mergeCell ref="D10:L10"/>
-    <mergeCell ref="M10:U10"/>
-    <mergeCell ref="D12:L12"/>
-    <mergeCell ref="M12:U12"/>
-    <mergeCell ref="D14:L14"/>
-    <mergeCell ref="M14:U14"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -5202,721 +5202,721 @@
   </sheetPr>
   <dimension ref="A1:HN494"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="HG1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="GQ1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="HK3" sqref="HK3"/>
+      <selection pane="bottomLeft" activeCell="HG4" sqref="HG4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" style="47" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" style="47" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="83.28515625" style="47" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" style="47" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" style="47" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.140625" style="47" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.453125" style="47" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7265625" style="47" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="83.26953125" style="47" customWidth="1"/>
+    <col min="4" max="4" width="12.26953125" style="47" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.453125" style="47" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.1796875" style="47" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15" style="47" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.5703125" style="47" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="34.140625" style="47" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="28.42578125" style="47" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.28515625" style="47" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.54296875" style="47" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="34.1796875" style="47" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="28.453125" style="47" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.26953125" style="47" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="14" style="47" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.28515625" style="47" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.26953125" style="47" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="18" style="47" customWidth="1"/>
-    <col min="15" max="15" width="12.7109375" style="47" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19.140625" style="101" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17.7109375" style="87" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.5703125" style="87" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="17.140625" style="47" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18.7109375" style="47" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="11.42578125" style="47" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="12.85546875" style="47" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="16.7109375" style="47" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="15.42578125" style="47" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="16.42578125" style="47" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="18.42578125" style="87" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="8.7109375" style="47" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="38.42578125" style="47" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="25.5703125" style="47" bestFit="1" customWidth="1"/>
-    <col min="31" max="32" width="15.85546875" style="47" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="16.42578125" style="47" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="15.28515625" style="47" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="15.5703125" style="47" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="13.85546875" style="47" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="28.5703125" style="47" customWidth="1"/>
-    <col min="38" max="38" width="13.7109375" style="47" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="11.28515625" style="47" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="12.7109375" style="47" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="15.28515625" style="47" customWidth="1"/>
-    <col min="42" max="42" width="15.28515625" style="47" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="16.28515625" style="47" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="18.28515625" style="87" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="15.140625" style="47" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="15.42578125" style="47" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="13.7109375" style="47" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="20.5703125" style="103" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="14.85546875" style="47" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="35.7109375" style="47" customWidth="1"/>
+    <col min="15" max="15" width="12.7265625" style="47" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.1796875" style="101" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.7265625" style="87" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.54296875" style="87" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="17.1796875" style="47" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18.7265625" style="47" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="11.453125" style="47" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.81640625" style="47" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="16.7265625" style="47" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="15.453125" style="47" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="16.453125" style="47" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="18.453125" style="87" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="8.7265625" style="47" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="38.453125" style="47" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="25.54296875" style="47" bestFit="1" customWidth="1"/>
+    <col min="31" max="32" width="15.81640625" style="47" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="16.453125" style="47" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="15.26953125" style="47" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="15.54296875" style="47" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="13.81640625" style="47" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="28.54296875" style="47" customWidth="1"/>
+    <col min="38" max="38" width="13.7265625" style="47" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="11.26953125" style="47" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="12.7265625" style="47" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="15.26953125" style="47" customWidth="1"/>
+    <col min="42" max="42" width="15.26953125" style="47" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="16.26953125" style="47" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="18.26953125" style="87" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="15.1796875" style="47" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="15.453125" style="47" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="13.7265625" style="47" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="20.54296875" style="103" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="14.81640625" style="47" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="35.7265625" style="47" customWidth="1"/>
     <col min="51" max="51" width="16" style="47" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="16.5703125" style="47" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="19.28515625" style="47" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="13.140625" style="47" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="14.5703125" style="47" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="12.28515625" style="103" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="12.5703125" style="103" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="12.140625" style="47" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="16.54296875" style="47" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="19.26953125" style="47" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="13.1796875" style="47" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="14.54296875" style="47" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="12.26953125" style="103" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="12.54296875" style="103" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="12.1796875" style="47" bestFit="1" customWidth="1"/>
     <col min="59" max="59" width="12" style="47" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="15.140625" style="47" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="14.42578125" style="47" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="14.85546875" style="47" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="12.5703125" style="103" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="12.85546875" style="103" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="12.42578125" style="47" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="12.28515625" style="47" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="12.140625" style="47" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="13.5703125" style="47" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="17.42578125" style="47" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="16.140625" style="47" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="17.140625" style="47" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="19.140625" style="47" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="11.85546875" style="47" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="15.1796875" style="47" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="14.453125" style="47" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="14.81640625" style="47" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="12.54296875" style="103" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="12.81640625" style="103" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="12.453125" style="47" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="12.26953125" style="47" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="12.1796875" style="47" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="13.54296875" style="47" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="17.453125" style="47" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="16.1796875" style="47" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="17.1796875" style="47" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="19.1796875" style="47" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="11.81640625" style="47" bestFit="1" customWidth="1"/>
     <col min="74" max="74" width="16" style="47" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="16.28515625" style="47" bestFit="1" customWidth="1"/>
-    <col min="76" max="77" width="14.5703125" style="47" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="16.26953125" style="47" bestFit="1" customWidth="1"/>
+    <col min="76" max="77" width="14.54296875" style="47" bestFit="1" customWidth="1"/>
     <col min="78" max="78" width="18" style="47" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="15.5703125" style="103" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="15.85546875" style="103" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="15.42578125" style="47" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="15.28515625" style="47" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="15.54296875" style="103" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="15.81640625" style="103" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="15.453125" style="47" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="15.26953125" style="47" bestFit="1" customWidth="1"/>
     <col min="83" max="83" width="19" style="47" bestFit="1" customWidth="1"/>
-    <col min="84" max="84" width="16.5703125" style="103" bestFit="1" customWidth="1"/>
-    <col min="85" max="85" width="16.85546875" style="103" bestFit="1" customWidth="1"/>
-    <col min="86" max="86" width="16.42578125" style="47" bestFit="1" customWidth="1"/>
-    <col min="87" max="87" width="16.28515625" style="47" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="16.54296875" style="103" bestFit="1" customWidth="1"/>
+    <col min="85" max="85" width="16.81640625" style="103" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="16.453125" style="47" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="16.26953125" style="47" bestFit="1" customWidth="1"/>
     <col min="88" max="88" width="19" style="47" bestFit="1" customWidth="1"/>
-    <col min="89" max="89" width="16.5703125" style="103" bestFit="1" customWidth="1"/>
-    <col min="90" max="90" width="16.85546875" style="103" bestFit="1" customWidth="1"/>
-    <col min="91" max="91" width="16.42578125" style="47" bestFit="1" customWidth="1"/>
-    <col min="92" max="92" width="16.28515625" style="47" bestFit="1" customWidth="1"/>
+    <col min="89" max="89" width="16.54296875" style="103" bestFit="1" customWidth="1"/>
+    <col min="90" max="90" width="16.81640625" style="103" bestFit="1" customWidth="1"/>
+    <col min="91" max="91" width="16.453125" style="47" bestFit="1" customWidth="1"/>
+    <col min="92" max="92" width="16.26953125" style="47" bestFit="1" customWidth="1"/>
     <col min="93" max="93" width="19" style="47" bestFit="1" customWidth="1"/>
-    <col min="94" max="94" width="16.5703125" style="103" bestFit="1" customWidth="1"/>
-    <col min="95" max="95" width="16.85546875" style="103" bestFit="1" customWidth="1"/>
-    <col min="96" max="96" width="16.42578125" style="47" bestFit="1" customWidth="1"/>
-    <col min="97" max="97" width="16.28515625" style="47" bestFit="1" customWidth="1"/>
+    <col min="94" max="94" width="16.54296875" style="103" bestFit="1" customWidth="1"/>
+    <col min="95" max="95" width="16.81640625" style="103" bestFit="1" customWidth="1"/>
+    <col min="96" max="96" width="16.453125" style="47" bestFit="1" customWidth="1"/>
+    <col min="97" max="97" width="16.26953125" style="47" bestFit="1" customWidth="1"/>
     <col min="98" max="98" width="19" style="47" bestFit="1" customWidth="1"/>
-    <col min="99" max="99" width="16.5703125" style="103" bestFit="1" customWidth="1"/>
-    <col min="100" max="100" width="16.85546875" style="103" bestFit="1" customWidth="1"/>
-    <col min="101" max="101" width="16.42578125" style="47" bestFit="1" customWidth="1"/>
-    <col min="102" max="102" width="16.28515625" style="47" bestFit="1" customWidth="1"/>
+    <col min="99" max="99" width="16.54296875" style="103" bestFit="1" customWidth="1"/>
+    <col min="100" max="100" width="16.81640625" style="103" bestFit="1" customWidth="1"/>
+    <col min="101" max="101" width="16.453125" style="47" bestFit="1" customWidth="1"/>
+    <col min="102" max="102" width="16.26953125" style="47" bestFit="1" customWidth="1"/>
     <col min="103" max="103" width="19" style="47" bestFit="1" customWidth="1"/>
-    <col min="104" max="104" width="16.5703125" style="103" bestFit="1" customWidth="1"/>
-    <col min="105" max="105" width="16.85546875" style="103" bestFit="1" customWidth="1"/>
-    <col min="106" max="106" width="16.42578125" style="47" bestFit="1" customWidth="1"/>
-    <col min="107" max="107" width="16.28515625" style="47" bestFit="1" customWidth="1"/>
-    <col min="108" max="108" width="12.140625" style="47" bestFit="1" customWidth="1"/>
-    <col min="109" max="109" width="13.5703125" style="47" bestFit="1" customWidth="1"/>
-    <col min="110" max="110" width="17.42578125" style="47" bestFit="1" customWidth="1"/>
-    <col min="111" max="111" width="21.42578125" style="47" customWidth="1"/>
-    <col min="112" max="112" width="17.140625" style="47" bestFit="1" customWidth="1"/>
-    <col min="113" max="113" width="19.140625" style="87" bestFit="1" customWidth="1"/>
-    <col min="114" max="114" width="11.85546875" style="47" bestFit="1" customWidth="1"/>
+    <col min="104" max="104" width="16.54296875" style="103" bestFit="1" customWidth="1"/>
+    <col min="105" max="105" width="16.81640625" style="103" bestFit="1" customWidth="1"/>
+    <col min="106" max="106" width="16.453125" style="47" bestFit="1" customWidth="1"/>
+    <col min="107" max="107" width="16.26953125" style="47" bestFit="1" customWidth="1"/>
+    <col min="108" max="108" width="12.1796875" style="47" bestFit="1" customWidth="1"/>
+    <col min="109" max="109" width="13.54296875" style="47" bestFit="1" customWidth="1"/>
+    <col min="110" max="110" width="17.453125" style="47" bestFit="1" customWidth="1"/>
+    <col min="111" max="111" width="21.453125" style="47" customWidth="1"/>
+    <col min="112" max="112" width="17.1796875" style="47" bestFit="1" customWidth="1"/>
+    <col min="113" max="113" width="19.1796875" style="87" bestFit="1" customWidth="1"/>
+    <col min="114" max="114" width="11.81640625" style="47" bestFit="1" customWidth="1"/>
     <col min="115" max="115" width="16" style="47" bestFit="1" customWidth="1"/>
-    <col min="116" max="116" width="16.28515625" style="47" bestFit="1" customWidth="1"/>
-    <col min="117" max="118" width="14.5703125" style="47" bestFit="1" customWidth="1"/>
+    <col min="116" max="116" width="16.26953125" style="47" bestFit="1" customWidth="1"/>
+    <col min="117" max="118" width="14.54296875" style="47" bestFit="1" customWidth="1"/>
     <col min="119" max="119" width="18" style="47" bestFit="1" customWidth="1"/>
-    <col min="120" max="120" width="15.5703125" style="103" bestFit="1" customWidth="1"/>
-    <col min="121" max="121" width="15.85546875" style="103" bestFit="1" customWidth="1"/>
-    <col min="122" max="122" width="15.42578125" style="47" bestFit="1" customWidth="1"/>
-    <col min="123" max="123" width="15.28515625" style="47" bestFit="1" customWidth="1"/>
+    <col min="120" max="120" width="15.54296875" style="103" bestFit="1" customWidth="1"/>
+    <col min="121" max="121" width="15.81640625" style="103" bestFit="1" customWidth="1"/>
+    <col min="122" max="122" width="15.453125" style="47" bestFit="1" customWidth="1"/>
+    <col min="123" max="123" width="15.26953125" style="47" bestFit="1" customWidth="1"/>
     <col min="124" max="124" width="19" style="47" bestFit="1" customWidth="1"/>
-    <col min="125" max="125" width="16.5703125" style="103" bestFit="1" customWidth="1"/>
-    <col min="126" max="126" width="16.85546875" style="103" bestFit="1" customWidth="1"/>
-    <col min="127" max="127" width="16.42578125" style="47" bestFit="1" customWidth="1"/>
-    <col min="128" max="128" width="16.28515625" style="47" bestFit="1" customWidth="1"/>
-    <col min="129" max="129" width="21.42578125" style="47" customWidth="1"/>
-    <col min="130" max="130" width="16.5703125" style="103" bestFit="1" customWidth="1"/>
-    <col min="131" max="131" width="16.85546875" style="103" bestFit="1" customWidth="1"/>
-    <col min="132" max="132" width="16.42578125" style="47" bestFit="1" customWidth="1"/>
-    <col min="133" max="133" width="16.28515625" style="47" bestFit="1" customWidth="1"/>
+    <col min="125" max="125" width="16.54296875" style="103" bestFit="1" customWidth="1"/>
+    <col min="126" max="126" width="16.81640625" style="103" bestFit="1" customWidth="1"/>
+    <col min="127" max="127" width="16.453125" style="47" bestFit="1" customWidth="1"/>
+    <col min="128" max="128" width="16.26953125" style="47" bestFit="1" customWidth="1"/>
+    <col min="129" max="129" width="21.453125" style="47" customWidth="1"/>
+    <col min="130" max="130" width="16.54296875" style="103" bestFit="1" customWidth="1"/>
+    <col min="131" max="131" width="16.81640625" style="103" bestFit="1" customWidth="1"/>
+    <col min="132" max="132" width="16.453125" style="47" bestFit="1" customWidth="1"/>
+    <col min="133" max="133" width="16.26953125" style="47" bestFit="1" customWidth="1"/>
     <col min="134" max="134" width="19" style="47" bestFit="1" customWidth="1"/>
-    <col min="135" max="135" width="16.5703125" style="103" bestFit="1" customWidth="1"/>
-    <col min="136" max="136" width="16.85546875" style="103" bestFit="1" customWidth="1"/>
-    <col min="137" max="137" width="16.42578125" style="47" bestFit="1" customWidth="1"/>
-    <col min="138" max="138" width="16.28515625" style="47" bestFit="1" customWidth="1"/>
-    <col min="139" max="139" width="20.85546875" style="47" bestFit="1" customWidth="1"/>
-    <col min="140" max="140" width="18.5703125" style="103" bestFit="1" customWidth="1"/>
-    <col min="141" max="141" width="18.85546875" style="103" bestFit="1" customWidth="1"/>
-    <col min="142" max="142" width="18.42578125" style="47" bestFit="1" customWidth="1"/>
-    <col min="143" max="143" width="18.28515625" style="47" bestFit="1" customWidth="1"/>
-    <col min="144" max="144" width="12.28515625" style="47" bestFit="1" customWidth="1"/>
-    <col min="145" max="145" width="13.7109375" style="47" bestFit="1" customWidth="1"/>
-    <col min="146" max="146" width="17.7109375" style="47" bestFit="1" customWidth="1"/>
-    <col min="147" max="147" width="18.85546875" style="47" bestFit="1" customWidth="1"/>
-    <col min="148" max="148" width="17.28515625" style="47" bestFit="1" customWidth="1"/>
-    <col min="149" max="149" width="19.28515625" style="87" bestFit="1" customWidth="1"/>
-    <col min="150" max="150" width="14.7109375" style="47" bestFit="1" customWidth="1"/>
-    <col min="151" max="151" width="15.42578125" style="47" bestFit="1" customWidth="1"/>
-    <col min="152" max="152" width="19.42578125" style="47" bestFit="1" customWidth="1"/>
-    <col min="153" max="153" width="18.42578125" style="47" bestFit="1" customWidth="1"/>
-    <col min="154" max="154" width="12.28515625" style="47" bestFit="1" customWidth="1"/>
-    <col min="155" max="155" width="13.7109375" style="47" bestFit="1" customWidth="1"/>
-    <col min="156" max="156" width="17.7109375" style="47" bestFit="1" customWidth="1"/>
-    <col min="157" max="157" width="16.28515625" style="47" bestFit="1" customWidth="1"/>
-    <col min="158" max="158" width="17.28515625" style="47" bestFit="1" customWidth="1"/>
-    <col min="159" max="159" width="19.28515625" style="87" bestFit="1" customWidth="1"/>
-    <col min="160" max="160" width="14.7109375" style="47" bestFit="1" customWidth="1"/>
-    <col min="161" max="161" width="15.42578125" style="47" bestFit="1" customWidth="1"/>
-    <col min="162" max="162" width="19.42578125" style="47" bestFit="1" customWidth="1"/>
-    <col min="163" max="163" width="18.42578125" style="47" bestFit="1" customWidth="1"/>
-    <col min="164" max="164" width="12.28515625" style="47" bestFit="1" customWidth="1"/>
-    <col min="165" max="165" width="13.7109375" style="47" bestFit="1" customWidth="1"/>
-    <col min="166" max="166" width="17.7109375" style="47" bestFit="1" customWidth="1"/>
-    <col min="167" max="167" width="16.28515625" style="47" bestFit="1" customWidth="1"/>
-    <col min="168" max="168" width="17.28515625" style="47" bestFit="1" customWidth="1"/>
-    <col min="169" max="169" width="19.28515625" style="87" bestFit="1" customWidth="1"/>
-    <col min="170" max="170" width="14.7109375" style="47" bestFit="1" customWidth="1"/>
-    <col min="171" max="171" width="15.42578125" style="47" bestFit="1" customWidth="1"/>
-    <col min="172" max="172" width="19.42578125" style="47" bestFit="1" customWidth="1"/>
-    <col min="173" max="173" width="18.42578125" style="47" bestFit="1" customWidth="1"/>
-    <col min="174" max="174" width="12.28515625" style="47" bestFit="1" customWidth="1"/>
-    <col min="175" max="175" width="13.7109375" style="47" bestFit="1" customWidth="1"/>
-    <col min="176" max="176" width="17.7109375" style="47" bestFit="1" customWidth="1"/>
-    <col min="177" max="177" width="16.28515625" style="47" bestFit="1" customWidth="1"/>
-    <col min="178" max="178" width="17.28515625" style="47" bestFit="1" customWidth="1"/>
-    <col min="179" max="179" width="19.28515625" style="87" bestFit="1" customWidth="1"/>
-    <col min="180" max="180" width="14.7109375" style="47" bestFit="1" customWidth="1"/>
-    <col min="181" max="181" width="15.42578125" style="47" bestFit="1" customWidth="1"/>
-    <col min="182" max="182" width="19.42578125" style="47" bestFit="1" customWidth="1"/>
-    <col min="183" max="183" width="18.42578125" style="47" bestFit="1" customWidth="1"/>
-    <col min="184" max="184" width="12.28515625" style="47" bestFit="1" customWidth="1"/>
-    <col min="185" max="185" width="13.7109375" style="47" bestFit="1" customWidth="1"/>
-    <col min="186" max="186" width="17.7109375" style="47" bestFit="1" customWidth="1"/>
-    <col min="187" max="187" width="16.28515625" style="47" bestFit="1" customWidth="1"/>
-    <col min="188" max="188" width="17.28515625" style="47" bestFit="1" customWidth="1"/>
-    <col min="189" max="189" width="19.28515625" style="87" bestFit="1" customWidth="1"/>
-    <col min="190" max="190" width="14.7109375" style="47" bestFit="1" customWidth="1"/>
-    <col min="191" max="191" width="15.42578125" style="47" bestFit="1" customWidth="1"/>
-    <col min="192" max="192" width="19.42578125" style="47" bestFit="1" customWidth="1"/>
-    <col min="193" max="193" width="18.42578125" style="47" bestFit="1" customWidth="1"/>
-    <col min="194" max="194" width="12.28515625" style="47" bestFit="1" customWidth="1"/>
-    <col min="195" max="195" width="13.7109375" style="47" bestFit="1" customWidth="1"/>
-    <col min="196" max="196" width="17.7109375" style="47" bestFit="1" customWidth="1"/>
-    <col min="197" max="197" width="16.28515625" style="47" bestFit="1" customWidth="1"/>
-    <col min="198" max="198" width="17.28515625" style="47" bestFit="1" customWidth="1"/>
-    <col min="199" max="199" width="19.28515625" style="87" bestFit="1" customWidth="1"/>
-    <col min="200" max="200" width="14.7109375" style="47" bestFit="1" customWidth="1"/>
-    <col min="201" max="201" width="15.42578125" style="47" bestFit="1" customWidth="1"/>
-    <col min="202" max="202" width="19.42578125" style="47" bestFit="1" customWidth="1"/>
-    <col min="203" max="203" width="18.42578125" style="47" bestFit="1" customWidth="1"/>
-    <col min="204" max="207" width="18.42578125" style="87" customWidth="1"/>
-    <col min="208" max="217" width="18.42578125" style="47" customWidth="1"/>
-    <col min="218" max="218" width="18.85546875" style="47" bestFit="1" customWidth="1"/>
-    <col min="219" max="219" width="15.7109375" style="47" bestFit="1" customWidth="1"/>
-    <col min="220" max="220" width="21.140625" style="47" customWidth="1"/>
-    <col min="221" max="221" width="23.140625" style="103" customWidth="1"/>
+    <col min="135" max="135" width="16.54296875" style="103" bestFit="1" customWidth="1"/>
+    <col min="136" max="136" width="16.81640625" style="103" bestFit="1" customWidth="1"/>
+    <col min="137" max="137" width="16.453125" style="47" bestFit="1" customWidth="1"/>
+    <col min="138" max="138" width="16.26953125" style="47" bestFit="1" customWidth="1"/>
+    <col min="139" max="139" width="20.81640625" style="47" bestFit="1" customWidth="1"/>
+    <col min="140" max="140" width="18.54296875" style="103" bestFit="1" customWidth="1"/>
+    <col min="141" max="141" width="18.81640625" style="103" bestFit="1" customWidth="1"/>
+    <col min="142" max="142" width="18.453125" style="47" bestFit="1" customWidth="1"/>
+    <col min="143" max="143" width="18.26953125" style="47" bestFit="1" customWidth="1"/>
+    <col min="144" max="144" width="12.26953125" style="47" bestFit="1" customWidth="1"/>
+    <col min="145" max="145" width="13.7265625" style="47" bestFit="1" customWidth="1"/>
+    <col min="146" max="146" width="17.7265625" style="47" bestFit="1" customWidth="1"/>
+    <col min="147" max="147" width="18.81640625" style="47" bestFit="1" customWidth="1"/>
+    <col min="148" max="148" width="17.26953125" style="47" bestFit="1" customWidth="1"/>
+    <col min="149" max="149" width="19.26953125" style="87" bestFit="1" customWidth="1"/>
+    <col min="150" max="150" width="14.7265625" style="47" bestFit="1" customWidth="1"/>
+    <col min="151" max="151" width="15.453125" style="47" bestFit="1" customWidth="1"/>
+    <col min="152" max="152" width="19.453125" style="47" bestFit="1" customWidth="1"/>
+    <col min="153" max="153" width="18.453125" style="47" bestFit="1" customWidth="1"/>
+    <col min="154" max="154" width="12.26953125" style="47" bestFit="1" customWidth="1"/>
+    <col min="155" max="155" width="13.7265625" style="47" bestFit="1" customWidth="1"/>
+    <col min="156" max="156" width="17.7265625" style="47" bestFit="1" customWidth="1"/>
+    <col min="157" max="157" width="16.26953125" style="47" bestFit="1" customWidth="1"/>
+    <col min="158" max="158" width="17.26953125" style="47" bestFit="1" customWidth="1"/>
+    <col min="159" max="159" width="19.26953125" style="87" bestFit="1" customWidth="1"/>
+    <col min="160" max="160" width="14.7265625" style="47" bestFit="1" customWidth="1"/>
+    <col min="161" max="161" width="15.453125" style="47" bestFit="1" customWidth="1"/>
+    <col min="162" max="162" width="19.453125" style="47" bestFit="1" customWidth="1"/>
+    <col min="163" max="163" width="18.453125" style="47" bestFit="1" customWidth="1"/>
+    <col min="164" max="164" width="12.26953125" style="47" bestFit="1" customWidth="1"/>
+    <col min="165" max="165" width="13.7265625" style="47" bestFit="1" customWidth="1"/>
+    <col min="166" max="166" width="17.7265625" style="47" bestFit="1" customWidth="1"/>
+    <col min="167" max="167" width="16.26953125" style="47" bestFit="1" customWidth="1"/>
+    <col min="168" max="168" width="17.26953125" style="47" bestFit="1" customWidth="1"/>
+    <col min="169" max="169" width="19.26953125" style="87" bestFit="1" customWidth="1"/>
+    <col min="170" max="170" width="14.7265625" style="47" bestFit="1" customWidth="1"/>
+    <col min="171" max="171" width="15.453125" style="47" bestFit="1" customWidth="1"/>
+    <col min="172" max="172" width="19.453125" style="47" bestFit="1" customWidth="1"/>
+    <col min="173" max="173" width="18.453125" style="47" bestFit="1" customWidth="1"/>
+    <col min="174" max="174" width="12.26953125" style="47" bestFit="1" customWidth="1"/>
+    <col min="175" max="175" width="13.7265625" style="47" bestFit="1" customWidth="1"/>
+    <col min="176" max="176" width="17.7265625" style="47" bestFit="1" customWidth="1"/>
+    <col min="177" max="177" width="16.26953125" style="47" bestFit="1" customWidth="1"/>
+    <col min="178" max="178" width="17.26953125" style="47" bestFit="1" customWidth="1"/>
+    <col min="179" max="179" width="19.26953125" style="87" bestFit="1" customWidth="1"/>
+    <col min="180" max="180" width="14.7265625" style="47" bestFit="1" customWidth="1"/>
+    <col min="181" max="181" width="15.453125" style="47" bestFit="1" customWidth="1"/>
+    <col min="182" max="182" width="19.453125" style="47" bestFit="1" customWidth="1"/>
+    <col min="183" max="183" width="18.453125" style="47" bestFit="1" customWidth="1"/>
+    <col min="184" max="184" width="12.26953125" style="47" bestFit="1" customWidth="1"/>
+    <col min="185" max="185" width="13.7265625" style="47" bestFit="1" customWidth="1"/>
+    <col min="186" max="186" width="17.7265625" style="47" bestFit="1" customWidth="1"/>
+    <col min="187" max="187" width="16.26953125" style="47" bestFit="1" customWidth="1"/>
+    <col min="188" max="188" width="17.26953125" style="47" bestFit="1" customWidth="1"/>
+    <col min="189" max="189" width="19.26953125" style="87" bestFit="1" customWidth="1"/>
+    <col min="190" max="190" width="14.7265625" style="47" bestFit="1" customWidth="1"/>
+    <col min="191" max="191" width="15.453125" style="47" bestFit="1" customWidth="1"/>
+    <col min="192" max="192" width="19.453125" style="47" bestFit="1" customWidth="1"/>
+    <col min="193" max="193" width="18.453125" style="47" bestFit="1" customWidth="1"/>
+    <col min="194" max="194" width="12.26953125" style="47" bestFit="1" customWidth="1"/>
+    <col min="195" max="195" width="13.7265625" style="47" bestFit="1" customWidth="1"/>
+    <col min="196" max="196" width="17.7265625" style="47" bestFit="1" customWidth="1"/>
+    <col min="197" max="197" width="16.26953125" style="47" bestFit="1" customWidth="1"/>
+    <col min="198" max="198" width="17.26953125" style="47" bestFit="1" customWidth="1"/>
+    <col min="199" max="199" width="19.26953125" style="87" bestFit="1" customWidth="1"/>
+    <col min="200" max="200" width="14.7265625" style="47" bestFit="1" customWidth="1"/>
+    <col min="201" max="201" width="15.453125" style="47" bestFit="1" customWidth="1"/>
+    <col min="202" max="202" width="19.453125" style="47" bestFit="1" customWidth="1"/>
+    <col min="203" max="203" width="18.453125" style="47" bestFit="1" customWidth="1"/>
+    <col min="204" max="207" width="18.453125" style="87" customWidth="1"/>
+    <col min="208" max="217" width="18.453125" style="47" customWidth="1"/>
+    <col min="218" max="218" width="18.81640625" style="47" bestFit="1" customWidth="1"/>
+    <col min="219" max="219" width="15.7265625" style="47" bestFit="1" customWidth="1"/>
+    <col min="220" max="220" width="21.1796875" style="47" customWidth="1"/>
+    <col min="221" max="221" width="23.1796875" style="103" customWidth="1"/>
     <col min="222" max="222" width="18" style="113" bestFit="1" customWidth="1"/>
-    <col min="223" max="16384" width="9.140625" style="47"/>
+    <col min="223" max="16384" width="9.1796875" style="47"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:222" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="264" t="s">
+    <row r="1" spans="1:222" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="313" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="265"/>
-      <c r="C1" s="265"/>
-      <c r="D1" s="265"/>
-      <c r="E1" s="265"/>
-      <c r="F1" s="265"/>
-      <c r="G1" s="265"/>
-      <c r="H1" s="265"/>
-      <c r="I1" s="265"/>
-      <c r="J1" s="265"/>
-      <c r="K1" s="265"/>
-      <c r="L1" s="266"/>
-      <c r="M1" s="254"/>
-      <c r="N1" s="249"/>
-      <c r="O1" s="249"/>
-      <c r="P1" s="249"/>
-      <c r="Q1" s="249"/>
-      <c r="R1" s="249"/>
-      <c r="S1" s="249"/>
-      <c r="T1" s="249"/>
-      <c r="U1" s="249"/>
-      <c r="V1" s="249"/>
-      <c r="W1" s="249"/>
-      <c r="X1" s="249"/>
-      <c r="Y1" s="249"/>
-      <c r="Z1" s="249"/>
-      <c r="AA1" s="249"/>
-      <c r="AB1" s="249"/>
-      <c r="AC1" s="249"/>
-      <c r="AD1" s="249"/>
-      <c r="AE1" s="249"/>
-      <c r="AF1" s="249"/>
-      <c r="AG1" s="249"/>
-      <c r="AH1" s="249"/>
-      <c r="AI1" s="249"/>
-      <c r="AJ1" s="249"/>
-      <c r="AK1" s="249"/>
-      <c r="AL1" s="249"/>
-      <c r="AM1" s="249"/>
-      <c r="AN1" s="249"/>
-      <c r="AO1" s="249"/>
-      <c r="AP1" s="249"/>
-      <c r="AQ1" s="249"/>
-      <c r="AR1" s="249"/>
-      <c r="AS1" s="249"/>
-      <c r="AT1" s="249"/>
-      <c r="AU1" s="249"/>
-      <c r="AV1" s="249"/>
-      <c r="AW1" s="249"/>
-      <c r="AX1" s="249"/>
-      <c r="AY1" s="249"/>
-      <c r="AZ1" s="249"/>
-      <c r="BA1" s="249"/>
-      <c r="BB1" s="250"/>
-      <c r="BC1" s="264" t="s">
+      <c r="B1" s="314"/>
+      <c r="C1" s="314"/>
+      <c r="D1" s="314"/>
+      <c r="E1" s="314"/>
+      <c r="F1" s="314"/>
+      <c r="G1" s="314"/>
+      <c r="H1" s="314"/>
+      <c r="I1" s="314"/>
+      <c r="J1" s="314"/>
+      <c r="K1" s="314"/>
+      <c r="L1" s="315"/>
+      <c r="M1" s="277"/>
+      <c r="N1" s="278"/>
+      <c r="O1" s="278"/>
+      <c r="P1" s="278"/>
+      <c r="Q1" s="278"/>
+      <c r="R1" s="278"/>
+      <c r="S1" s="278"/>
+      <c r="T1" s="278"/>
+      <c r="U1" s="278"/>
+      <c r="V1" s="278"/>
+      <c r="W1" s="278"/>
+      <c r="X1" s="278"/>
+      <c r="Y1" s="278"/>
+      <c r="Z1" s="278"/>
+      <c r="AA1" s="278"/>
+      <c r="AB1" s="278"/>
+      <c r="AC1" s="278"/>
+      <c r="AD1" s="278"/>
+      <c r="AE1" s="278"/>
+      <c r="AF1" s="278"/>
+      <c r="AG1" s="278"/>
+      <c r="AH1" s="278"/>
+      <c r="AI1" s="278"/>
+      <c r="AJ1" s="278"/>
+      <c r="AK1" s="278"/>
+      <c r="AL1" s="278"/>
+      <c r="AM1" s="278"/>
+      <c r="AN1" s="278"/>
+      <c r="AO1" s="278"/>
+      <c r="AP1" s="278"/>
+      <c r="AQ1" s="278"/>
+      <c r="AR1" s="278"/>
+      <c r="AS1" s="278"/>
+      <c r="AT1" s="278"/>
+      <c r="AU1" s="278"/>
+      <c r="AV1" s="278"/>
+      <c r="AW1" s="278"/>
+      <c r="AX1" s="278"/>
+      <c r="AY1" s="278"/>
+      <c r="AZ1" s="278"/>
+      <c r="BA1" s="278"/>
+      <c r="BB1" s="306"/>
+      <c r="BC1" s="313" t="s">
         <v>16</v>
       </c>
-      <c r="BD1" s="265"/>
-      <c r="BE1" s="265"/>
-      <c r="BF1" s="265"/>
-      <c r="BG1" s="265"/>
-      <c r="BH1" s="265"/>
-      <c r="BI1" s="266"/>
-      <c r="BJ1" s="267" t="s">
+      <c r="BD1" s="314"/>
+      <c r="BE1" s="314"/>
+      <c r="BF1" s="314"/>
+      <c r="BG1" s="314"/>
+      <c r="BH1" s="314"/>
+      <c r="BI1" s="315"/>
+      <c r="BJ1" s="316" t="s">
         <v>17</v>
       </c>
-      <c r="BK1" s="268"/>
-      <c r="BL1" s="268"/>
-      <c r="BM1" s="268"/>
-      <c r="BN1" s="269"/>
-      <c r="BO1" s="270" t="s">
+      <c r="BK1" s="317"/>
+      <c r="BL1" s="317"/>
+      <c r="BM1" s="317"/>
+      <c r="BN1" s="318"/>
+      <c r="BO1" s="319" t="s">
         <v>18</v>
       </c>
-      <c r="BP1" s="271"/>
-      <c r="BQ1" s="271"/>
-      <c r="BR1" s="271"/>
-      <c r="BS1" s="271"/>
-      <c r="BT1" s="271"/>
-      <c r="BU1" s="271"/>
-      <c r="BV1" s="271"/>
-      <c r="BW1" s="271"/>
-      <c r="BX1" s="271"/>
-      <c r="BY1" s="271"/>
-      <c r="BZ1" s="271"/>
-      <c r="CA1" s="271"/>
-      <c r="CB1" s="271"/>
-      <c r="CC1" s="271"/>
-      <c r="CD1" s="271"/>
-      <c r="CE1" s="271"/>
-      <c r="CF1" s="271"/>
-      <c r="CG1" s="271"/>
-      <c r="CH1" s="271"/>
-      <c r="CI1" s="271"/>
-      <c r="CJ1" s="271"/>
-      <c r="CK1" s="271"/>
-      <c r="CL1" s="271"/>
-      <c r="CM1" s="271"/>
-      <c r="CN1" s="271"/>
-      <c r="CO1" s="271"/>
-      <c r="CP1" s="271"/>
-      <c r="CQ1" s="271"/>
-      <c r="CR1" s="271"/>
-      <c r="CS1" s="271"/>
-      <c r="CT1" s="271"/>
-      <c r="CU1" s="271"/>
-      <c r="CV1" s="271"/>
-      <c r="CW1" s="271"/>
-      <c r="CX1" s="271"/>
-      <c r="CY1" s="271"/>
-      <c r="CZ1" s="271"/>
-      <c r="DA1" s="271"/>
-      <c r="DB1" s="271"/>
-      <c r="DC1" s="272"/>
-      <c r="DD1" s="296" t="s">
+      <c r="BP1" s="320"/>
+      <c r="BQ1" s="320"/>
+      <c r="BR1" s="320"/>
+      <c r="BS1" s="320"/>
+      <c r="BT1" s="320"/>
+      <c r="BU1" s="320"/>
+      <c r="BV1" s="320"/>
+      <c r="BW1" s="320"/>
+      <c r="BX1" s="320"/>
+      <c r="BY1" s="320"/>
+      <c r="BZ1" s="320"/>
+      <c r="CA1" s="320"/>
+      <c r="CB1" s="320"/>
+      <c r="CC1" s="320"/>
+      <c r="CD1" s="320"/>
+      <c r="CE1" s="320"/>
+      <c r="CF1" s="320"/>
+      <c r="CG1" s="320"/>
+      <c r="CH1" s="320"/>
+      <c r="CI1" s="320"/>
+      <c r="CJ1" s="320"/>
+      <c r="CK1" s="320"/>
+      <c r="CL1" s="320"/>
+      <c r="CM1" s="320"/>
+      <c r="CN1" s="320"/>
+      <c r="CO1" s="320"/>
+      <c r="CP1" s="320"/>
+      <c r="CQ1" s="320"/>
+      <c r="CR1" s="320"/>
+      <c r="CS1" s="320"/>
+      <c r="CT1" s="320"/>
+      <c r="CU1" s="320"/>
+      <c r="CV1" s="320"/>
+      <c r="CW1" s="320"/>
+      <c r="CX1" s="320"/>
+      <c r="CY1" s="320"/>
+      <c r="CZ1" s="320"/>
+      <c r="DA1" s="320"/>
+      <c r="DB1" s="320"/>
+      <c r="DC1" s="321"/>
+      <c r="DD1" s="291" t="s">
         <v>19</v>
       </c>
-      <c r="DE1" s="297"/>
-      <c r="DF1" s="297"/>
-      <c r="DG1" s="297"/>
-      <c r="DH1" s="297"/>
-      <c r="DI1" s="297"/>
-      <c r="DJ1" s="297"/>
-      <c r="DK1" s="297"/>
-      <c r="DL1" s="297"/>
-      <c r="DM1" s="297"/>
-      <c r="DN1" s="297"/>
-      <c r="DO1" s="297"/>
-      <c r="DP1" s="297"/>
-      <c r="DQ1" s="297"/>
-      <c r="DR1" s="297"/>
-      <c r="DS1" s="297"/>
-      <c r="DT1" s="297"/>
-      <c r="DU1" s="297"/>
-      <c r="DV1" s="297"/>
-      <c r="DW1" s="297"/>
-      <c r="DX1" s="297"/>
-      <c r="DY1" s="297"/>
-      <c r="DZ1" s="297"/>
-      <c r="EA1" s="297"/>
-      <c r="EB1" s="297"/>
-      <c r="EC1" s="297"/>
-      <c r="ED1" s="297"/>
-      <c r="EE1" s="297"/>
-      <c r="EF1" s="297"/>
-      <c r="EG1" s="297"/>
-      <c r="EH1" s="297"/>
-      <c r="EI1" s="297"/>
-      <c r="EJ1" s="297"/>
-      <c r="EK1" s="297"/>
-      <c r="EL1" s="297"/>
-      <c r="EM1" s="298"/>
-      <c r="EN1" s="254"/>
-      <c r="EO1" s="249"/>
-      <c r="EP1" s="249"/>
-      <c r="EQ1" s="249"/>
-      <c r="ER1" s="249"/>
-      <c r="ES1" s="249"/>
-      <c r="ET1" s="249"/>
-      <c r="EU1" s="249"/>
-      <c r="EV1" s="249"/>
-      <c r="EW1" s="249"/>
-      <c r="EX1" s="249"/>
-      <c r="EY1" s="249"/>
-      <c r="EZ1" s="249"/>
-      <c r="FA1" s="249"/>
-      <c r="FB1" s="249"/>
-      <c r="FC1" s="249"/>
-      <c r="FD1" s="249"/>
-      <c r="FE1" s="249"/>
-      <c r="FF1" s="249"/>
-      <c r="FG1" s="249"/>
-      <c r="FH1" s="249"/>
-      <c r="FI1" s="249"/>
-      <c r="FJ1" s="249"/>
-      <c r="FK1" s="249"/>
-      <c r="FL1" s="249"/>
-      <c r="FM1" s="249"/>
-      <c r="FN1" s="249"/>
-      <c r="FO1" s="249"/>
-      <c r="FP1" s="249"/>
-      <c r="FQ1" s="249"/>
-      <c r="FR1" s="249"/>
-      <c r="FS1" s="249"/>
-      <c r="FT1" s="249"/>
-      <c r="FU1" s="249"/>
-      <c r="FV1" s="249"/>
-      <c r="FW1" s="249"/>
-      <c r="FX1" s="249"/>
-      <c r="FY1" s="249"/>
-      <c r="FZ1" s="249"/>
-      <c r="GA1" s="249"/>
-      <c r="GB1" s="249"/>
-      <c r="GC1" s="249"/>
-      <c r="GD1" s="249"/>
-      <c r="GE1" s="249"/>
-      <c r="GF1" s="249"/>
-      <c r="GG1" s="249"/>
-      <c r="GH1" s="249"/>
-      <c r="GI1" s="249"/>
-      <c r="GJ1" s="249"/>
-      <c r="GK1" s="249"/>
-      <c r="GL1" s="249"/>
-      <c r="GM1" s="249"/>
-      <c r="GN1" s="249"/>
-      <c r="GO1" s="249"/>
-      <c r="GP1" s="249"/>
-      <c r="GQ1" s="249"/>
-      <c r="GR1" s="249"/>
-      <c r="GS1" s="249"/>
-      <c r="GT1" s="249"/>
-      <c r="GU1" s="249"/>
-      <c r="GV1" s="311" t="s">
-        <v>230</v>
-      </c>
-      <c r="GW1" s="312"/>
-      <c r="GX1" s="312"/>
-      <c r="GY1" s="313"/>
+      <c r="DE1" s="292"/>
+      <c r="DF1" s="292"/>
+      <c r="DG1" s="292"/>
+      <c r="DH1" s="292"/>
+      <c r="DI1" s="292"/>
+      <c r="DJ1" s="292"/>
+      <c r="DK1" s="292"/>
+      <c r="DL1" s="292"/>
+      <c r="DM1" s="292"/>
+      <c r="DN1" s="292"/>
+      <c r="DO1" s="292"/>
+      <c r="DP1" s="292"/>
+      <c r="DQ1" s="292"/>
+      <c r="DR1" s="292"/>
+      <c r="DS1" s="292"/>
+      <c r="DT1" s="292"/>
+      <c r="DU1" s="292"/>
+      <c r="DV1" s="292"/>
+      <c r="DW1" s="292"/>
+      <c r="DX1" s="292"/>
+      <c r="DY1" s="292"/>
+      <c r="DZ1" s="292"/>
+      <c r="EA1" s="292"/>
+      <c r="EB1" s="292"/>
+      <c r="EC1" s="292"/>
+      <c r="ED1" s="292"/>
+      <c r="EE1" s="292"/>
+      <c r="EF1" s="292"/>
+      <c r="EG1" s="292"/>
+      <c r="EH1" s="292"/>
+      <c r="EI1" s="292"/>
+      <c r="EJ1" s="292"/>
+      <c r="EK1" s="292"/>
+      <c r="EL1" s="292"/>
+      <c r="EM1" s="293"/>
+      <c r="EN1" s="277"/>
+      <c r="EO1" s="278"/>
+      <c r="EP1" s="278"/>
+      <c r="EQ1" s="278"/>
+      <c r="ER1" s="278"/>
+      <c r="ES1" s="278"/>
+      <c r="ET1" s="278"/>
+      <c r="EU1" s="278"/>
+      <c r="EV1" s="278"/>
+      <c r="EW1" s="278"/>
+      <c r="EX1" s="278"/>
+      <c r="EY1" s="278"/>
+      <c r="EZ1" s="278"/>
+      <c r="FA1" s="278"/>
+      <c r="FB1" s="278"/>
+      <c r="FC1" s="278"/>
+      <c r="FD1" s="278"/>
+      <c r="FE1" s="278"/>
+      <c r="FF1" s="278"/>
+      <c r="FG1" s="278"/>
+      <c r="FH1" s="278"/>
+      <c r="FI1" s="278"/>
+      <c r="FJ1" s="278"/>
+      <c r="FK1" s="278"/>
+      <c r="FL1" s="278"/>
+      <c r="FM1" s="278"/>
+      <c r="FN1" s="278"/>
+      <c r="FO1" s="278"/>
+      <c r="FP1" s="278"/>
+      <c r="FQ1" s="278"/>
+      <c r="FR1" s="278"/>
+      <c r="FS1" s="278"/>
+      <c r="FT1" s="278"/>
+      <c r="FU1" s="278"/>
+      <c r="FV1" s="278"/>
+      <c r="FW1" s="278"/>
+      <c r="FX1" s="278"/>
+      <c r="FY1" s="278"/>
+      <c r="FZ1" s="278"/>
+      <c r="GA1" s="278"/>
+      <c r="GB1" s="278"/>
+      <c r="GC1" s="278"/>
+      <c r="GD1" s="278"/>
+      <c r="GE1" s="278"/>
+      <c r="GF1" s="278"/>
+      <c r="GG1" s="278"/>
+      <c r="GH1" s="278"/>
+      <c r="GI1" s="278"/>
+      <c r="GJ1" s="278"/>
+      <c r="GK1" s="278"/>
+      <c r="GL1" s="278"/>
+      <c r="GM1" s="278"/>
+      <c r="GN1" s="278"/>
+      <c r="GO1" s="278"/>
+      <c r="GP1" s="278"/>
+      <c r="GQ1" s="278"/>
+      <c r="GR1" s="278"/>
+      <c r="GS1" s="278"/>
+      <c r="GT1" s="278"/>
+      <c r="GU1" s="278"/>
+      <c r="GV1" s="258" t="s">
+        <v>227</v>
+      </c>
+      <c r="GW1" s="259"/>
+      <c r="GX1" s="259"/>
+      <c r="GY1" s="260"/>
       <c r="HA1" s="194"/>
       <c r="HB1" s="194"/>
       <c r="HC1" s="194"/>
-      <c r="HD1" s="302" t="s">
+      <c r="HD1" s="249" t="s">
         <v>217</v>
       </c>
-      <c r="HE1" s="303"/>
-      <c r="HF1" s="303"/>
-      <c r="HG1" s="303"/>
-      <c r="HH1" s="303"/>
-      <c r="HI1" s="304"/>
+      <c r="HE1" s="250"/>
+      <c r="HF1" s="250"/>
+      <c r="HG1" s="250"/>
+      <c r="HH1" s="250"/>
+      <c r="HI1" s="251"/>
       <c r="HJ1" s="92"/>
       <c r="HK1" s="91"/>
       <c r="HL1" s="97"/>
       <c r="HM1" s="108"/>
       <c r="HN1" s="110"/>
     </row>
-    <row r="2" spans="1:222" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="249"/>
-      <c r="B2" s="249"/>
-      <c r="C2" s="249"/>
-      <c r="D2" s="249"/>
-      <c r="E2" s="249"/>
-      <c r="F2" s="249"/>
-      <c r="G2" s="249"/>
-      <c r="H2" s="249"/>
-      <c r="I2" s="250"/>
-      <c r="J2" s="282" t="s">
+    <row r="2" spans="1:222" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="278"/>
+      <c r="B2" s="278"/>
+      <c r="C2" s="278"/>
+      <c r="D2" s="278"/>
+      <c r="E2" s="278"/>
+      <c r="F2" s="278"/>
+      <c r="G2" s="278"/>
+      <c r="H2" s="278"/>
+      <c r="I2" s="306"/>
+      <c r="J2" s="325" t="s">
         <v>20</v>
       </c>
-      <c r="K2" s="283"/>
+      <c r="K2" s="326"/>
       <c r="L2" s="48"/>
-      <c r="M2" s="251"/>
-      <c r="N2" s="252"/>
-      <c r="O2" s="252"/>
-      <c r="P2" s="252"/>
-      <c r="Q2" s="252"/>
-      <c r="R2" s="252"/>
-      <c r="S2" s="252"/>
-      <c r="T2" s="253"/>
-      <c r="U2" s="284" t="s">
+      <c r="M2" s="307"/>
+      <c r="N2" s="308"/>
+      <c r="O2" s="308"/>
+      <c r="P2" s="308"/>
+      <c r="Q2" s="308"/>
+      <c r="R2" s="308"/>
+      <c r="S2" s="308"/>
+      <c r="T2" s="309"/>
+      <c r="U2" s="327" t="s">
         <v>21</v>
       </c>
-      <c r="V2" s="285"/>
-      <c r="W2" s="285"/>
-      <c r="X2" s="285"/>
-      <c r="Y2" s="285"/>
-      <c r="Z2" s="285"/>
-      <c r="AA2" s="285"/>
-      <c r="AB2" s="285"/>
-      <c r="AC2" s="285"/>
-      <c r="AD2" s="285"/>
-      <c r="AE2" s="285"/>
-      <c r="AF2" s="285"/>
-      <c r="AG2" s="285"/>
-      <c r="AH2" s="285"/>
-      <c r="AI2" s="285"/>
-      <c r="AJ2" s="285"/>
-      <c r="AK2" s="286"/>
-      <c r="AL2" s="287" t="s">
+      <c r="V2" s="328"/>
+      <c r="W2" s="328"/>
+      <c r="X2" s="328"/>
+      <c r="Y2" s="328"/>
+      <c r="Z2" s="328"/>
+      <c r="AA2" s="328"/>
+      <c r="AB2" s="328"/>
+      <c r="AC2" s="328"/>
+      <c r="AD2" s="328"/>
+      <c r="AE2" s="328"/>
+      <c r="AF2" s="328"/>
+      <c r="AG2" s="328"/>
+      <c r="AH2" s="328"/>
+      <c r="AI2" s="328"/>
+      <c r="AJ2" s="328"/>
+      <c r="AK2" s="329"/>
+      <c r="AL2" s="279" t="s">
         <v>22</v>
       </c>
-      <c r="AM2" s="288"/>
-      <c r="AN2" s="288"/>
-      <c r="AO2" s="288"/>
-      <c r="AP2" s="288"/>
-      <c r="AQ2" s="288"/>
-      <c r="AR2" s="288"/>
-      <c r="AS2" s="288"/>
-      <c r="AT2" s="288"/>
-      <c r="AU2" s="289"/>
-      <c r="AV2" s="290" t="s">
+      <c r="AM2" s="280"/>
+      <c r="AN2" s="280"/>
+      <c r="AO2" s="280"/>
+      <c r="AP2" s="280"/>
+      <c r="AQ2" s="280"/>
+      <c r="AR2" s="280"/>
+      <c r="AS2" s="280"/>
+      <c r="AT2" s="280"/>
+      <c r="AU2" s="281"/>
+      <c r="AV2" s="282" t="s">
         <v>23</v>
       </c>
-      <c r="AW2" s="291"/>
-      <c r="AX2" s="291"/>
-      <c r="AY2" s="291"/>
-      <c r="AZ2" s="291"/>
-      <c r="BA2" s="291"/>
-      <c r="BB2" s="292"/>
-      <c r="BC2" s="279"/>
-      <c r="BD2" s="280"/>
-      <c r="BE2" s="280"/>
-      <c r="BF2" s="280"/>
-      <c r="BG2" s="280"/>
-      <c r="BH2" s="280"/>
-      <c r="BI2" s="281"/>
-      <c r="BJ2" s="279"/>
-      <c r="BK2" s="280"/>
-      <c r="BL2" s="280"/>
-      <c r="BM2" s="280"/>
-      <c r="BN2" s="281"/>
-      <c r="BO2" s="293" t="s">
+      <c r="AW2" s="283"/>
+      <c r="AX2" s="283"/>
+      <c r="AY2" s="283"/>
+      <c r="AZ2" s="283"/>
+      <c r="BA2" s="283"/>
+      <c r="BB2" s="284"/>
+      <c r="BC2" s="288"/>
+      <c r="BD2" s="289"/>
+      <c r="BE2" s="289"/>
+      <c r="BF2" s="289"/>
+      <c r="BG2" s="289"/>
+      <c r="BH2" s="289"/>
+      <c r="BI2" s="290"/>
+      <c r="BJ2" s="288"/>
+      <c r="BK2" s="289"/>
+      <c r="BL2" s="289"/>
+      <c r="BM2" s="289"/>
+      <c r="BN2" s="290"/>
+      <c r="BO2" s="285" t="s">
         <v>24</v>
       </c>
-      <c r="BP2" s="294"/>
-      <c r="BQ2" s="294"/>
-      <c r="BR2" s="294"/>
-      <c r="BS2" s="294"/>
-      <c r="BT2" s="294"/>
-      <c r="BU2" s="294"/>
-      <c r="BV2" s="294"/>
-      <c r="BW2" s="294"/>
-      <c r="BX2" s="294"/>
-      <c r="BY2" s="295"/>
-      <c r="BZ2" s="273" t="s">
+      <c r="BP2" s="286"/>
+      <c r="BQ2" s="286"/>
+      <c r="BR2" s="286"/>
+      <c r="BS2" s="286"/>
+      <c r="BT2" s="286"/>
+      <c r="BU2" s="286"/>
+      <c r="BV2" s="286"/>
+      <c r="BW2" s="286"/>
+      <c r="BX2" s="286"/>
+      <c r="BY2" s="287"/>
+      <c r="BZ2" s="294" t="s">
         <v>25</v>
       </c>
-      <c r="CA2" s="274"/>
-      <c r="CB2" s="274"/>
-      <c r="CC2" s="274"/>
-      <c r="CD2" s="275"/>
-      <c r="CE2" s="255" t="s">
+      <c r="CA2" s="295"/>
+      <c r="CB2" s="295"/>
+      <c r="CC2" s="295"/>
+      <c r="CD2" s="296"/>
+      <c r="CE2" s="310" t="s">
         <v>26</v>
       </c>
-      <c r="CF2" s="256"/>
-      <c r="CG2" s="256"/>
-      <c r="CH2" s="256"/>
-      <c r="CI2" s="257"/>
-      <c r="CJ2" s="258" t="s">
+      <c r="CF2" s="311"/>
+      <c r="CG2" s="311"/>
+      <c r="CH2" s="311"/>
+      <c r="CI2" s="312"/>
+      <c r="CJ2" s="300" t="s">
         <v>27</v>
       </c>
-      <c r="CK2" s="259"/>
-      <c r="CL2" s="259"/>
-      <c r="CM2" s="259"/>
-      <c r="CN2" s="260"/>
-      <c r="CO2" s="299" t="s">
+      <c r="CK2" s="301"/>
+      <c r="CL2" s="301"/>
+      <c r="CM2" s="301"/>
+      <c r="CN2" s="302"/>
+      <c r="CO2" s="297" t="s">
         <v>28</v>
       </c>
-      <c r="CP2" s="300"/>
-      <c r="CQ2" s="300"/>
-      <c r="CR2" s="300"/>
-      <c r="CS2" s="301"/>
-      <c r="CT2" s="261" t="s">
-        <v>227</v>
-      </c>
-      <c r="CU2" s="262"/>
-      <c r="CV2" s="262"/>
-      <c r="CW2" s="262"/>
-      <c r="CX2" s="263"/>
-      <c r="CY2" s="276" t="s">
+      <c r="CP2" s="298"/>
+      <c r="CQ2" s="298"/>
+      <c r="CR2" s="298"/>
+      <c r="CS2" s="299"/>
+      <c r="CT2" s="303" t="s">
+        <v>224</v>
+      </c>
+      <c r="CU2" s="304"/>
+      <c r="CV2" s="304"/>
+      <c r="CW2" s="304"/>
+      <c r="CX2" s="305"/>
+      <c r="CY2" s="322" t="s">
         <v>216</v>
       </c>
-      <c r="CZ2" s="277"/>
-      <c r="DA2" s="277"/>
-      <c r="DB2" s="277"/>
-      <c r="DC2" s="278"/>
-      <c r="DD2" s="293" t="s">
+      <c r="CZ2" s="323"/>
+      <c r="DA2" s="323"/>
+      <c r="DB2" s="323"/>
+      <c r="DC2" s="324"/>
+      <c r="DD2" s="285" t="s">
         <v>24</v>
       </c>
-      <c r="DE2" s="294"/>
-      <c r="DF2" s="294"/>
-      <c r="DG2" s="294"/>
-      <c r="DH2" s="294"/>
-      <c r="DI2" s="294"/>
-      <c r="DJ2" s="294"/>
-      <c r="DK2" s="294"/>
-      <c r="DL2" s="294"/>
-      <c r="DM2" s="294"/>
-      <c r="DN2" s="295"/>
-      <c r="DO2" s="273" t="s">
+      <c r="DE2" s="286"/>
+      <c r="DF2" s="286"/>
+      <c r="DG2" s="286"/>
+      <c r="DH2" s="286"/>
+      <c r="DI2" s="286"/>
+      <c r="DJ2" s="286"/>
+      <c r="DK2" s="286"/>
+      <c r="DL2" s="286"/>
+      <c r="DM2" s="286"/>
+      <c r="DN2" s="287"/>
+      <c r="DO2" s="294" t="s">
         <v>29</v>
       </c>
-      <c r="DP2" s="274"/>
-      <c r="DQ2" s="274"/>
-      <c r="DR2" s="274"/>
-      <c r="DS2" s="275"/>
-      <c r="DT2" s="255" t="s">
+      <c r="DP2" s="295"/>
+      <c r="DQ2" s="295"/>
+      <c r="DR2" s="295"/>
+      <c r="DS2" s="296"/>
+      <c r="DT2" s="310" t="s">
         <v>30</v>
       </c>
-      <c r="DU2" s="256"/>
-      <c r="DV2" s="256"/>
-      <c r="DW2" s="256"/>
-      <c r="DX2" s="257"/>
-      <c r="DY2" s="258" t="s">
+      <c r="DU2" s="311"/>
+      <c r="DV2" s="311"/>
+      <c r="DW2" s="311"/>
+      <c r="DX2" s="312"/>
+      <c r="DY2" s="300" t="s">
         <v>31</v>
       </c>
-      <c r="DZ2" s="259"/>
-      <c r="EA2" s="259"/>
-      <c r="EB2" s="259"/>
-      <c r="EC2" s="260"/>
-      <c r="ED2" s="299" t="s">
+      <c r="DZ2" s="301"/>
+      <c r="EA2" s="301"/>
+      <c r="EB2" s="301"/>
+      <c r="EC2" s="302"/>
+      <c r="ED2" s="297" t="s">
         <v>32</v>
       </c>
-      <c r="EE2" s="300"/>
-      <c r="EF2" s="300"/>
-      <c r="EG2" s="300"/>
-      <c r="EH2" s="301"/>
-      <c r="EI2" s="261" t="s">
+      <c r="EE2" s="298"/>
+      <c r="EF2" s="298"/>
+      <c r="EG2" s="298"/>
+      <c r="EH2" s="299"/>
+      <c r="EI2" s="303" t="s">
         <v>33</v>
       </c>
-      <c r="EJ2" s="262"/>
-      <c r="EK2" s="262"/>
-      <c r="EL2" s="262"/>
-      <c r="EM2" s="263"/>
-      <c r="EN2" s="314" t="s">
+      <c r="EJ2" s="304"/>
+      <c r="EK2" s="304"/>
+      <c r="EL2" s="304"/>
+      <c r="EM2" s="305"/>
+      <c r="EN2" s="261" t="s">
         <v>34</v>
       </c>
-      <c r="EO2" s="315"/>
-      <c r="EP2" s="315"/>
-      <c r="EQ2" s="315"/>
-      <c r="ER2" s="315"/>
-      <c r="ES2" s="315"/>
-      <c r="ET2" s="315"/>
-      <c r="EU2" s="315"/>
-      <c r="EV2" s="315"/>
-      <c r="EW2" s="316"/>
-      <c r="EX2" s="317" t="s">
+      <c r="EO2" s="262"/>
+      <c r="EP2" s="262"/>
+      <c r="EQ2" s="262"/>
+      <c r="ER2" s="262"/>
+      <c r="ES2" s="262"/>
+      <c r="ET2" s="262"/>
+      <c r="EU2" s="262"/>
+      <c r="EV2" s="262"/>
+      <c r="EW2" s="263"/>
+      <c r="EX2" s="264" t="s">
         <v>35</v>
       </c>
-      <c r="EY2" s="318"/>
-      <c r="EZ2" s="318"/>
-      <c r="FA2" s="318"/>
-      <c r="FB2" s="318"/>
-      <c r="FC2" s="318"/>
-      <c r="FD2" s="318"/>
-      <c r="FE2" s="318"/>
-      <c r="FF2" s="318"/>
-      <c r="FG2" s="319"/>
-      <c r="FH2" s="320" t="s">
+      <c r="EY2" s="265"/>
+      <c r="EZ2" s="265"/>
+      <c r="FA2" s="265"/>
+      <c r="FB2" s="265"/>
+      <c r="FC2" s="265"/>
+      <c r="FD2" s="265"/>
+      <c r="FE2" s="265"/>
+      <c r="FF2" s="265"/>
+      <c r="FG2" s="266"/>
+      <c r="FH2" s="267" t="s">
         <v>36</v>
       </c>
-      <c r="FI2" s="321"/>
-      <c r="FJ2" s="321"/>
-      <c r="FK2" s="321"/>
-      <c r="FL2" s="321"/>
-      <c r="FM2" s="321"/>
-      <c r="FN2" s="321"/>
-      <c r="FO2" s="321"/>
-      <c r="FP2" s="321"/>
-      <c r="FQ2" s="322"/>
-      <c r="FR2" s="323" t="s">
+      <c r="FI2" s="268"/>
+      <c r="FJ2" s="268"/>
+      <c r="FK2" s="268"/>
+      <c r="FL2" s="268"/>
+      <c r="FM2" s="268"/>
+      <c r="FN2" s="268"/>
+      <c r="FO2" s="268"/>
+      <c r="FP2" s="268"/>
+      <c r="FQ2" s="269"/>
+      <c r="FR2" s="270" t="s">
         <v>37</v>
       </c>
-      <c r="FS2" s="324"/>
-      <c r="FT2" s="324"/>
-      <c r="FU2" s="324"/>
-      <c r="FV2" s="324"/>
-      <c r="FW2" s="324"/>
-      <c r="FX2" s="324"/>
-      <c r="FY2" s="324"/>
-      <c r="FZ2" s="324"/>
-      <c r="GA2" s="324"/>
-      <c r="GB2" s="325" t="s">
-        <v>225</v>
-      </c>
-      <c r="GC2" s="326"/>
-      <c r="GD2" s="326"/>
-      <c r="GE2" s="326"/>
-      <c r="GF2" s="326"/>
-      <c r="GG2" s="326"/>
-      <c r="GH2" s="326"/>
-      <c r="GI2" s="326"/>
-      <c r="GJ2" s="326"/>
-      <c r="GK2" s="327"/>
-      <c r="GL2" s="328" t="s">
-        <v>226</v>
-      </c>
-      <c r="GM2" s="329"/>
-      <c r="GN2" s="329"/>
-      <c r="GO2" s="329"/>
-      <c r="GP2" s="329"/>
-      <c r="GQ2" s="329"/>
-      <c r="GR2" s="329"/>
-      <c r="GS2" s="329"/>
-      <c r="GT2" s="329"/>
-      <c r="GU2" s="329"/>
-      <c r="GV2" s="308" t="s">
-        <v>231</v>
-      </c>
-      <c r="GW2" s="309"/>
-      <c r="GX2" s="309"/>
-      <c r="GY2" s="310"/>
-      <c r="GZ2" s="305" t="s">
-        <v>242</v>
-      </c>
-      <c r="HA2" s="306"/>
-      <c r="HB2" s="306"/>
-      <c r="HC2" s="307"/>
+      <c r="FS2" s="271"/>
+      <c r="FT2" s="271"/>
+      <c r="FU2" s="271"/>
+      <c r="FV2" s="271"/>
+      <c r="FW2" s="271"/>
+      <c r="FX2" s="271"/>
+      <c r="FY2" s="271"/>
+      <c r="FZ2" s="271"/>
+      <c r="GA2" s="271"/>
+      <c r="GB2" s="272" t="s">
+        <v>222</v>
+      </c>
+      <c r="GC2" s="273"/>
+      <c r="GD2" s="273"/>
+      <c r="GE2" s="273"/>
+      <c r="GF2" s="273"/>
+      <c r="GG2" s="273"/>
+      <c r="GH2" s="273"/>
+      <c r="GI2" s="273"/>
+      <c r="GJ2" s="273"/>
+      <c r="GK2" s="274"/>
+      <c r="GL2" s="275" t="s">
+        <v>223</v>
+      </c>
+      <c r="GM2" s="276"/>
+      <c r="GN2" s="276"/>
+      <c r="GO2" s="276"/>
+      <c r="GP2" s="276"/>
+      <c r="GQ2" s="276"/>
+      <c r="GR2" s="276"/>
+      <c r="GS2" s="276"/>
+      <c r="GT2" s="276"/>
+      <c r="GU2" s="276"/>
+      <c r="GV2" s="255" t="s">
+        <v>228</v>
+      </c>
+      <c r="GW2" s="256"/>
+      <c r="GX2" s="256"/>
+      <c r="GY2" s="257"/>
+      <c r="GZ2" s="252" t="s">
+        <v>239</v>
+      </c>
+      <c r="HA2" s="253"/>
+      <c r="HB2" s="253"/>
+      <c r="HC2" s="254"/>
       <c r="HD2" s="90"/>
       <c r="HE2" s="90"/>
       <c r="HF2" s="90"/>
@@ -5931,7 +5931,7 @@
       <c r="HM2" s="109"/>
       <c r="HN2" s="111"/>
     </row>
-    <row r="3" spans="1:222" ht="24" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:222" ht="23" x14ac:dyDescent="0.25">
       <c r="A3" s="115" t="s">
         <v>2</v>
       </c>
@@ -6386,7 +6386,7 @@
         <v>165</v>
       </c>
       <c r="EV3" s="151" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="EW3" s="77" t="s">
         <v>166</v>
@@ -6416,7 +6416,7 @@
         <v>174</v>
       </c>
       <c r="FF3" s="128" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="FG3" s="131" t="s">
         <v>175</v>
@@ -6446,7 +6446,7 @@
         <v>183</v>
       </c>
       <c r="FP3" s="128" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="FQ3" s="131" t="s">
         <v>184</v>
@@ -6476,130 +6476,130 @@
         <v>192</v>
       </c>
       <c r="FZ3" s="128" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="GA3" s="77" t="s">
         <v>193</v>
       </c>
       <c r="GB3" s="176" t="s">
+        <v>240</v>
+      </c>
+      <c r="GC3" s="128" t="s">
+        <v>241</v>
+      </c>
+      <c r="GD3" s="128" t="s">
+        <v>242</v>
+      </c>
+      <c r="GE3" s="128" t="s">
         <v>243</v>
       </c>
-      <c r="GC3" s="128" t="s">
+      <c r="GF3" s="128" t="s">
         <v>244</v>
       </c>
-      <c r="GD3" s="128" t="s">
+      <c r="GG3" s="129" t="s">
         <v>245</v>
       </c>
-      <c r="GE3" s="128" t="s">
+      <c r="GH3" s="128" t="s">
         <v>246</v>
       </c>
-      <c r="GF3" s="128" t="s">
+      <c r="GI3" s="128" t="s">
         <v>247</v>
       </c>
-      <c r="GG3" s="129" t="s">
+      <c r="GJ3" s="128" t="s">
         <v>248</v>
       </c>
-      <c r="GH3" s="128" t="s">
+      <c r="GK3" s="77" t="s">
         <v>249</v>
       </c>
-      <c r="GI3" s="128" t="s">
+      <c r="GL3" s="176" t="s">
         <v>250</v>
       </c>
-      <c r="GJ3" s="128" t="s">
+      <c r="GM3" s="128" t="s">
         <v>251</v>
       </c>
-      <c r="GK3" s="77" t="s">
+      <c r="GN3" s="128" t="s">
         <v>252</v>
       </c>
-      <c r="GL3" s="176" t="s">
+      <c r="GO3" s="128" t="s">
         <v>253</v>
       </c>
-      <c r="GM3" s="128" t="s">
+      <c r="GP3" s="128" t="s">
         <v>254</v>
       </c>
-      <c r="GN3" s="128" t="s">
+      <c r="GQ3" s="129" t="s">
         <v>255</v>
       </c>
-      <c r="GO3" s="128" t="s">
+      <c r="GR3" s="128" t="s">
         <v>256</v>
       </c>
-      <c r="GP3" s="128" t="s">
+      <c r="GS3" s="128" t="s">
         <v>257</v>
       </c>
-      <c r="GQ3" s="129" t="s">
+      <c r="GT3" s="128" t="s">
         <v>258</v>
       </c>
-      <c r="GR3" s="128" t="s">
+      <c r="GU3" s="77" t="s">
         <v>259</v>
       </c>
-      <c r="GS3" s="128" t="s">
-        <v>260</v>
-      </c>
-      <c r="GT3" s="128" t="s">
-        <v>261</v>
-      </c>
-      <c r="GU3" s="77" t="s">
-        <v>262</v>
-      </c>
       <c r="GV3" s="93" t="s">
+        <v>229</v>
+      </c>
+      <c r="GW3" s="93" t="s">
+        <v>230</v>
+      </c>
+      <c r="GX3" s="93" t="s">
+        <v>231</v>
+      </c>
+      <c r="GY3" s="93" t="s">
         <v>232</v>
       </c>
-      <c r="GW3" s="93" t="s">
-        <v>233</v>
-      </c>
-      <c r="GX3" s="93" t="s">
-        <v>234</v>
-      </c>
-      <c r="GY3" s="93" t="s">
+      <c r="GZ3" s="77" t="s">
         <v>235</v>
       </c>
-      <c r="GZ3" s="77" t="s">
+      <c r="HA3" s="77" t="s">
+        <v>236</v>
+      </c>
+      <c r="HB3" s="77" t="s">
+        <v>237</v>
+      </c>
+      <c r="HC3" s="77" t="s">
         <v>238</v>
-      </c>
-      <c r="HA3" s="77" t="s">
-        <v>239</v>
-      </c>
-      <c r="HB3" s="77" t="s">
-        <v>240</v>
-      </c>
-      <c r="HC3" s="77" t="s">
-        <v>241</v>
       </c>
       <c r="HD3" s="77" t="s">
         <v>218</v>
       </c>
       <c r="HE3" s="77" t="s">
+        <v>261</v>
+      </c>
+      <c r="HF3" s="77" t="s">
+        <v>262</v>
+      </c>
+      <c r="HG3" s="77" t="s">
+        <v>263</v>
+      </c>
+      <c r="HH3" s="77" t="s">
         <v>219</v>
       </c>
-      <c r="HF3" s="77" t="s">
+      <c r="HI3" s="77" t="s">
         <v>220</v>
-      </c>
-      <c r="HG3" s="77" t="s">
-        <v>221</v>
-      </c>
-      <c r="HH3" s="77" t="s">
-        <v>222</v>
-      </c>
-      <c r="HI3" s="77" t="s">
-        <v>223</v>
       </c>
       <c r="HJ3" s="63" t="s">
         <v>210</v>
       </c>
       <c r="HK3" s="177" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="HL3" s="178" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="HM3" s="179" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="HN3" s="180" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="4" spans="1:222" s="60" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="4" spans="1:222" s="60" customFormat="1" ht="11.5" x14ac:dyDescent="0.25">
       <c r="A4" s="181"/>
       <c r="B4" s="182"/>
       <c r="C4" s="181"/>
@@ -6823,7 +6823,7 @@
       <c r="HM4" s="189"/>
       <c r="HN4" s="193"/>
     </row>
-    <row r="5" spans="1:222" ht="12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:222" ht="11.5" x14ac:dyDescent="0.25">
       <c r="A5" s="64"/>
       <c r="B5" s="65"/>
       <c r="C5" s="64"/>
@@ -7043,7 +7043,7 @@
       <c r="HI5" s="56"/>
       <c r="HM5" s="105"/>
     </row>
-    <row r="6" spans="1:222" ht="12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:222" ht="11.5" x14ac:dyDescent="0.25">
       <c r="A6" s="74"/>
       <c r="B6" s="71"/>
       <c r="C6" s="71"/>
@@ -7263,7 +7263,7 @@
       <c r="HI6" s="74"/>
       <c r="HM6" s="106"/>
     </row>
-    <row r="7" spans="1:222" ht="12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:222" ht="11.5" x14ac:dyDescent="0.25">
       <c r="A7" s="74"/>
       <c r="B7" s="71"/>
       <c r="C7" s="71"/>
@@ -7483,7 +7483,7 @@
       <c r="HI7" s="56"/>
       <c r="HM7" s="105"/>
     </row>
-    <row r="8" spans="1:222" ht="12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:222" ht="11.5" x14ac:dyDescent="0.25">
       <c r="A8" s="74"/>
       <c r="B8" s="71"/>
       <c r="C8" s="71"/>
@@ -7703,7 +7703,7 @@
       <c r="HI8" s="74"/>
       <c r="HM8" s="106"/>
     </row>
-    <row r="9" spans="1:222" ht="12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:222" ht="11.5" x14ac:dyDescent="0.25">
       <c r="A9" s="74"/>
       <c r="B9" s="71"/>
       <c r="C9" s="71"/>
@@ -7923,7 +7923,7 @@
       <c r="HI9" s="56"/>
       <c r="HM9" s="105"/>
     </row>
-    <row r="10" spans="1:222" ht="12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:222" ht="11.5" x14ac:dyDescent="0.25">
       <c r="A10" s="74"/>
       <c r="B10" s="71"/>
       <c r="C10" s="71"/>
@@ -8143,7 +8143,7 @@
       <c r="HI10" s="74"/>
       <c r="HM10" s="106"/>
     </row>
-    <row r="11" spans="1:222" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:222" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="74"/>
       <c r="B11" s="71"/>
       <c r="C11" s="71"/>
@@ -8363,7 +8363,7 @@
       <c r="HI11" s="56"/>
       <c r="HM11" s="105"/>
     </row>
-    <row r="12" spans="1:222" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:222" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="74"/>
       <c r="B12" s="71"/>
       <c r="C12" s="71"/>
@@ -8583,7 +8583,7 @@
       <c r="HI12" s="74"/>
       <c r="HM12" s="106"/>
     </row>
-    <row r="13" spans="1:222" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:222" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="74"/>
       <c r="B13" s="71"/>
       <c r="C13" s="71"/>
@@ -8803,7 +8803,7 @@
       <c r="HI13" s="56"/>
       <c r="HM13" s="105"/>
     </row>
-    <row r="14" spans="1:222" s="71" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:222" s="71" customFormat="1" ht="11.5" x14ac:dyDescent="0.25">
       <c r="A14" s="74"/>
       <c r="B14" s="74"/>
       <c r="C14" s="74"/>
@@ -8937,7 +8937,7 @@
       <c r="HM14" s="106"/>
       <c r="HN14" s="112"/>
     </row>
-    <row r="15" spans="1:222" s="71" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:222" s="71" customFormat="1" ht="11.5" x14ac:dyDescent="0.25">
       <c r="A15" s="74"/>
       <c r="B15" s="74"/>
       <c r="C15" s="74"/>
@@ -9071,7 +9071,7 @@
       <c r="HM15" s="106"/>
       <c r="HN15" s="112"/>
     </row>
-    <row r="16" spans="1:222" s="71" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:222" s="71" customFormat="1" ht="11.5" x14ac:dyDescent="0.25">
       <c r="A16" s="74"/>
       <c r="B16" s="74"/>
       <c r="C16" s="74"/>
@@ -9205,7 +9205,7 @@
       <c r="HM16" s="106"/>
       <c r="HN16" s="112"/>
     </row>
-    <row r="17" spans="1:222" s="71" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:222" s="71" customFormat="1" ht="11.5" x14ac:dyDescent="0.25">
       <c r="A17" s="74"/>
       <c r="B17" s="74"/>
       <c r="C17" s="74"/>
@@ -9335,7 +9335,7 @@
       <c r="HM17" s="106"/>
       <c r="HN17" s="112"/>
     </row>
-    <row r="18" spans="1:222" s="71" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:222" s="71" customFormat="1" ht="11.5" x14ac:dyDescent="0.25">
       <c r="A18" s="74"/>
       <c r="B18" s="74"/>
       <c r="C18" s="74"/>
@@ -9465,7 +9465,7 @@
       <c r="HM18" s="106"/>
       <c r="HN18" s="112"/>
     </row>
-    <row r="19" spans="1:222" s="71" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:222" s="71" customFormat="1" ht="11.5" x14ac:dyDescent="0.25">
       <c r="A19" s="74"/>
       <c r="B19" s="74"/>
       <c r="C19" s="74"/>
@@ -9595,7 +9595,7 @@
       <c r="HM19" s="106"/>
       <c r="HN19" s="112"/>
     </row>
-    <row r="20" spans="1:222" s="71" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:222" s="71" customFormat="1" ht="11.5" x14ac:dyDescent="0.25">
       <c r="A20" s="74"/>
       <c r="B20" s="74"/>
       <c r="C20" s="74"/>
@@ -9725,7 +9725,7 @@
       <c r="HM20" s="106"/>
       <c r="HN20" s="112"/>
     </row>
-    <row r="21" spans="1:222" s="71" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:222" s="71" customFormat="1" ht="11.5" x14ac:dyDescent="0.25">
       <c r="A21" s="74"/>
       <c r="B21" s="74"/>
       <c r="C21" s="74"/>
@@ -9855,7 +9855,7 @@
       <c r="HM21" s="106"/>
       <c r="HN21" s="112"/>
     </row>
-    <row r="22" spans="1:222" s="71" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:222" s="71" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="49"/>
       <c r="B22" s="50"/>
       <c r="C22" s="49"/>
@@ -10063,7 +10063,7 @@
       <c r="HM22" s="105"/>
       <c r="HN22" s="112"/>
     </row>
-    <row r="23" spans="1:222" s="73" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:222" s="73" customFormat="1" ht="11.5" x14ac:dyDescent="0.25">
       <c r="A23" s="72"/>
       <c r="D23" s="72"/>
       <c r="E23" s="72"/>
@@ -10178,7 +10178,7 @@
       <c r="HM23" s="107"/>
       <c r="HN23" s="113"/>
     </row>
-    <row r="24" spans="1:222" s="73" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:222" s="73" customFormat="1" ht="11.5" x14ac:dyDescent="0.25">
       <c r="A24" s="72"/>
       <c r="D24" s="72"/>
       <c r="E24" s="72"/>
@@ -10293,7 +10293,7 @@
       <c r="HM24" s="107"/>
       <c r="HN24" s="113"/>
     </row>
-    <row r="25" spans="1:222" s="73" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:222" s="73" customFormat="1" ht="11.5" x14ac:dyDescent="0.25">
       <c r="A25" s="72"/>
       <c r="D25" s="72"/>
       <c r="E25" s="72"/>
@@ -10408,7 +10408,7 @@
       <c r="HM25" s="107"/>
       <c r="HN25" s="113"/>
     </row>
-    <row r="26" spans="1:222" s="73" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:222" s="73" customFormat="1" ht="11.5" x14ac:dyDescent="0.25">
       <c r="A26" s="72"/>
       <c r="D26" s="72"/>
       <c r="E26" s="72"/>
@@ -10523,7 +10523,7 @@
       <c r="HM26" s="107"/>
       <c r="HN26" s="113"/>
     </row>
-    <row r="27" spans="1:222" s="73" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:222" s="73" customFormat="1" ht="11.5" x14ac:dyDescent="0.25">
       <c r="A27" s="72"/>
       <c r="D27" s="72"/>
       <c r="E27" s="72"/>
@@ -10638,7 +10638,7 @@
       <c r="HM27" s="107"/>
       <c r="HN27" s="113"/>
     </row>
-    <row r="28" spans="1:222" s="73" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:222" s="73" customFormat="1" ht="11.5" x14ac:dyDescent="0.25">
       <c r="A28" s="72"/>
       <c r="D28" s="72"/>
       <c r="E28" s="72"/>
@@ -10753,7 +10753,7 @@
       <c r="HM28" s="107"/>
       <c r="HN28" s="113"/>
     </row>
-    <row r="29" spans="1:222" s="73" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:222" s="73" customFormat="1" ht="11.5" x14ac:dyDescent="0.25">
       <c r="A29" s="72"/>
       <c r="D29" s="72"/>
       <c r="E29" s="72"/>
@@ -10868,7 +10868,7 @@
       <c r="HM29" s="107"/>
       <c r="HN29" s="113"/>
     </row>
-    <row r="30" spans="1:222" s="73" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:222" s="73" customFormat="1" ht="11.5" x14ac:dyDescent="0.25">
       <c r="A30" s="72"/>
       <c r="D30" s="72"/>
       <c r="E30" s="72"/>
@@ -10982,7 +10982,7 @@
       <c r="HM30" s="107"/>
       <c r="HN30" s="113"/>
     </row>
-    <row r="31" spans="1:222" s="73" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:222" s="73" customFormat="1" ht="11.5" x14ac:dyDescent="0.25">
       <c r="A31" s="72"/>
       <c r="D31" s="72"/>
       <c r="E31" s="72"/>
@@ -11097,7 +11097,7 @@
       <c r="HM31" s="107"/>
       <c r="HN31" s="113"/>
     </row>
-    <row r="32" spans="1:222" s="73" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:222" s="73" customFormat="1" ht="11.5" x14ac:dyDescent="0.25">
       <c r="A32" s="72"/>
       <c r="D32" s="72"/>
       <c r="E32" s="72"/>
@@ -11212,35 +11212,35 @@
       <c r="HM32" s="107"/>
       <c r="HN32" s="113"/>
     </row>
-    <row r="33" spans="109:110" ht="12" x14ac:dyDescent="0.2">
+    <row r="33" spans="109:110" ht="11.5" x14ac:dyDescent="0.25">
       <c r="DE33" s="61"/>
       <c r="DF33" s="61"/>
     </row>
-    <row r="34" spans="109:110" ht="12" x14ac:dyDescent="0.2">
+    <row r="34" spans="109:110" ht="11.5" x14ac:dyDescent="0.25">
       <c r="DE34" s="61"/>
       <c r="DF34" s="61"/>
     </row>
-    <row r="35" spans="109:110" ht="12" x14ac:dyDescent="0.2">
+    <row r="35" spans="109:110" ht="11.5" x14ac:dyDescent="0.25">
       <c r="DE35" s="61"/>
       <c r="DF35" s="61"/>
     </row>
-    <row r="36" spans="109:110" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="109:110" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="DE36" s="61"/>
       <c r="DF36" s="61"/>
     </row>
-    <row r="37" spans="109:110" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="109:110" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="DE37" s="61"/>
       <c r="DF37" s="61"/>
     </row>
-    <row r="38" spans="109:110" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="109:110" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="DE38" s="61"/>
       <c r="DF38" s="61"/>
     </row>
-    <row r="39" spans="109:110" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="109:110" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="DE39" s="61"/>
       <c r="DF39" s="61"/>
     </row>
-    <row r="489" spans="16:222" s="62" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="489" spans="16:222" s="62" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="P489" s="102"/>
       <c r="Q489" s="88"/>
       <c r="R489" s="88"/>
@@ -11290,7 +11290,7 @@
       <c r="HM489" s="104"/>
       <c r="HN489" s="114"/>
     </row>
-    <row r="490" spans="16:222" s="62" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="490" spans="16:222" s="62" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="P490" s="102"/>
       <c r="Q490" s="88"/>
       <c r="R490" s="88"/>
@@ -11340,7 +11340,7 @@
       <c r="HM490" s="104"/>
       <c r="HN490" s="114"/>
     </row>
-    <row r="491" spans="16:222" s="62" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="491" spans="16:222" s="62" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="P491" s="102"/>
       <c r="Q491" s="88"/>
       <c r="R491" s="88"/>
@@ -11390,7 +11390,7 @@
       <c r="HM491" s="104"/>
       <c r="HN491" s="114"/>
     </row>
-    <row r="492" spans="16:222" s="62" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="492" spans="16:222" s="62" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="P492" s="102"/>
       <c r="Q492" s="88"/>
       <c r="R492" s="88"/>
@@ -11437,7 +11437,7 @@
       <c r="HM492" s="104"/>
       <c r="HN492" s="114"/>
     </row>
-    <row r="493" spans="16:222" s="62" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="493" spans="16:222" s="62" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="P493" s="102"/>
       <c r="Q493" s="88"/>
       <c r="R493" s="88"/>
@@ -11484,7 +11484,7 @@
       <c r="HM493" s="104"/>
       <c r="HN493" s="114"/>
     </row>
-    <row r="494" spans="16:222" s="62" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="494" spans="16:222" s="62" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="P494" s="102"/>
       <c r="Q494" s="88"/>
       <c r="R494" s="88"/>
@@ -11540,28 +11540,6 @@
   </protectedRanges>
   <autoFilter ref="A3:HK32" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
   <mergeCells count="38">
-    <mergeCell ref="HD1:HI1"/>
-    <mergeCell ref="GZ2:HC2"/>
-    <mergeCell ref="GV2:GY2"/>
-    <mergeCell ref="GV1:GY1"/>
-    <mergeCell ref="EN2:EW2"/>
-    <mergeCell ref="EX2:FG2"/>
-    <mergeCell ref="FH2:FQ2"/>
-    <mergeCell ref="FR2:GA2"/>
-    <mergeCell ref="GB2:GK2"/>
-    <mergeCell ref="GL2:GU2"/>
-    <mergeCell ref="EN1:GU1"/>
-    <mergeCell ref="AL2:AU2"/>
-    <mergeCell ref="AV2:BB2"/>
-    <mergeCell ref="BO2:BY2"/>
-    <mergeCell ref="BJ2:BN2"/>
-    <mergeCell ref="DD1:EM1"/>
-    <mergeCell ref="DO2:DS2"/>
-    <mergeCell ref="DD2:DN2"/>
-    <mergeCell ref="CO2:CS2"/>
-    <mergeCell ref="DY2:EC2"/>
-    <mergeCell ref="ED2:EH2"/>
-    <mergeCell ref="EI2:EM2"/>
     <mergeCell ref="A2:I2"/>
     <mergeCell ref="M2:T2"/>
     <mergeCell ref="M1:BB1"/>
@@ -11578,6 +11556,28 @@
     <mergeCell ref="BC2:BI2"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="U2:AK2"/>
+    <mergeCell ref="AL2:AU2"/>
+    <mergeCell ref="AV2:BB2"/>
+    <mergeCell ref="BO2:BY2"/>
+    <mergeCell ref="BJ2:BN2"/>
+    <mergeCell ref="DD1:EM1"/>
+    <mergeCell ref="DO2:DS2"/>
+    <mergeCell ref="DD2:DN2"/>
+    <mergeCell ref="CO2:CS2"/>
+    <mergeCell ref="DY2:EC2"/>
+    <mergeCell ref="ED2:EH2"/>
+    <mergeCell ref="EI2:EM2"/>
+    <mergeCell ref="HD1:HI1"/>
+    <mergeCell ref="GZ2:HC2"/>
+    <mergeCell ref="GV2:GY2"/>
+    <mergeCell ref="GV1:GY1"/>
+    <mergeCell ref="EN2:EW2"/>
+    <mergeCell ref="EX2:FG2"/>
+    <mergeCell ref="FH2:FQ2"/>
+    <mergeCell ref="FR2:GA2"/>
+    <mergeCell ref="GB2:GK2"/>
+    <mergeCell ref="GL2:GU2"/>
+    <mergeCell ref="EN1:GU1"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>